<commit_message>
removed 'No Result' value
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -4718,11 +4718,6 @@
           <t>Contact Name</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="9" ht="29" customHeight="1">
       <c r="A9" s="15" t="inlineStr">
@@ -4755,11 +4750,6 @@
           <t>Contact Role</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="10" ht="43.5" customHeight="1">
       <c r="A10" s="15" t="inlineStr">
@@ -4792,11 +4782,6 @@
           <t>Mimimum Response Duration</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="11" ht="43.5" customHeight="1">
       <c r="A11" s="15" t="inlineStr">
@@ -4827,11 +4812,6 @@
       <c r="F11" s="14" t="inlineStr">
         <is>
           <t>Background treatment</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>No result</t>
         </is>
       </c>
     </row>
@@ -4858,11 +4838,6 @@
           <t>Data Monitoring Committee Indicator</t>
         </is>
       </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="13" ht="43.5" customHeight="1">
       <c r="A13" s="15" t="inlineStr">
@@ -4895,11 +4870,6 @@
           <t>Dosage Levels</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="14" ht="43.5" customHeight="1">
       <c r="A14" s="15" t="inlineStr">
@@ -4932,11 +4902,6 @@
           <t>Dose Form</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="15" ht="43.5" customHeight="1">
       <c r="A15" s="15" t="inlineStr">
@@ -4969,11 +4934,6 @@
           <t>Administration Frequency</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="16" ht="43.5" customHeight="1">
       <c r="A16" s="15" t="inlineStr">
@@ -5004,11 +4964,6 @@
       <c r="F16" s="14" t="inlineStr">
         <is>
           <t>Dosage Units</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>No result</t>
         </is>
       </c>
     </row>
@@ -5035,11 +4990,6 @@
           <t>Extension Trial Indicator</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="18" ht="29" customHeight="1">
       <c r="A18" s="15" t="inlineStr">
@@ -5066,11 +5016,6 @@
       <c r="F18" s="14" t="inlineStr">
         <is>
           <t>Planned Country of Investigational Sites</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>No result</t>
         </is>
       </c>
     </row>
@@ -5097,11 +5042,6 @@
           <t>Healthy Subject Indicator Study Population</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="20" ht="29" customHeight="1">
       <c r="A20" s="15" t="inlineStr">
@@ -5126,11 +5066,6 @@
           <t>Healthy Subject Indicator Study Cohort</t>
         </is>
       </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="21" ht="58" customHeight="1">
       <c r="A21" s="15" t="inlineStr">
@@ -5260,11 +5195,6 @@
           <t>Trial Duration Value + Units</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="25" ht="29" customHeight="1">
       <c r="A25" s="15" t="inlineStr">
@@ -5289,11 +5219,6 @@
           <t>Multiple Site Eu Site Trial Indicator</t>
         </is>
       </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="26" ht="29" customHeight="1">
       <c r="A26" s="15" t="inlineStr">
@@ -5347,11 +5272,6 @@
           <t>Number of Groups/Cohorts</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="28" ht="29" customHeight="1">
       <c r="A28" s="15" t="inlineStr">
@@ -5376,11 +5296,6 @@
           <t>Number of Trial Sites EU State</t>
         </is>
       </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="29" ht="43.5" customHeight="1">
       <c r="A29" s="15" t="inlineStr">
@@ -5521,11 +5436,6 @@
           <t>Observational Model</t>
         </is>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="33" ht="29" customHeight="1">
       <c r="A33" s="15" t="inlineStr">
@@ -5550,11 +5460,6 @@
           <t>Observational Time Perspective</t>
         </is>
       </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="34" ht="29" customHeight="1">
       <c r="A34" s="15" t="inlineStr">
@@ -5579,11 +5484,6 @@
           <t>Observational Study Population Description</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="35" ht="29" customHeight="1">
       <c r="A35" s="15" t="inlineStr">
@@ -5608,11 +5508,6 @@
           <t>Observational Study Sampling Method</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="36" ht="29" customHeight="1">
       <c r="A36" s="15" t="inlineStr">
@@ -5645,11 +5540,6 @@
           <t>Exploratory Outcome Measure</t>
         </is>
       </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="37" ht="29" customHeight="1">
       <c r="A37" s="15" t="inlineStr">
@@ -5682,11 +5572,6 @@
           <t>Primary Outcome Measure</t>
         </is>
       </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="38" ht="29" customHeight="1">
       <c r="A38" s="15" t="inlineStr">
@@ -5719,11 +5604,6 @@
           <t>Secondary Outcome Measure</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="39" ht="43.5" customHeight="1">
       <c r="A39" s="15" t="inlineStr">
@@ -5750,11 +5630,6 @@
       <c r="F39" s="14" t="inlineStr">
         <is>
           <t>Pharmacologic Class</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>No result</t>
         </is>
       </c>
     </row>
@@ -5781,11 +5656,6 @@
           <t>Pediatric Investigation Plan Indicator</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="41" ht="72.5" customHeight="1">
       <c r="A41" s="15" t="inlineStr">
@@ -5843,11 +5713,6 @@
           <t>Planned Duration of Intervention Value + Unit</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="43">
       <c r="A43" s="15" t="inlineStr">
@@ -5872,11 +5737,6 @@
           <t>Randomized Indicator</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="44">
       <c r="A44" s="15" t="inlineStr">
@@ -5901,11 +5761,6 @@
           <t>Rare disease indicator</t>
         </is>
       </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="45" ht="43.5" customHeight="1">
       <c r="A45" s="15" t="inlineStr">
@@ -5938,11 +5793,6 @@
           <t>Registry Identifier</t>
         </is>
       </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="46" ht="43.5" customHeight="1">
       <c r="A46" s="15" t="inlineStr">
@@ -5975,11 +5825,6 @@
           <t>Route of Administration</t>
         </is>
       </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="47" ht="58" customHeight="1">
       <c r="A47" s="15" t="inlineStr">
@@ -6010,11 +5855,6 @@
       <c r="F47" s="14" t="inlineStr">
         <is>
           <t>Retained Biospecimen Description</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t>No result</t>
         </is>
       </c>
     </row>
@@ -6041,11 +5881,6 @@
           <t>Sex of Participants</t>
         </is>
       </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="49" ht="29" customHeight="1">
       <c r="A49" s="15" t="inlineStr">
@@ -6075,11 +5910,6 @@
           <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
         </is>
       </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="50" ht="29" customHeight="1">
       <c r="A50" s="15" t="inlineStr">
@@ -6106,11 +5936,6 @@
       <c r="F50" s="14" t="inlineStr">
         <is>
           <t>Sponsor's Study Reference ID</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>No result</t>
         </is>
       </c>
     </row>
@@ -6137,11 +5962,6 @@
           <t>Single Site Eu State Trial Indicator</t>
         </is>
       </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="52" ht="29" customHeight="1">
       <c r="A52" s="15" t="inlineStr">
@@ -6166,11 +5986,6 @@
           <t>Study Type</t>
         </is>
       </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="53" ht="87" customHeight="1">
       <c r="A53" s="15" t="inlineStr">
@@ -6229,11 +6044,6 @@
           <t>Intervention Control Type</t>
         </is>
       </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="55">
       <c r="A55" s="15" t="inlineStr">
@@ -6258,11 +6068,6 @@
           <t>Therapeutic Area</t>
         </is>
       </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="56" ht="29" customHeight="1">
       <c r="A56" s="15" t="inlineStr">
@@ -6289,11 +6094,6 @@
       <c r="F56" s="14" t="inlineStr">
         <is>
           <t>Trial Intent Types</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>No result</t>
         </is>
       </c>
     </row>
@@ -6391,11 +6191,6 @@
           <t>Investigational Intervention</t>
         </is>
       </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>No result</t>
-        </is>
-      </c>
     </row>
     <row r="60">
       <c r="A60" s="15" t="inlineStr">
@@ -6418,11 +6213,6 @@
       <c r="F60" s="14" t="inlineStr">
         <is>
           <t>Trial Type</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>No result</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Replaced JSONATA column with Results column in output file
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -4417,7 +4417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H60"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E28" zoomScale="182" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
@@ -4468,7 +4468,7 @@
       </c>
       <c r="G1" s="30" t="inlineStr">
         <is>
-          <t>JSONATA</t>
+          <t>Mapping Result</t>
         </is>
       </c>
     </row>
@@ -4497,11 +4497,6 @@
       </c>
       <c r="G2" s="34" t="inlineStr">
         <is>
-          <t>$exists(study.versions.studyDesigns.characteristics[code="C98704"]) ? "Y" : ""</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
           <t>Y</t>
         </is>
       </c>
@@ -4531,12 +4526,6 @@
       </c>
       <c r="G3" s="34" t="inlineStr">
         <is>
-          <t>$min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
-study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
           <t xml:space="preserve">18 ["Year","Year"] </t>
         </is>
       </c>
@@ -4566,12 +4555,6 @@
       </c>
       <c r="G4" s="31" t="inlineStr">
         <is>
-          <t>$max([study.versions.studyDesigns.population.plannedAge.maxValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.value]) &amp; " " &amp; 
-study.versions.studyDesigns.population.plannedAge.maxValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.unit.standardCode.decode</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
           <t xml:space="preserve">100 ["Year","Year"] </t>
         </is>
       </c>
@@ -4609,7 +4592,7 @@
       </c>
       <c r="G5" s="31" t="inlineStr">
         <is>
-          <t>study.versions.studyDesigns.biospecimenRetentions.includesDNA</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4646,7 +4629,7 @@
       </c>
       <c r="G6" s="31" t="inlineStr">
         <is>
-          <t>study.versions.studyDesigns.biospecimenRetentions.isRetained</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4683,7 +4666,7 @@
       </c>
       <c r="G7" s="31" t="inlineStr">
         <is>
-          <t>x</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4718,6 +4701,11 @@
           <t>Contact Name</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="29" customHeight="1">
       <c r="A9" s="15" t="inlineStr">
@@ -4750,6 +4738,11 @@
           <t>Contact Role</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="43.5" customHeight="1">
       <c r="A10" s="15" t="inlineStr">
@@ -4782,6 +4775,11 @@
           <t>Mimimum Response Duration</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="43.5" customHeight="1">
       <c r="A11" s="15" t="inlineStr">
@@ -4812,6 +4810,11 @@
       <c r="F11" s="14" t="inlineStr">
         <is>
           <t>Background treatment</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4838,6 +4841,11 @@
           <t>Data Monitoring Committee Indicator</t>
         </is>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="13" ht="43.5" customHeight="1">
       <c r="A13" s="15" t="inlineStr">
@@ -4870,6 +4878,11 @@
           <t>Dosage Levels</t>
         </is>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="14" ht="43.5" customHeight="1">
       <c r="A14" s="15" t="inlineStr">
@@ -4902,6 +4915,11 @@
           <t>Dose Form</t>
         </is>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="43.5" customHeight="1">
       <c r="A15" s="15" t="inlineStr">
@@ -4934,6 +4952,11 @@
           <t>Administration Frequency</t>
         </is>
       </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="16" ht="43.5" customHeight="1">
       <c r="A16" s="15" t="inlineStr">
@@ -4964,6 +4987,11 @@
       <c r="F16" s="14" t="inlineStr">
         <is>
           <t>Dosage Units</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4990,6 +5018,11 @@
           <t>Extension Trial Indicator</t>
         </is>
       </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="29" customHeight="1">
       <c r="A18" s="15" t="inlineStr">
@@ -5016,6 +5049,11 @@
       <c r="F18" s="14" t="inlineStr">
         <is>
           <t>Planned Country of Investigational Sites</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5042,6 +5080,11 @@
           <t>Healthy Subject Indicator Study Population</t>
         </is>
       </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="20" ht="29" customHeight="1">
       <c r="A20" s="15" t="inlineStr">
@@ -5066,6 +5109,11 @@
           <t>Healthy Subject Indicator Study Cohort</t>
         </is>
       </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="21" ht="58" customHeight="1">
       <c r="A21" s="15" t="inlineStr">
@@ -5121,11 +5169,6 @@
       </c>
       <c r="G22" s="32" t="inlineStr">
         <is>
-          <t>study.versions.studyDesigns[studyType.code="C98388"].model.decode</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
           <t>PARALLEL</t>
         </is>
       </c>
@@ -5162,11 +5205,6 @@
         </is>
       </c>
       <c r="G23" s="31" t="inlineStr">
-        <is>
-          <t>study.versions.studyInterventions.type.decode</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
         <is>
           <t>Pharmacologic Substance</t>
         </is>
@@ -5195,6 +5233,11 @@
           <t>Trial Duration Value + Units</t>
         </is>
       </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="25" ht="29" customHeight="1">
       <c r="A25" s="15" t="inlineStr">
@@ -5219,6 +5262,11 @@
           <t>Multiple Site Eu Site Trial Indicator</t>
         </is>
       </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="26" ht="29" customHeight="1">
       <c r="A26" s="15" t="inlineStr">
@@ -5272,6 +5320,11 @@
           <t>Number of Groups/Cohorts</t>
         </is>
       </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="28" ht="29" customHeight="1">
       <c r="A28" s="15" t="inlineStr">
@@ -5296,6 +5349,11 @@
           <t>Number of Trial Sites EU State</t>
         </is>
       </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="43.5" customHeight="1">
       <c r="A29" s="15" t="inlineStr">
@@ -5330,7 +5388,7 @@
       </c>
       <c r="G29" s="33" t="inlineStr">
         <is>
-          <t>study.versions.studyDesigns.objectives[level.code="C163559"].text</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5366,11 +5424,6 @@
         </is>
       </c>
       <c r="G30" s="33" t="inlineStr">
-        <is>
-          <t>study.versions.studyDesigns.objectives[level.code="C85826"].text</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
         <is>
           <t>•	To evaluate the effect of intravenous infusions of Beroclin administered once daily on motor symptoms in subjects with early stage Parkinson s disease.</t>
         </is>
@@ -5436,6 +5489,11 @@
           <t>Observational Model</t>
         </is>
       </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="33" ht="29" customHeight="1">
       <c r="A33" s="15" t="inlineStr">
@@ -5460,6 +5518,11 @@
           <t>Observational Time Perspective</t>
         </is>
       </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="34" ht="29" customHeight="1">
       <c r="A34" s="15" t="inlineStr">
@@ -5484,6 +5547,11 @@
           <t>Observational Study Population Description</t>
         </is>
       </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="35" ht="29" customHeight="1">
       <c r="A35" s="15" t="inlineStr">
@@ -5508,6 +5576,11 @@
           <t>Observational Study Sampling Method</t>
         </is>
       </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="29" customHeight="1">
       <c r="A36" s="15" t="inlineStr">
@@ -5540,6 +5613,11 @@
           <t>Exploratory Outcome Measure</t>
         </is>
       </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="37" ht="29" customHeight="1">
       <c r="A37" s="15" t="inlineStr">
@@ -5572,6 +5650,11 @@
           <t>Primary Outcome Measure</t>
         </is>
       </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="38" ht="29" customHeight="1">
       <c r="A38" s="15" t="inlineStr">
@@ -5604,6 +5687,11 @@
           <t>Secondary Outcome Measure</t>
         </is>
       </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="39" ht="43.5" customHeight="1">
       <c r="A39" s="15" t="inlineStr">
@@ -5630,6 +5718,11 @@
       <c r="F39" s="14" t="inlineStr">
         <is>
           <t>Pharmacologic Class</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5656,6 +5749,11 @@
           <t>Pediatric Investigation Plan Indicator</t>
         </is>
       </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="41" ht="72.5" customHeight="1">
       <c r="A41" s="15" t="inlineStr">
@@ -5682,7 +5780,7 @@
       </c>
       <c r="G41" s="31" t="inlineStr">
         <is>
-          <t xml:space="preserve">study.versions.studyDesigns.population.plannedEnrollmentNumber.value </t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5711,6 +5809,11 @@
       <c r="F42" s="14" t="inlineStr">
         <is>
           <t>Planned Duration of Intervention Value + Unit</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5737,6 +5840,11 @@
           <t>Randomized Indicator</t>
         </is>
       </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="15" t="inlineStr">
@@ -5761,6 +5869,11 @@
           <t>Rare disease indicator</t>
         </is>
       </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="45" ht="43.5" customHeight="1">
       <c r="A45" s="15" t="inlineStr">
@@ -5793,6 +5906,11 @@
           <t>Registry Identifier</t>
         </is>
       </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="46" ht="43.5" customHeight="1">
       <c r="A46" s="15" t="inlineStr">
@@ -5825,6 +5943,11 @@
           <t>Route of Administration</t>
         </is>
       </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="47" ht="58" customHeight="1">
       <c r="A47" s="15" t="inlineStr">
@@ -5855,6 +5978,11 @@
       <c r="F47" s="14" t="inlineStr">
         <is>
           <t>Retained Biospecimen Description</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5881,6 +6009,11 @@
           <t>Sex of Participants</t>
         </is>
       </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="49" ht="29" customHeight="1">
       <c r="A49" s="15" t="inlineStr">
@@ -5907,7 +6040,7 @@
       </c>
       <c r="G49" s="32" t="inlineStr">
         <is>
-          <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5936,6 +6069,11 @@
       <c r="F50" s="14" t="inlineStr">
         <is>
           <t>Sponsor's Study Reference ID</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5962,6 +6100,11 @@
           <t>Single Site Eu State Trial Indicator</t>
         </is>
       </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="52" ht="29" customHeight="1">
       <c r="A52" s="15" t="inlineStr">
@@ -5986,6 +6129,11 @@
           <t>Study Type</t>
         </is>
       </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="53" ht="87" customHeight="1">
       <c r="A53" s="15" t="inlineStr">
@@ -6012,11 +6160,6 @@
       </c>
       <c r="G53" s="31" t="inlineStr">
         <is>
-          <t>study.versions.studyDesigns.blindingSchema.standardCode.decode</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
           <t>Double Blind Study</t>
         </is>
       </c>
@@ -6044,6 +6187,11 @@
           <t>Intervention Control Type</t>
         </is>
       </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="15" t="inlineStr">
@@ -6068,6 +6216,11 @@
           <t>Therapeutic Area</t>
         </is>
       </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="56" ht="29" customHeight="1">
       <c r="A56" s="15" t="inlineStr">
@@ -6094,6 +6247,11 @@
       <c r="F56" s="14" t="inlineStr">
         <is>
           <t>Trial Intent Types</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6122,11 +6280,6 @@
       </c>
       <c r="G57" s="31" t="inlineStr">
         <is>
-          <t>study.versions.titles[type.code="C207616"].text</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
           <t>Safety and Efficacy of the Xanomeline Transdermal Therapeutic System (TTS) in Patients with Mild to Moderate Alzheimer's Disease</t>
         </is>
       </c>
@@ -6156,7 +6309,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>study.study.versions.studyDesigns.studyPhase.standardCode.decode</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6189,6 +6342,11 @@
       <c r="F59" s="14" t="inlineStr">
         <is>
           <t>Investigational Intervention</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6213,6 +6371,11 @@
       <c r="F60" s="14" t="inlineStr">
         <is>
           <t>Trial Type</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
debugged for integer results issue
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -4592,7 +4592,7 @@
       </c>
       <c r="G5" s="31" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="G6" s="31" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="G7" s="31" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4703,7 +4703,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4740,7 +4740,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4814,7 +4814,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4843,7 +4843,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4880,7 +4880,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5111,7 +5111,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5140,7 +5140,7 @@
       </c>
       <c r="G21" s="31" t="inlineStr">
         <is>
-          <t>study.versions.studyDesigns.indications.label</t>
+          <t>["Parkinson's disease", "Parkinson's disease"]</t>
         </is>
       </c>
     </row>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5293,7 +5293,7 @@
       </c>
       <c r="G26" s="31" t="inlineStr">
         <is>
-          <t>$count(study.versions.studyDesigns.arms)</t>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5351,7 +5351,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5388,7 +5388,7 @@
       </c>
       <c r="G29" s="33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5462,7 +5462,7 @@
       </c>
       <c r="G31" s="39" t="inlineStr">
         <is>
-          <t>study.versions.studyDesigns.objectives[level.code="C85827"].{id: text}</t>
+          <t>{'Objective_2': '•\tTo evaluate the safety and tolerability of intravenous infusions of Beroclin administered once daily in subjects with early stage Parkinson s disease.'}</t>
         </is>
       </c>
     </row>
@@ -5491,7 +5491,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5549,7 +5549,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5578,7 +5578,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5615,7 +5615,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5689,7 +5689,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5751,7 +5751,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5780,7 +5780,7 @@
       </c>
       <c r="G41" s="31" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5842,7 +5842,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5871,7 +5871,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5945,7 +5945,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6040,7 +6040,7 @@
       </c>
       <c r="G49" s="32" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6102,7 +6102,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6131,7 +6131,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6309,7 +6309,7 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6346,7 +6346,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t> </t>
+          <t>None</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code Update with error message for jsonata code
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -4468,7 +4468,7 @@
       </c>
       <c r="G1" s="30" t="inlineStr">
         <is>
-          <t>Mapping Result</t>
+          <t>Mapping Results</t>
         </is>
       </c>
     </row>
@@ -4703,7 +4703,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4740,7 +4740,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4777,7 +4777,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4814,7 +4814,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4843,7 +4843,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4880,7 +4880,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4991,7 +4991,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5082,7 +5082,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5111,7 +5111,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5235,7 +5235,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5264,7 +5264,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5322,7 +5322,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5351,7 +5351,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5491,7 +5491,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5549,7 +5549,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5578,7 +5578,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5615,7 +5615,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5689,7 +5689,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5722,7 +5722,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5751,7 +5751,7 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5813,7 +5813,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5842,7 +5842,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5871,7 +5871,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5945,7 +5945,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5982,7 +5982,7 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6011,7 +6011,7 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6040,7 +6040,7 @@
       </c>
       <c r="G49" s="32" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>Error in expression for Clinical Study Sponsor; Sponsor; Study Sponsor: study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
         </is>
       </c>
     </row>
@@ -6073,7 +6073,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6102,7 +6102,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6131,7 +6131,7 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6346,7 +6346,7 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -6375,7 +6375,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>None</t>
+          <t> </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
new run with more mappings
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="38040" yWindow="-10920" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-12030" yWindow="-21600" windowWidth="30435" windowHeight="20985" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" state="visible" r:id="rId1"/>
@@ -14,7 +14,9 @@
     <sheet name="TS" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="TS Parameters" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'TS Parameters'!$A$1:$G$60</definedName>
+  </definedNames>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -348,12 +350,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -363,12 +359,10 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -381,7 +375,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -982,7 +982,7 @@
       <c r="C1" s="41" t="n"/>
       <c r="D1" s="41" t="n"/>
       <c r="E1" s="42" t="n"/>
-      <c r="F1" s="38" t="inlineStr">
+      <c r="F1" s="36" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -1778,7 +1778,7 @@
       <c r="C1" s="41" t="n"/>
       <c r="D1" s="41" t="n"/>
       <c r="E1" s="42" t="n"/>
-      <c r="F1" s="38" t="inlineStr">
+      <c r="F1" s="36" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -2364,7 +2364,7 @@
       <c r="C1" s="41" t="n"/>
       <c r="D1" s="41" t="n"/>
       <c r="E1" s="42" t="n"/>
-      <c r="F1" s="38" t="inlineStr">
+      <c r="F1" s="36" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -3093,7 +3093,7 @@
       <c r="C1" s="41" t="n"/>
       <c r="D1" s="41" t="n"/>
       <c r="E1" s="42" t="n"/>
-      <c r="F1" s="38" t="inlineStr">
+      <c r="F1" s="36" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -3706,141 +3706,114 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
   <cols>
-    <col width="14.6328125" customWidth="1" style="16" min="1" max="5"/>
-    <col width="21.453125" customWidth="1" style="16" min="6" max="7"/>
-    <col width="39" customWidth="1" style="16" min="8" max="8"/>
-    <col width="21.453125" customWidth="1" style="16" min="9" max="10"/>
-    <col width="32.6328125" customWidth="1" style="16" min="11" max="12"/>
-    <col width="21.453125" customWidth="1" style="16" min="13" max="15"/>
-    <col width="17.36328125" customWidth="1" style="29" min="16" max="16"/>
-    <col width="8.6328125" customWidth="1" style="16" min="17" max="16384"/>
+    <col width="19.7265625" bestFit="1" customWidth="1" style="16" min="1" max="1"/>
+    <col width="19" bestFit="1" customWidth="1" style="16" min="2" max="2"/>
+    <col width="7.6328125" bestFit="1" customWidth="1" style="16" min="3" max="3"/>
+    <col width="14.6328125" customWidth="1" style="16" min="4" max="5"/>
+    <col width="21.453125" customWidth="1" style="16" min="6" max="6"/>
+    <col width="26.6328125" customWidth="1" style="16" min="7" max="7"/>
+    <col width="29.81640625" customWidth="1" style="16" min="8" max="8"/>
+    <col width="8.6328125" customWidth="1" style="16" min="9" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="21" customHeight="1">
-      <c r="A1" s="40" t="inlineStr">
-        <is>
-          <t>SDTM</t>
-        </is>
-      </c>
-      <c r="B1" s="41" t="n"/>
-      <c r="C1" s="41" t="n"/>
-      <c r="D1" s="41" t="n"/>
-      <c r="E1" s="42" t="n"/>
-      <c r="F1" s="38" t="inlineStr">
-        <is>
-          <t>USDM</t>
-        </is>
-      </c>
-      <c r="G1" s="41" t="n"/>
-      <c r="H1" s="41" t="n"/>
-      <c r="I1" s="41" t="n"/>
-      <c r="J1" s="41" t="n"/>
-      <c r="K1" s="41" t="n"/>
-      <c r="L1" s="41" t="n"/>
-      <c r="M1" s="41" t="n"/>
-      <c r="N1" s="41" t="n"/>
-      <c r="O1" s="41" t="n"/>
-      <c r="P1" s="42" t="n"/>
-    </row>
-    <row r="2" ht="21" customHeight="1">
-      <c r="A2" s="10" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">Variable Name </t>
         </is>
       </c>
-      <c r="B2" s="10" t="inlineStr">
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">Variable Label </t>
         </is>
       </c>
-      <c r="C2" s="10" t="inlineStr">
+      <c r="C1" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">Type </t>
         </is>
       </c>
-      <c r="D2" s="10" t="inlineStr">
+      <c r="D1" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">Role </t>
         </is>
       </c>
-      <c r="E2" s="10" t="inlineStr">
+      <c r="E1" s="10" t="inlineStr">
         <is>
           <t xml:space="preserve">Core </t>
         </is>
       </c>
-      <c r="F2" s="11" t="inlineStr">
-        <is>
-          <t>Class</t>
-        </is>
-      </c>
-      <c r="G2" s="11" t="inlineStr">
-        <is>
-          <t>Attribute</t>
-        </is>
-      </c>
-      <c r="H2" s="11" t="inlineStr">
-        <is>
-          <t>Overall Notes</t>
-        </is>
-      </c>
-      <c r="I2" s="11" t="inlineStr">
-        <is>
-          <t>Target Path</t>
-        </is>
-      </c>
-      <c r="J2" s="11" t="inlineStr">
-        <is>
-          <t>Target Notes</t>
-        </is>
-      </c>
-      <c r="K2" s="11" t="inlineStr">
-        <is>
-          <t>Condition Path</t>
-        </is>
-      </c>
-      <c r="L2" s="11" t="inlineStr">
-        <is>
-          <t>Condition Notes</t>
-        </is>
-      </c>
-      <c r="M2" s="11" t="inlineStr">
+      <c r="F1" s="11" t="inlineStr">
         <is>
           <t>Mapping Name</t>
         </is>
       </c>
-      <c r="N2" s="11" t="inlineStr">
-        <is>
-          <t>Mapping Category</t>
-        </is>
-      </c>
-      <c r="O2" s="11" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="P2" s="24" t="inlineStr">
-        <is>
-          <t xml:space="preserve">v4.0 Change </t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="93" customHeight="1">
+      <c r="G1" s="10" t="inlineStr">
+        <is>
+          <t>JSONATA</t>
+        </is>
+      </c>
+      <c r="H1" s="28" t="inlineStr">
+        <is>
+          <t>Fixed content</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="93" customHeight="1">
+      <c r="A2" s="9" t="inlineStr">
+        <is>
+          <t>STUDYID</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="inlineStr">
+        <is>
+          <t>Study Identifier</t>
+        </is>
+      </c>
+      <c r="C2" s="9" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="D2" s="9" t="inlineStr">
+        <is>
+          <t>Identifier</t>
+        </is>
+      </c>
+      <c r="E2" s="9" t="inlineStr">
+        <is>
+          <t>Req</t>
+        </is>
+      </c>
+      <c r="F2" s="6" t="inlineStr">
+        <is>
+          <t>Sponsor Study Identifier</t>
+        </is>
+      </c>
+      <c r="G2" s="37" t="inlineStr">
+        <is>
+          <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];
+studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
+        </is>
+      </c>
+      <c r="H2" s="39" t="n"/>
+    </row>
+    <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>STUDYID</t>
+          <t>DOMAIN</t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>Study Identifier</t>
+          <t>Domain Abbreviation</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
@@ -3858,403 +3831,271 @@
           <t>Req</t>
         </is>
       </c>
-      <c r="F3" s="6" t="inlineStr">
-        <is>
-          <t>StudyIdentifier</t>
-        </is>
-      </c>
-      <c r="G3" s="6" t="inlineStr">
-        <is>
-          <t>text</t>
-        </is>
-      </c>
-      <c r="H3" s="6" t="n"/>
-      <c r="I3" s="6" t="inlineStr">
-        <is>
-          <t>StudyVersion/@studyIdentifiers/StudyIdentifier/@text</t>
-        </is>
-      </c>
-      <c r="J3" s="6" t="n"/>
-      <c r="K3" s="6" t="inlineStr">
-        <is>
-          <t>StudyRole/@code/Code/@code="C70793" | 
-StudyRole/@organizations | 
-StudyVersion/@studyIdentifiers/StudyIdentifier/@scope</t>
-        </is>
-      </c>
-      <c r="L3" s="6" t="inlineStr">
-        <is>
-          <t>Identifies the sponsor role | 
-Identifies the sponsor organization from the role | 
-Identifies the sponsor organization from the study identifier</t>
-        </is>
-      </c>
-      <c r="M3" s="6" t="inlineStr">
-        <is>
-          <t>Sponsor Study Identifier</t>
-        </is>
-      </c>
-      <c r="N3" s="6" t="inlineStr">
-        <is>
-          <t>Study Identifier</t>
-        </is>
-      </c>
-      <c r="O3" s="6" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P3" s="26" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="29" customHeight="1">
+      <c r="F3" s="5" t="n"/>
+      <c r="G3" s="38" t="n"/>
+      <c r="H3" s="9" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>DOMAIN</t>
+          <t>TSSEQ</t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>Domain Abbreviation</t>
+          <t>Sequence Number</t>
         </is>
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
+          <t>Num</t>
+        </is>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t>Identifier</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t>Req</t>
+        </is>
+      </c>
+      <c r="F4" s="12" t="n"/>
+      <c r="G4" s="38" t="n"/>
+      <c r="H4" s="39" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="9" t="inlineStr">
+        <is>
+          <t>TSGRPID</t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="inlineStr">
+        <is>
+          <t>Group ID</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
           <t>Char</t>
         </is>
       </c>
-      <c r="D4" s="9" t="inlineStr">
+      <c r="D5" s="9" t="inlineStr">
         <is>
           <t>Identifier</t>
         </is>
       </c>
-      <c r="E4" s="9" t="inlineStr">
+      <c r="E5" s="9" t="inlineStr">
+        <is>
+          <t>Perm</t>
+        </is>
+      </c>
+      <c r="F5" s="12" t="n"/>
+      <c r="G5" s="38" t="n"/>
+      <c r="H5" s="39" t="n"/>
+    </row>
+    <row r="6" ht="43.5" customHeight="1">
+      <c r="A6" s="9" t="inlineStr">
+        <is>
+          <t>TSPARMCD</t>
+        </is>
+      </c>
+      <c r="B6" s="9" t="inlineStr">
+        <is>
+          <t>Trial Summary Parameter Short Name</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t>Topic</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
         <is>
           <t>Req</t>
         </is>
       </c>
-      <c r="F4" s="5" t="n"/>
-      <c r="G4" s="5" t="n"/>
-      <c r="H4" s="9" t="inlineStr">
-        <is>
-          <t>Set to "TS"</t>
-        </is>
-      </c>
-      <c r="I4" s="5" t="n"/>
-      <c r="J4" s="5" t="n"/>
-      <c r="K4" s="5" t="n"/>
-      <c r="L4" s="5" t="n"/>
-      <c r="M4" s="5" t="n"/>
-      <c r="N4" s="5" t="n"/>
-      <c r="O4" s="5" t="n"/>
-      <c r="P4" s="28" t="n"/>
-    </row>
-    <row r="5" ht="29" customHeight="1">
-      <c r="A5" s="9" t="inlineStr">
-        <is>
-          <t>TSSEQ</t>
-        </is>
-      </c>
-      <c r="B5" s="9" t="inlineStr">
-        <is>
-          <t>Sequence Number</t>
-        </is>
-      </c>
-      <c r="C5" s="9" t="inlineStr">
-        <is>
-          <t>Num</t>
-        </is>
-      </c>
-      <c r="D5" s="9" t="inlineStr">
-        <is>
-          <t>Identifier</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
+      <c r="F6" s="12" t="n"/>
+      <c r="G6" s="38" t="n"/>
+      <c r="H6" s="39" t="n"/>
+    </row>
+    <row r="7" ht="29" customHeight="1">
+      <c r="A7" s="9" t="inlineStr">
+        <is>
+          <t>TSPARM</t>
+        </is>
+      </c>
+      <c r="B7" s="9" t="inlineStr">
+        <is>
+          <t>Trial Summary Parameter</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t>Synonym Qualifier</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="inlineStr">
         <is>
           <t>Req</t>
         </is>
       </c>
-      <c r="F5" s="12" t="n"/>
-      <c r="G5" s="12" t="n"/>
-      <c r="H5" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Will be mapped per trial summary parameter </t>
-        </is>
-      </c>
-      <c r="I5" s="12" t="n"/>
-      <c r="J5" s="5" t="n"/>
-      <c r="K5" s="4" t="n"/>
-      <c r="L5" s="5" t="n"/>
-      <c r="M5" s="12" t="n"/>
-      <c r="N5" s="5" t="n"/>
-      <c r="O5" s="5" t="n"/>
-      <c r="P5" s="28" t="n"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="9" t="inlineStr">
-        <is>
-          <t>TSGRPID</t>
-        </is>
-      </c>
-      <c r="B6" s="9" t="inlineStr">
-        <is>
-          <t>Group ID</t>
-        </is>
-      </c>
-      <c r="C6" s="9" t="inlineStr">
+      <c r="F7" s="12" t="n"/>
+      <c r="G7" s="38" t="n"/>
+      <c r="H7" s="39" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>TSVAL</t>
+        </is>
+      </c>
+      <c r="B8" s="9" t="inlineStr">
+        <is>
+          <t>Parameter Value</t>
+        </is>
+      </c>
+      <c r="C8" s="9" t="inlineStr">
         <is>
           <t>Char</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t>Identifier</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
+      <c r="D8" s="9" t="inlineStr">
+        <is>
+          <t>Result Qualifier</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="F8" s="12" t="n"/>
+      <c r="G8" s="38" t="n"/>
+      <c r="H8" s="39" t="n"/>
+    </row>
+    <row r="9" ht="29" customHeight="1">
+      <c r="A9" s="9" t="inlineStr">
+        <is>
+          <t>TSVALNF</t>
+        </is>
+      </c>
+      <c r="B9" s="9" t="inlineStr">
+        <is>
+          <t>Parameter Value Null Flavor</t>
+        </is>
+      </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t>Result Qualifier</t>
+        </is>
+      </c>
+      <c r="E9" s="9" t="inlineStr">
         <is>
           <t>Perm</t>
         </is>
       </c>
-      <c r="F6" s="12" t="n"/>
-      <c r="G6" s="12" t="n"/>
-      <c r="H6" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Will be mapped per trial summary parameter </t>
-        </is>
-      </c>
-      <c r="I6" s="12" t="n"/>
-      <c r="J6" s="5" t="n"/>
-      <c r="K6" s="4" t="n"/>
-      <c r="L6" s="5" t="n"/>
-      <c r="M6" s="12" t="n"/>
-      <c r="N6" s="5" t="n"/>
-      <c r="O6" s="5" t="n"/>
-      <c r="P6" s="28" t="n"/>
-    </row>
-    <row r="7" ht="43.5" customHeight="1">
-      <c r="A7" s="9" t="inlineStr">
-        <is>
-          <t>TSPARMCD</t>
-        </is>
-      </c>
-      <c r="B7" s="9" t="inlineStr">
-        <is>
-          <t>Trial Summary Parameter Short Name</t>
-        </is>
-      </c>
-      <c r="C7" s="9" t="inlineStr">
+      <c r="F9" s="12" t="n"/>
+      <c r="G9" s="38" t="n"/>
+      <c r="H9" s="39" t="n"/>
+    </row>
+    <row r="10" ht="29" customHeight="1">
+      <c r="A10" s="9" t="inlineStr">
+        <is>
+          <t>TSVALCD</t>
+        </is>
+      </c>
+      <c r="B10" s="9" t="inlineStr">
+        <is>
+          <t>Parameter Value Code</t>
+        </is>
+      </c>
+      <c r="C10" s="9" t="inlineStr">
         <is>
           <t>Char</t>
         </is>
       </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t>Topic</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
-        <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F7" s="12" t="n"/>
-      <c r="G7" s="12" t="n"/>
-      <c r="H7" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Will be mapped per trial summary parameter </t>
-        </is>
-      </c>
-      <c r="I7" s="12" t="n"/>
-      <c r="J7" s="5" t="n"/>
-      <c r="K7" s="4" t="n"/>
-      <c r="L7" s="5" t="n"/>
-      <c r="M7" s="12" t="n"/>
-      <c r="N7" s="5" t="n"/>
-      <c r="O7" s="5" t="n"/>
-      <c r="P7" s="28" t="n"/>
-    </row>
-    <row r="8" ht="29" customHeight="1">
-      <c r="A8" s="9" t="inlineStr">
-        <is>
-          <t>TSPARM</t>
-        </is>
-      </c>
-      <c r="B8" s="9" t="inlineStr">
-        <is>
-          <t>Trial Summary Parameter</t>
-        </is>
-      </c>
-      <c r="C8" s="9" t="inlineStr">
+      <c r="D10" s="9" t="inlineStr">
+        <is>
+          <t>Result Qualifier</t>
+        </is>
+      </c>
+      <c r="E10" s="9" t="inlineStr">
+        <is>
+          <t>Exp</t>
+        </is>
+      </c>
+      <c r="F10" s="12" t="n"/>
+      <c r="G10" s="38" t="n"/>
+      <c r="H10" s="39" t="n"/>
+    </row>
+    <row r="11" ht="29" customHeight="1">
+      <c r="A11" s="9" t="inlineStr">
+        <is>
+          <t>TSVCDREF</t>
+        </is>
+      </c>
+      <c r="B11" s="9" t="inlineStr">
+        <is>
+          <t>Name of Reference Terminology</t>
+        </is>
+      </c>
+      <c r="C11" s="9" t="inlineStr">
         <is>
           <t>Char</t>
         </is>
       </c>
-      <c r="D8" s="9" t="inlineStr">
-        <is>
-          <t>Synonym Qualifier</t>
-        </is>
-      </c>
-      <c r="E8" s="9" t="inlineStr">
-        <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F8" s="12" t="n"/>
-      <c r="G8" s="12" t="n"/>
-      <c r="H8" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Will be mapped per trial summary parameter </t>
-        </is>
-      </c>
-      <c r="I8" s="12" t="n"/>
-      <c r="J8" s="5" t="n"/>
-      <c r="K8" s="4" t="n"/>
-      <c r="L8" s="5" t="n"/>
-      <c r="M8" s="12" t="n"/>
-      <c r="N8" s="5" t="n"/>
-      <c r="O8" s="5" t="n"/>
-      <c r="P8" s="28" t="n"/>
-    </row>
-    <row r="9" ht="87" customHeight="1">
-      <c r="A9" s="9" t="inlineStr">
-        <is>
-          <t>TSVAL</t>
-        </is>
-      </c>
-      <c r="B9" s="9" t="inlineStr">
-        <is>
-          <t>Parameter Value</t>
-        </is>
-      </c>
-      <c r="C9" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
+      <c r="D11" s="9" t="inlineStr">
         <is>
           <t>Result Qualifier</t>
         </is>
       </c>
-      <c r="E9" s="9" t="inlineStr">
+      <c r="E11" s="9" t="inlineStr">
         <is>
           <t>Exp</t>
         </is>
       </c>
-      <c r="F9" s="12" t="n"/>
-      <c r="G9" s="12" t="n"/>
-      <c r="H9" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Will be mapped per trial summary parameter. When the mapping resolved to Yes or No values, then the corresponding CDISC CT codes need to be used; TSVAL="Y" and TSVALCD="C49488" or TSVAL="N" and TSVALCD="C49487" </t>
-        </is>
-      </c>
-      <c r="I9" s="12" t="n"/>
-      <c r="J9" s="5" t="n"/>
-      <c r="K9" s="5" t="n"/>
-      <c r="L9" s="5" t="n"/>
-      <c r="M9" s="12" t="n"/>
-      <c r="N9" s="5" t="n"/>
-      <c r="O9" s="5" t="n"/>
-      <c r="P9" s="28" t="n"/>
-    </row>
-    <row r="10" ht="43.5" customHeight="1">
-      <c r="A10" s="9" t="inlineStr">
-        <is>
-          <t>TSVALNF</t>
-        </is>
-      </c>
-      <c r="B10" s="9" t="inlineStr">
-        <is>
-          <t>Parameter Value Null Flavor</t>
-        </is>
-      </c>
-      <c r="C10" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D10" s="9" t="inlineStr">
-        <is>
-          <t>Result Qualifier</t>
-        </is>
-      </c>
-      <c r="E10" s="9" t="inlineStr">
-        <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="F10" s="12" t="n"/>
-      <c r="G10" s="12" t="n"/>
-      <c r="H10" s="4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Will be mapped per trial summary parameter </t>
-        </is>
-      </c>
-      <c r="I10" s="12" t="n"/>
-      <c r="J10" s="5" t="n"/>
-      <c r="K10" s="4" t="n"/>
-      <c r="L10" s="5" t="n"/>
-      <c r="M10" s="12" t="n"/>
-      <c r="N10" s="5" t="n"/>
-      <c r="O10" s="5" t="n"/>
-      <c r="P10" s="28" t="n"/>
-    </row>
-    <row r="11" ht="87" customHeight="1">
-      <c r="A11" s="9" t="inlineStr">
-        <is>
-          <t>TSVALCD</t>
-        </is>
-      </c>
-      <c r="B11" s="9" t="inlineStr">
-        <is>
-          <t>Parameter Value Code</t>
-        </is>
-      </c>
-      <c r="C11" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D11" s="9" t="inlineStr">
-        <is>
-          <t>Result Qualifier</t>
-        </is>
-      </c>
-      <c r="E11" s="9" t="inlineStr">
-        <is>
-          <t>Exp</t>
-        </is>
-      </c>
-      <c r="F11" s="12" t="n"/>
-      <c r="G11" s="12" t="n"/>
-      <c r="H11" s="12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Will be mapped per trial summary parameter. When the mapping resolved to Yes or No values, then the corresponding CDISC CT codes need to be used; TSVAL="Y" and TSVALCD="C49488" or TSVAL="N" and TSVALCD="C49487" </t>
-        </is>
-      </c>
-      <c r="I11" s="12" t="n"/>
-      <c r="J11" s="5" t="n"/>
-      <c r="K11" s="4" t="n"/>
-      <c r="L11" s="5" t="n"/>
-      <c r="M11" s="12" t="n"/>
-      <c r="N11" s="5" t="n"/>
-      <c r="O11" s="5" t="n"/>
-      <c r="P11" s="28" t="n"/>
+      <c r="F11" s="12" t="inlineStr">
+        <is>
+          <t>Name of Reference Terminology</t>
+        </is>
+      </c>
+      <c r="G11" s="38" t="inlineStr">
+        <is>
+          <t>..code.codeSystem</t>
+        </is>
+      </c>
+      <c r="H11" s="39" t="n"/>
     </row>
     <row r="12" ht="43.5" customHeight="1">
       <c r="A12" s="9" t="inlineStr">
         <is>
-          <t>TSVCDREF</t>
+          <t>TSVCDVER</t>
         </is>
       </c>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>Name of Reference Terminology</t>
+          <t>Version of the Reference Terminology</t>
         </is>
       </c>
       <c r="C12" s="9" t="inlineStr">
@@ -4274,119 +4115,17 @@
       </c>
       <c r="F12" s="12" t="inlineStr">
         <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="G12" s="12" t="inlineStr">
-        <is>
-          <t>codeSystem</t>
-        </is>
-      </c>
-      <c r="H12" s="12" t="n"/>
-      <c r="I12" s="12" t="inlineStr">
-        <is>
-          <t>code/@codeSystem</t>
-        </is>
-      </c>
-      <c r="J12" s="5" t="inlineStr">
-        <is>
-          <t>Align path to the corresponding code or decode mapped for the specific code item it refers to.</t>
-        </is>
-      </c>
-      <c r="K12" s="4" t="inlineStr"/>
-      <c r="L12" s="5" t="inlineStr"/>
-      <c r="M12" s="12" t="inlineStr">
-        <is>
-          <t>Name of Reference Terminology</t>
-        </is>
-      </c>
-      <c r="N12" s="5" t="inlineStr">
-        <is>
-          <t>Study Design</t>
-        </is>
-      </c>
-      <c r="O12" s="5" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P12" s="28" t="n"/>
-    </row>
-    <row r="13" ht="43.5" customHeight="1">
-      <c r="A13" s="9" t="inlineStr">
-        <is>
-          <t>TSVCDVER</t>
-        </is>
-      </c>
-      <c r="B13" s="9" t="inlineStr">
-        <is>
-          <t>Version of the Reference Terminology</t>
-        </is>
-      </c>
-      <c r="C13" s="9" t="inlineStr">
-        <is>
-          <t>Char</t>
-        </is>
-      </c>
-      <c r="D13" s="9" t="inlineStr">
-        <is>
-          <t>Result Qualifier</t>
-        </is>
-      </c>
-      <c r="E13" s="9" t="inlineStr">
-        <is>
-          <t>Exp</t>
-        </is>
-      </c>
-      <c r="F13" s="12" t="inlineStr">
-        <is>
-          <t>Code</t>
-        </is>
-      </c>
-      <c r="G13" s="12" t="inlineStr">
-        <is>
-          <t>codeSystemVersion</t>
-        </is>
-      </c>
-      <c r="H13" s="12" t="n"/>
-      <c r="I13" s="12" t="inlineStr">
-        <is>
-          <t>code/@codeSystemVersion</t>
-        </is>
-      </c>
-      <c r="J13" s="5" t="inlineStr">
-        <is>
-          <t>Align path to the corresponding code or decode mapped for the specific code item it refers to.</t>
-        </is>
-      </c>
-      <c r="K13" s="4" t="inlineStr"/>
-      <c r="L13" s="5" t="inlineStr"/>
-      <c r="M13" s="12" t="inlineStr">
-        <is>
           <t>Version of Reference Terminology</t>
         </is>
       </c>
-      <c r="N13" s="5" t="inlineStr">
-        <is>
-          <t>Study Design</t>
-        </is>
-      </c>
-      <c r="O13" s="5" t="inlineStr">
-        <is>
-          <t>Mapped</t>
-        </is>
-      </c>
-      <c r="P13" s="28" t="n"/>
+      <c r="G12" s="38" t="inlineStr">
+        <is>
+          <t>..code.codeSystemVersion</t>
+        </is>
+      </c>
+      <c r="H12" s="39" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F1:P1"/>
-    <mergeCell ref="A1:E1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I12" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="I13" r:id="rId2"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4399,8 +4138,8 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="182" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.81640625" defaultRowHeight="14.5"/>
@@ -4446,7 +4185,7 @@
           <t>Mapping Name</t>
         </is>
       </c>
-      <c r="G1" s="30" t="inlineStr">
+      <c r="G1" s="28" t="inlineStr">
         <is>
           <t>Mapping Results</t>
         </is>
@@ -4475,7 +4214,7 @@
           <t>Adaptive Design Indicator</t>
         </is>
       </c>
-      <c r="G2" s="34" t="inlineStr">
+      <c r="G2" s="31" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
@@ -4504,7 +4243,7 @@
           <t>Study Minimum Age + Unit Study Population</t>
         </is>
       </c>
-      <c r="G3" s="34" t="inlineStr">
+      <c r="G3" s="31" t="inlineStr">
         <is>
           <t xml:space="preserve">18 ["Year","Year"] </t>
         </is>
@@ -4533,7 +4272,7 @@
           <t>Study Maximum Age + Unit Study Population</t>
         </is>
       </c>
-      <c r="G4" s="31" t="inlineStr">
+      <c r="G4" s="29" t="inlineStr">
         <is>
           <t xml:space="preserve">100 ["Year","Year"] </t>
         </is>
@@ -4570,7 +4309,7 @@
           <t>Biospecimen retention contains DNA indicator</t>
         </is>
       </c>
-      <c r="G5" s="31" t="inlineStr">
+      <c r="G5" s="29" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4607,7 +4346,7 @@
           <t>Biospecimen retention indicator</t>
         </is>
       </c>
-      <c r="G6" s="31" t="inlineStr">
+      <c r="G6" s="29" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4639,12 +4378,8 @@
           <t>If applicable, combine with the corresponding intervention variables by a common unique tsgrpid</t>
         </is>
       </c>
-      <c r="F7" s="14" t="inlineStr">
-        <is>
-          <t>(International) Non Proprietary Comparator Drug Name</t>
-        </is>
-      </c>
-      <c r="G7" s="31" t="inlineStr">
+      <c r="F7" s="14" t="n"/>
+      <c r="G7" s="29" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4752,12 +4487,12 @@
       </c>
       <c r="F10" s="14" t="inlineStr">
         <is>
-          <t>Mimimum Response Duration</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t> </t>
+          <t>Minimum Response Duration</t>
+        </is>
+      </c>
+      <c r="G10" s="29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '1 Day'}</t>
         </is>
       </c>
     </row>
@@ -4792,7 +4527,7 @@
           <t>Background treatment</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" s="29" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4858,9 +4593,9 @@
           <t>Dosage Levels</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t> </t>
+      <c r="G13" s="29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 20}</t>
         </is>
       </c>
     </row>
@@ -4895,9 +4630,9 @@
           <t>Dose Form</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t> </t>
+      <c r="G14" s="29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'TABLET'}</t>
         </is>
       </c>
     </row>
@@ -4932,9 +4667,9 @@
           <t>Administration Frequency</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t> </t>
+      <c r="G15" s="29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'BID'}</t>
         </is>
       </c>
     </row>
@@ -4969,9 +4704,9 @@
           <t>Dosage Units</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t> </t>
+      <c r="G16" s="29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'Milligram'}</t>
         </is>
       </c>
     </row>
@@ -5118,7 +4853,7 @@
           <t>Study design Diagnosis or Condition</t>
         </is>
       </c>
-      <c r="G21" s="31" t="inlineStr">
+      <c r="G21" s="29" t="inlineStr">
         <is>
           <t>["Parkinson's disease", "Parkinson's disease"]</t>
         </is>
@@ -5147,7 +4882,7 @@
           <t>Intervention Model</t>
         </is>
       </c>
-      <c r="G22" s="32" t="inlineStr">
+      <c r="G22" s="30" t="inlineStr">
         <is>
           <t>PARALLEL</t>
         </is>
@@ -5184,9 +4919,9 @@
           <t>Intervention Type</t>
         </is>
       </c>
-      <c r="G23" s="31" t="inlineStr">
-        <is>
-          <t>Pharmacologic Substance</t>
+      <c r="G23" s="29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'Pharmacologic Substance'}</t>
         </is>
       </c>
     </row>
@@ -5271,7 +5006,7 @@
           <t>Number of Arms</t>
         </is>
       </c>
-      <c r="G26" s="31" t="inlineStr">
+      <c r="G26" s="29" t="inlineStr">
         <is>
           <t>2</t>
         </is>
@@ -5366,7 +5101,7 @@
           <t>Exploratory Objective</t>
         </is>
       </c>
-      <c r="G29" s="33" t="inlineStr">
+      <c r="G29" s="29" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -5403,7 +5138,7 @@
           <t>Primary Objective</t>
         </is>
       </c>
-      <c r="G30" s="33" t="inlineStr">
+      <c r="G30" s="29" t="inlineStr">
         <is>
           <t>{'Objective_1': '•\tTo evaluate the effect of intravenous infusions of Beroclin administered once daily on motor symptoms in subjects with early stage Parkinson s disease.'}</t>
         </is>
@@ -5440,7 +5175,7 @@
           <t>Secondary Objective</t>
         </is>
       </c>
-      <c r="G31" s="33" t="inlineStr">
+      <c r="G31" s="29" t="inlineStr">
         <is>
           <t>{'Objective_2': '•\tTo evaluate the safety and tolerability of intravenous infusions of Beroclin administered once daily in subjects with early stage Parkinson s disease.'}</t>
         </is>
@@ -5469,7 +5204,7 @@
           <t>Observational Model</t>
         </is>
       </c>
-      <c r="G32" s="39" t="inlineStr">
+      <c r="G32" s="32" t="inlineStr">
         <is>
           <t>COHORT</t>
         </is>
@@ -5498,7 +5233,7 @@
           <t>Observational Time Perspective</t>
         </is>
       </c>
-      <c r="G33" s="32" t="inlineStr">
+      <c r="G33" s="30" t="inlineStr">
         <is>
           <t>PROSPECTIVE</t>
         </is>
@@ -5527,7 +5262,7 @@
           <t>Observational Study Population Description</t>
         </is>
       </c>
-      <c r="G34" s="32" t="inlineStr">
+      <c r="G34" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -5556,7 +5291,7 @@
           <t>Observational Study Sampling Method</t>
         </is>
       </c>
-      <c r="G35" s="32" t="inlineStr">
+      <c r="G35" s="30" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -5593,7 +5328,7 @@
           <t>Exploratory Outcome Measure</t>
         </is>
       </c>
-      <c r="G36" s="31" t="inlineStr">
+      <c r="G36" s="29" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -5630,7 +5365,7 @@
           <t>Primary Outcome Measure</t>
         </is>
       </c>
-      <c r="G37" s="31" t="inlineStr">
+      <c r="G37" s="29" t="inlineStr">
         <is>
           <t>{}</t>
         </is>
@@ -5667,7 +5402,7 @@
           <t>Secondary Outcome Measure</t>
         </is>
       </c>
-      <c r="G38" s="31" t="inlineStr">
+      <c r="G38" s="29" t="inlineStr">
         <is>
           <t>{}</t>
         </is>
@@ -5758,7 +5493,7 @@
           <t>Target Enrollment Number</t>
         </is>
       </c>
-      <c r="G41" s="31" t="inlineStr">
+      <c r="G41" s="29" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -5791,9 +5526,9 @@
           <t>Planned Duration of Intervention Value + Unit</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t> </t>
+      <c r="G42" s="30" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '14 Day'}</t>
         </is>
       </c>
     </row>
@@ -6018,7 +5753,7 @@
           <t>Sponsor Name - Organization</t>
         </is>
       </c>
-      <c r="G49" s="32" t="inlineStr">
+      <c r="G49" s="30" t="inlineStr">
         <is>
           <t>Error in expression for Clinical Study Sponsor; Sponsor; Study Sponsor: study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
         </is>
@@ -6138,13 +5873,13 @@
           <t>Blinding Schema</t>
         </is>
       </c>
-      <c r="G53" s="31" t="inlineStr">
+      <c r="G53" s="29" t="inlineStr">
         <is>
           <t>Double Blind Study</t>
         </is>
       </c>
     </row>
-    <row r="54">
+    <row r="54" ht="29" customHeight="1">
       <c r="A54" s="15" t="inlineStr">
         <is>
           <t>Control Type</t>
@@ -6167,9 +5902,9 @@
           <t>Intervention Control Type</t>
         </is>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t> </t>
+      <c r="G54" s="30" t="inlineStr">
+        <is>
+          <t>{}</t>
         </is>
       </c>
     </row>
@@ -6258,9 +5993,9 @@
           <t>Full Title</t>
         </is>
       </c>
-      <c r="G57" s="31" t="inlineStr">
-        <is>
-          <t>Safety and Efficacy of the Xanomeline Transdermal Therapeutic System (TTS) in Patients with Mild to Moderate Alzheimer's Disease</t>
+      <c r="G57" s="29" t="inlineStr">
+        <is>
+          <t>A Phase II, Placebo-, Real-World Data Controlled study of Beroclin in subjects with early Parkinson disease</t>
         </is>
       </c>
     </row>
@@ -6287,7 +6022,7 @@
           <t>Trial Phase</t>
         </is>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="G58" s="32" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -6324,9 +6059,9 @@
           <t>Investigational Intervention</t>
         </is>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t> </t>
+      <c r="G59" s="29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'LY900018'}</t>
         </is>
       </c>
     </row>
@@ -6360,6 +6095,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G60"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
test with swap columns
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -3706,7 +3706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
@@ -3727,42 +3727,57 @@
     <row r="1" ht="21" customHeight="1">
       <c r="A1" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Variable Name </t>
+          <t>STUDYID</t>
         </is>
       </c>
       <c r="B1" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Variable Label </t>
+          <t>DOMAIN</t>
         </is>
       </c>
       <c r="C1" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Type </t>
+          <t>TSSEQ</t>
         </is>
       </c>
       <c r="D1" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Role </t>
+          <t>TSGRPID</t>
         </is>
       </c>
       <c r="E1" s="10" t="inlineStr">
         <is>
-          <t xml:space="preserve">Core </t>
+          <t>TSPARMCD</t>
         </is>
       </c>
       <c r="F1" s="11" t="inlineStr">
         <is>
-          <t>Mapping Name</t>
+          <t>TSPARM</t>
         </is>
       </c>
       <c r="G1" s="10" t="inlineStr">
         <is>
-          <t>JSONATA</t>
+          <t>TSVAL</t>
         </is>
       </c>
       <c r="H1" s="28" t="inlineStr">
         <is>
-          <t>Fixed content</t>
+          <t>TSVALNF</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>TSVALCD</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>TSVCDREF</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>TSVCDVER</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
update for TS sheet
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-12030" yWindow="-21600" windowWidth="30435" windowHeight="20985" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="10875" yWindow="-18885" windowWidth="26010" windowHeight="16860" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="1" state="visible" r:id="rId1"/>
@@ -363,6 +363,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -375,13 +379,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -982,7 +982,7 @@
       <c r="C1" s="41" t="n"/>
       <c r="D1" s="41" t="n"/>
       <c r="E1" s="42" t="n"/>
-      <c r="F1" s="36" t="inlineStr">
+      <c r="F1" s="38" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -1778,7 +1778,7 @@
       <c r="C1" s="41" t="n"/>
       <c r="D1" s="41" t="n"/>
       <c r="E1" s="42" t="n"/>
-      <c r="F1" s="36" t="inlineStr">
+      <c r="F1" s="38" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -2364,7 +2364,7 @@
       <c r="C1" s="41" t="n"/>
       <c r="D1" s="41" t="n"/>
       <c r="E1" s="42" t="n"/>
-      <c r="F1" s="36" t="inlineStr">
+      <c r="F1" s="38" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -3093,7 +3093,7 @@
       <c r="C1" s="41" t="n"/>
       <c r="D1" s="41" t="n"/>
       <c r="E1" s="42" t="n"/>
-      <c r="F1" s="36" t="inlineStr">
+      <c r="F1" s="38" t="inlineStr">
         <is>
           <t>USDM</t>
         </is>
@@ -3706,10 +3706,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.6328125" defaultRowHeight="14.5"/>
@@ -3789,36 +3789,39 @@
       </c>
       <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>Study Identifier</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C2" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D2" s="9" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E2" s="9" t="inlineStr">
         <is>
-          <t>Req</t>
+          <t>ADAPT</t>
         </is>
       </c>
       <c r="F2" s="6" t="inlineStr">
         <is>
-          <t>Sponsor Study Identifier</t>
-        </is>
-      </c>
-      <c r="G2" s="37" t="inlineStr">
-        <is>
-          <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];
-studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
-        </is>
-      </c>
-      <c r="H2" s="39" t="n"/>
+          <t>Adaptive Design</t>
+        </is>
+      </c>
+      <c r="G2" s="39" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H2" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
@@ -3828,29 +3831,37 @@
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>Domain Abbreviation</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D3" s="9" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E3" s="9" t="inlineStr">
         <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F3" s="5" t="n"/>
-      <c r="G3" s="38" t="n"/>
+          <t>AGEMIN</t>
+        </is>
+      </c>
+      <c r="F3" s="5" t="inlineStr">
+        <is>
+          <t>Planned Minimum Age of Subjects</t>
+        </is>
+      </c>
+      <c r="G3" s="33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">18 ["Year","Year"] </t>
+        </is>
+      </c>
       <c r="H3" s="9" t="inlineStr">
         <is>
-          <t>"TS"</t>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -3862,27 +3873,39 @@
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>Sequence Number</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>Num</t>
+          <t> </t>
         </is>
       </c>
       <c r="D4" s="9" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E4" s="9" t="inlineStr">
         <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F4" s="12" t="n"/>
-      <c r="G4" s="38" t="n"/>
-      <c r="H4" s="39" t="n"/>
+          <t>AGEMAX</t>
+        </is>
+      </c>
+      <c r="F4" s="12" t="inlineStr">
+        <is>
+          <t>Planned Minimum Age of Subjects</t>
+        </is>
+      </c>
+      <c r="G4" s="33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">100 ["Year","Year"] </t>
+        </is>
+      </c>
+      <c r="H4" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="9" t="inlineStr">
@@ -3892,27 +3915,39 @@
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>Group ID</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C5" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t>Identifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E5" s="9" t="inlineStr">
         <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="F5" s="12" t="n"/>
-      <c r="G5" s="38" t="n"/>
-      <c r="H5" s="39" t="n"/>
+          <t>BRDNAIND</t>
+        </is>
+      </c>
+      <c r="F5" s="12" t="inlineStr">
+        <is>
+          <t>Biospecimen Retention contains DNA Ind</t>
+        </is>
+      </c>
+      <c r="G5" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H5" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="43.5" customHeight="1">
       <c r="A6" s="9" t="inlineStr">
@@ -3922,27 +3957,39 @@
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>Trial Summary Parameter Short Name</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C6" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D6" s="9" t="inlineStr">
         <is>
-          <t>Topic</t>
+          <t> </t>
         </is>
       </c>
       <c r="E6" s="9" t="inlineStr">
         <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F6" s="12" t="n"/>
-      <c r="G6" s="38" t="n"/>
-      <c r="H6" s="39" t="n"/>
+          <t>BRIND</t>
+        </is>
+      </c>
+      <c r="F6" s="12" t="inlineStr">
+        <is>
+          <t>Biospecimen Retention indicator</t>
+        </is>
+      </c>
+      <c r="G6" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H6" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="29" customHeight="1">
       <c r="A7" s="9" t="inlineStr">
@@ -3952,27 +3999,39 @@
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>Trial Summary Parameter</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C7" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D7" s="9" t="inlineStr">
         <is>
-          <t>Synonym Qualifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E7" s="9" t="inlineStr">
         <is>
-          <t>Req</t>
-        </is>
-      </c>
-      <c r="F7" s="12" t="n"/>
-      <c r="G7" s="38" t="n"/>
-      <c r="H7" s="39" t="n"/>
+          <t>COMPTRT</t>
+        </is>
+      </c>
+      <c r="F7" s="12" t="inlineStr">
+        <is>
+          <t>Comparative Treatment Name</t>
+        </is>
+      </c>
+      <c r="G7" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H7" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="inlineStr">
@@ -3982,27 +4041,39 @@
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>Parameter Value</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D8" s="9" t="inlineStr">
         <is>
-          <t>Result Qualifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E8" s="9" t="inlineStr">
         <is>
-          <t>Exp</t>
-        </is>
-      </c>
-      <c r="F8" s="12" t="n"/>
-      <c r="G8" s="38" t="n"/>
-      <c r="H8" s="39" t="n"/>
+          <t>CONNAME</t>
+        </is>
+      </c>
+      <c r="F8" s="12" t="inlineStr">
+        <is>
+          <t>Contact Name</t>
+        </is>
+      </c>
+      <c r="G8" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H8" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="29" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
@@ -4012,27 +4083,39 @@
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>Parameter Value Null Flavor</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C9" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D9" s="9" t="inlineStr">
         <is>
-          <t>Result Qualifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E9" s="9" t="inlineStr">
         <is>
-          <t>Perm</t>
-        </is>
-      </c>
-      <c r="F9" s="12" t="n"/>
-      <c r="G9" s="38" t="n"/>
-      <c r="H9" s="39" t="n"/>
+          <t>CONROLE</t>
+        </is>
+      </c>
+      <c r="F9" s="12" t="inlineStr">
+        <is>
+          <t>Contact Role</t>
+        </is>
+      </c>
+      <c r="G9" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H9" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="10" ht="29" customHeight="1">
       <c r="A10" s="9" t="inlineStr">
@@ -4042,27 +4125,39 @@
       </c>
       <c r="B10" s="9" t="inlineStr">
         <is>
-          <t>Parameter Value Code</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C10" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D10" s="9" t="inlineStr">
         <is>
-          <t>Result Qualifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E10" s="9" t="inlineStr">
         <is>
-          <t>Exp</t>
-        </is>
-      </c>
-      <c r="F10" s="12" t="n"/>
-      <c r="G10" s="38" t="n"/>
-      <c r="H10" s="39" t="n"/>
+          <t>CRMDUR</t>
+        </is>
+      </c>
+      <c r="F10" s="12" t="inlineStr">
+        <is>
+          <t>Confirmed Response Minimum Duration</t>
+        </is>
+      </c>
+      <c r="G10" s="33" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '1 Day'}</t>
+        </is>
+      </c>
+      <c r="H10" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="11" ht="29" customHeight="1">
       <c r="A11" s="9" t="inlineStr">
@@ -4072,35 +4167,39 @@
       </c>
       <c r="B11" s="9" t="inlineStr">
         <is>
-          <t>Name of Reference Terminology</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C11" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D11" s="9" t="inlineStr">
         <is>
-          <t>Result Qualifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E11" s="9" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>CURTRT</t>
         </is>
       </c>
       <c r="F11" s="12" t="inlineStr">
         <is>
-          <t>Name of Reference Terminology</t>
-        </is>
-      </c>
-      <c r="G11" s="38" t="inlineStr">
-        <is>
-          <t>..code.codeSystem</t>
-        </is>
-      </c>
-      <c r="H11" s="39" t="n"/>
+          <t>Current Therapy or Treatment</t>
+        </is>
+      </c>
+      <c r="G11" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H11" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="12" ht="43.5" customHeight="1">
       <c r="A12" s="9" t="inlineStr">
@@ -4110,35 +4209,1815 @@
       </c>
       <c r="B12" s="9" t="inlineStr">
         <is>
-          <t>Version of the Reference Terminology</t>
+          <t>"TS"</t>
         </is>
       </c>
       <c r="C12" s="9" t="inlineStr">
         <is>
-          <t>Char</t>
+          <t> </t>
         </is>
       </c>
       <c r="D12" s="9" t="inlineStr">
         <is>
-          <t>Result Qualifier</t>
+          <t> </t>
         </is>
       </c>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>Exp</t>
+          <t>DMCIND</t>
         </is>
       </c>
       <c r="F12" s="12" t="inlineStr">
         <is>
-          <t>Version of Reference Terminology</t>
-        </is>
-      </c>
-      <c r="G12" s="38" t="inlineStr">
-        <is>
-          <t>..code.codeSystemVersion</t>
-        </is>
-      </c>
-      <c r="H12" s="39" t="n"/>
+          <t>Data Monitoring Committee Indicator</t>
+        </is>
+      </c>
+      <c r="G12" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H12" s="34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>DOSE</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Dose Level; Dose per Administration</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 20}</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>DOSFRM</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Dose Form</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'TABLET'}</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>DOSFRQ</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Dosing Frequency</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'BID'}</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>DOSU</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Dose Units</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'Milligram'}</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>EXTTIND</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Extension Trial Indicator</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>FCNTRY</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Planned Country of Investigational Sites</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>HLTSUBJI</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Healthy Subject Indicator</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>HLTSUBJI</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Healthy Subject Indicator</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>INDIC</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Trial Disease/Condition Indication; Trial Disease/Condition Indication Description</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>["Parkinson's disease", "Parkinson's disease"]</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>INTMODEL</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Intervention Model</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>PARALLEL</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>INTTYPE</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Intervention Type</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'Pharmacologic Substance'}</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>LENGTH</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Trial Length</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>MSEUTIND</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Multiple Site EU Site Trial Indicator</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>NARMS</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Planned Number of Arms</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>NCOHORT</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Number of Groups/Cohorts</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>NUMSEUST</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Number of Trial Sites EU State</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>OBJEXP</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Trial Exploratory Objective</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>OBJPRIM</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Study Primary Objective; Trial Primary Objective</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>{'Objective_1': '•\tTo evaluate the effect of intravenous infusions of Beroclin administered once daily on motor symptoms in subjects with early stage Parkinson s disease.'}</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>OBJSEC</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Study Secondary Objective; Trial Secondary Objective</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>{'Objective_2': '•\tTo evaluate the safety and tolerability of intravenous infusions of Beroclin administered once daily in subjects with early stage Parkinson s disease.'}</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>OBSMODEL</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Observational Model</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>COHORT</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>OBSTIMP</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Observational Time Perspective</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>PROSPECTIVE</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>OBSTPOPD</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Obs Study Population Description</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>OBSTSMM</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Observational Study Sampling Method</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>OUTMSEXP</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Exploratory Outcome Measure</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>OUTMSPRI</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Primary Outcome Measure</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>OUTMSSEC</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Secondary Outcome Measure</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>PCLAS</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Pharmacologic Class</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>PIPIND</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Pediatric Investigation Plan Indicator</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>PLANSUB</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Anticipated Enrollment; Planned Enrollment; Planned Number of Subjects; Target Enrollment</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>PTRTDUR</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Planned Treatment Duration</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '14 Day'}</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>RANDOM</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Trial is Randomized</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>RDIND</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Rare Disease Indicator</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>REGID</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Registry Identifier</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>ROUTE</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Route of Administration</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>RTSPCDES</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Retained Biospecimen Description</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>SEXPOP</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Sex of Participants</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>SPONSOR</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Clinical Study Sponsor; Sponsor; Study Sponsor</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Error in expression for Clinical Study Sponsor; Sponsor; Study Sponsor: study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>SPREFID</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Sponsor's Study Reference ID</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>SSEUTIND</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Single Site EU State Trial Indicator</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>STYPE</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Study Type; Study Type Classification</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>TBLIND</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Study Blinding Design; Study Blinding Schema; Study Masking Design; Trial Blinding Design; Trial Blinding Schema; Trial Masking Design</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>Double Blind Study</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>TCNTRL</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Control Type</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>THERAREA</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Therapeutic Area</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>TINDTP</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>Trial Intent Type</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>Official Study Title; Study Title; Trial Title</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>A Phase II, Placebo-, Real-World Data Controlled study of Beroclin in subjects with early Parkinson disease</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>TPHASE</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Trial Phase; Trial Phase Classification</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>TRT</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Investigational Therapy or Treatment</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'LY900018'}</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>"TS"</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>TTYPE</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Trial Scope; Trial Type</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4153,8 +6032,8 @@
   </sheetPr>
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="10.81640625" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
update results and code
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -3784,7 +3784,7 @@
     <row r="2" ht="93" customHeight="1">
       <c r="A2" s="9" t="inlineStr">
         <is>
-          <t>STUDYID</t>
+          <t> </t>
         </is>
       </c>
       <c r="B2" s="9" t="inlineStr">
@@ -3826,7 +3826,7 @@
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>DOMAIN</t>
+          <t> </t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
@@ -3868,7 +3868,7 @@
     <row r="4">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>TSSEQ</t>
+          <t> </t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="5">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t>TSGRPID</t>
+          <t> </t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
@@ -3952,7 +3952,7 @@
     <row r="6" ht="43.5" customHeight="1">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t>TSPARMCD</t>
+          <t> </t>
         </is>
       </c>
       <c r="B6" s="9" t="inlineStr">
@@ -3994,7 +3994,7 @@
     <row r="7" ht="29" customHeight="1">
       <c r="A7" s="9" t="inlineStr">
         <is>
-          <t>TSPARM</t>
+          <t> </t>
         </is>
       </c>
       <c r="B7" s="9" t="inlineStr">
@@ -4036,7 +4036,7 @@
     <row r="8">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>TSVAL</t>
+          <t> </t>
         </is>
       </c>
       <c r="B8" s="9" t="inlineStr">
@@ -4078,7 +4078,7 @@
     <row r="9" ht="29" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>TSVALNF</t>
+          <t> </t>
         </is>
       </c>
       <c r="B9" s="9" t="inlineStr">
@@ -4120,7 +4120,7 @@
     <row r="10" ht="29" customHeight="1">
       <c r="A10" s="9" t="inlineStr">
         <is>
-          <t>TSVALCD</t>
+          <t> </t>
         </is>
       </c>
       <c r="B10" s="9" t="inlineStr">
@@ -4162,7 +4162,7 @@
     <row r="11" ht="29" customHeight="1">
       <c r="A11" s="9" t="inlineStr">
         <is>
-          <t>TSVCDREF</t>
+          <t> </t>
         </is>
       </c>
       <c r="B11" s="9" t="inlineStr">
@@ -4204,7 +4204,7 @@
     <row r="12" ht="43.5" customHeight="1">
       <c r="A12" s="9" t="inlineStr">
         <is>
-          <t>TSVCDVER</t>
+          <t> </t>
         </is>
       </c>
       <c r="B12" s="9" t="inlineStr">
@@ -4244,6 +4244,11 @@
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4281,6 +4286,11 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4318,6 +4328,11 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4355,6 +4370,11 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4392,6 +4412,11 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4429,6 +4454,11 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4466,6 +4496,11 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4503,6 +4538,11 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4540,6 +4580,11 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4577,6 +4622,11 @@
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4614,6 +4664,11 @@
       </c>
     </row>
     <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4651,6 +4706,11 @@
       </c>
     </row>
     <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4688,6 +4748,11 @@
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4725,6 +4790,11 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4762,6 +4832,11 @@
       </c>
     </row>
     <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4799,6 +4874,11 @@
       </c>
     </row>
     <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4836,6 +4916,11 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4873,6 +4958,11 @@
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4910,6 +5000,11 @@
       </c>
     </row>
     <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4947,6 +5042,11 @@
       </c>
     </row>
     <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -4984,6 +5084,11 @@
       </c>
     </row>
     <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5021,6 +5126,11 @@
       </c>
     </row>
     <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B34" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5058,6 +5168,11 @@
       </c>
     </row>
     <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B35" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5095,6 +5210,11 @@
       </c>
     </row>
     <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B36" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5132,6 +5252,11 @@
       </c>
     </row>
     <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B37" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5169,6 +5294,11 @@
       </c>
     </row>
     <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B38" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5206,6 +5336,11 @@
       </c>
     </row>
     <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B39" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5243,6 +5378,11 @@
       </c>
     </row>
     <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B40" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5280,6 +5420,11 @@
       </c>
     </row>
     <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5317,6 +5462,11 @@
       </c>
     </row>
     <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B42" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5354,6 +5504,11 @@
       </c>
     </row>
     <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B43" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5391,6 +5546,11 @@
       </c>
     </row>
     <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B44" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5428,6 +5588,11 @@
       </c>
     </row>
     <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B45" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5465,6 +5630,11 @@
       </c>
     </row>
     <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B46" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5502,6 +5672,11 @@
       </c>
     </row>
     <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B47" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5539,6 +5714,11 @@
       </c>
     </row>
     <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B48" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5576,6 +5756,11 @@
       </c>
     </row>
     <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B49" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5613,6 +5798,11 @@
       </c>
     </row>
     <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B50" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5650,6 +5840,11 @@
       </c>
     </row>
     <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B51" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5687,6 +5882,11 @@
       </c>
     </row>
     <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B52" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5724,6 +5924,11 @@
       </c>
     </row>
     <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B53" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5761,6 +5966,11 @@
       </c>
     </row>
     <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B54" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5798,6 +6008,11 @@
       </c>
     </row>
     <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B55" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5835,6 +6050,11 @@
       </c>
     </row>
     <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B56" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5872,6 +6092,11 @@
       </c>
     </row>
     <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5909,6 +6134,11 @@
       </c>
     </row>
     <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B58" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5946,6 +6176,11 @@
       </c>
     </row>
     <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B59" t="inlineStr">
         <is>
           <t>"TS"</t>
@@ -5983,6 +6218,11 @@
       </c>
     </row>
     <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="B60" t="inlineStr">
         <is>
           <t>"TS"</t>

</xml_diff>

<commit_message>
Updated code with StudyId
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -3706,7 +3706,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -3784,7 +3784,7 @@
     <row r="2" ht="93" customHeight="1">
       <c r="A2" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B2" s="9" t="inlineStr">
@@ -3826,7 +3826,7 @@
     <row r="3">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
@@ -3868,7 +3868,7 @@
     <row r="4">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
@@ -3910,7 +3910,7 @@
     <row r="5">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
@@ -3930,17 +3930,17 @@
       </c>
       <c r="E5" s="9" t="inlineStr">
         <is>
-          <t>BRDNAIND</t>
+          <t>CRMDUR</t>
         </is>
       </c>
       <c r="F5" s="12" t="inlineStr">
         <is>
-          <t>Biospecimen Retention contains DNA Ind</t>
+          <t>Confirmed Response Minimum Duration</t>
         </is>
       </c>
       <c r="G5" s="33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': '1 Day'}</t>
         </is>
       </c>
       <c r="H5" s="34" t="inlineStr">
@@ -3952,7 +3952,7 @@
     <row r="6" ht="43.5" customHeight="1">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B6" s="9" t="inlineStr">
@@ -3972,17 +3972,17 @@
       </c>
       <c r="E6" s="9" t="inlineStr">
         <is>
-          <t>BRIND</t>
+          <t>DOSE</t>
         </is>
       </c>
       <c r="F6" s="12" t="inlineStr">
         <is>
-          <t>Biospecimen Retention indicator</t>
+          <t>Dose Level; Dose per Administration</t>
         </is>
       </c>
       <c r="G6" s="33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': 20}</t>
         </is>
       </c>
       <c r="H6" s="34" t="inlineStr">
@@ -3994,7 +3994,7 @@
     <row r="7" ht="29" customHeight="1">
       <c r="A7" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B7" s="9" t="inlineStr">
@@ -4014,17 +4014,17 @@
       </c>
       <c r="E7" s="9" t="inlineStr">
         <is>
-          <t>COMPTRT</t>
+          <t>DOSFRM</t>
         </is>
       </c>
       <c r="F7" s="12" t="inlineStr">
         <is>
-          <t>Comparative Treatment Name</t>
+          <t>Dose Form</t>
         </is>
       </c>
       <c r="G7" s="33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': 'TABLET'}</t>
         </is>
       </c>
       <c r="H7" s="34" t="inlineStr">
@@ -4036,7 +4036,7 @@
     <row r="8">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B8" s="9" t="inlineStr">
@@ -4056,17 +4056,17 @@
       </c>
       <c r="E8" s="9" t="inlineStr">
         <is>
-          <t>CONNAME</t>
+          <t>DOSFRQ</t>
         </is>
       </c>
       <c r="F8" s="12" t="inlineStr">
         <is>
-          <t>Contact Name</t>
+          <t>Dosing Frequency</t>
         </is>
       </c>
       <c r="G8" s="33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': 'BID'}</t>
         </is>
       </c>
       <c r="H8" s="34" t="inlineStr">
@@ -4078,7 +4078,7 @@
     <row r="9" ht="29" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B9" s="9" t="inlineStr">
@@ -4098,17 +4098,17 @@
       </c>
       <c r="E9" s="9" t="inlineStr">
         <is>
-          <t>CONROLE</t>
+          <t>DOSU</t>
         </is>
       </c>
       <c r="F9" s="12" t="inlineStr">
         <is>
-          <t>Contact Role</t>
+          <t>Dose Units</t>
         </is>
       </c>
       <c r="G9" s="33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': 'Milligram'}</t>
         </is>
       </c>
       <c r="H9" s="34" t="inlineStr">
@@ -4120,7 +4120,7 @@
     <row r="10" ht="29" customHeight="1">
       <c r="A10" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B10" s="9" t="inlineStr">
@@ -4140,17 +4140,17 @@
       </c>
       <c r="E10" s="9" t="inlineStr">
         <is>
-          <t>CRMDUR</t>
+          <t>INDIC</t>
         </is>
       </c>
       <c r="F10" s="12" t="inlineStr">
         <is>
-          <t>Confirmed Response Minimum Duration</t>
+          <t>Trial Disease/Condition Indication; Trial Disease/Condition Indication Description</t>
         </is>
       </c>
       <c r="G10" s="33" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': '1 Day'}</t>
+          <t>["Parkinson's disease", "Parkinson's disease"]</t>
         </is>
       </c>
       <c r="H10" s="34" t="inlineStr">
@@ -4162,7 +4162,7 @@
     <row r="11" ht="29" customHeight="1">
       <c r="A11" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B11" s="9" t="inlineStr">
@@ -4182,17 +4182,17 @@
       </c>
       <c r="E11" s="9" t="inlineStr">
         <is>
-          <t>CURTRT</t>
+          <t>INTMODEL</t>
         </is>
       </c>
       <c r="F11" s="12" t="inlineStr">
         <is>
-          <t>Current Therapy or Treatment</t>
+          <t>Intervention Model</t>
         </is>
       </c>
       <c r="G11" s="33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>PARALLEL</t>
         </is>
       </c>
       <c r="H11" s="34" t="inlineStr">
@@ -4204,7 +4204,7 @@
     <row r="12" ht="43.5" customHeight="1">
       <c r="A12" s="9" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B12" s="9" t="inlineStr">
@@ -4224,17 +4224,17 @@
       </c>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>DMCIND</t>
+          <t>INTTYPE</t>
         </is>
       </c>
       <c r="F12" s="12" t="inlineStr">
         <is>
-          <t>Data Monitoring Committee Indicator</t>
+          <t>Intervention Type</t>
         </is>
       </c>
       <c r="G12" s="33" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': 'Pharmacologic Substance'}</t>
         </is>
       </c>
       <c r="H12" s="34" t="inlineStr">
@@ -4246,7 +4246,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -4266,17 +4266,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>DOSE</t>
+          <t>NARMS</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Dose Level; Dose per Administration</t>
+          <t>Planned Number of Arms</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 20}</t>
+          <t>2</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -4288,7 +4288,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -4308,17 +4308,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>DOSFRM</t>
+          <t>OBJPRIM</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Dose Form</t>
+          <t>Study Primary Objective; Trial Primary Objective</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'TABLET'}</t>
+          <t>{'Objective_1': '•\tTo evaluate the effect of intravenous infusions of Beroclin administered once daily on motor symptoms in subjects with early stage Parkinson s disease.'}</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -4330,7 +4330,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -4350,17 +4350,17 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>DOSFRQ</t>
+          <t>OBJSEC</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Dosing Frequency</t>
+          <t>Study Secondary Objective; Trial Secondary Objective</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'BID'}</t>
+          <t>{'Objective_2': '•\tTo evaluate the safety and tolerability of intravenous infusions of Beroclin administered once daily in subjects with early stage Parkinson s disease.'}</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -4372,7 +4372,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -4392,17 +4392,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>DOSU</t>
+          <t>OBSMODEL</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Dose Units</t>
+          <t>Observational Model</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Milligram'}</t>
+          <t>COHORT</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -4414,7 +4414,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -4434,17 +4434,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>EXTTIND</t>
+          <t>OBSTIMP</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Extension Trial Indicator</t>
+          <t>Observational Time Perspective</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t> </t>
+          <t>PROSPECTIVE</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -4456,7 +4456,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -4476,17 +4476,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>FCNTRY</t>
+          <t>OUTMSPRI</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Planned Country of Investigational Sites</t>
+          <t>Primary Outcome Measure</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{}</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -4498,7 +4498,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -4518,17 +4518,17 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>HLTSUBJI</t>
+          <t>OUTMSSEC</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Healthy Subject Indicator</t>
+          <t>Secondary Outcome Measure</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{}</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -4540,7 +4540,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -4560,17 +4560,17 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>HLTSUBJI</t>
+          <t>PTRTDUR</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Healthy Subject Indicator</t>
+          <t>Planned Treatment Duration</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': '14 Day'}</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -4582,7 +4582,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -4602,17 +4602,17 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>INDIC</t>
+          <t>SPONSOR</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Trial Disease/Condition Indication; Trial Disease/Condition Indication Description</t>
+          <t>Clinical Study Sponsor; Sponsor; Study Sponsor</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>["Parkinson's disease", "Parkinson's disease"]</t>
+          <t>Error in expression for Clinical Study Sponsor; Sponsor; Study Sponsor: study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -4624,7 +4624,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -4644,17 +4644,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>INTMODEL</t>
+          <t>TBLIND</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Intervention Model</t>
+          <t>Study Blinding Design; Study Blinding Schema; Study Masking Design; Trial Blinding Design; Trial Blinding Schema; Trial Masking Design</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>PARALLEL</t>
+          <t>Double Blind Study</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -4666,7 +4666,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -4686,17 +4686,17 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>INTTYPE</t>
+          <t>TCNTRL</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Intervention Type</t>
+          <t>Control Type</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Pharmacologic Substance'}</t>
+          <t>{}</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -4708,7 +4708,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -4728,17 +4728,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>LENGTH</t>
+          <t>TITLE</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Trial Length</t>
+          <t>Official Study Title; Study Title; Trial Title</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t> </t>
+          <t>A Phase II, Placebo-, Real-World Data Controlled study of Beroclin in subjects with early Parkinson disease</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -4750,7 +4750,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>CB0321</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -4770,1490 +4770,20 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>MSEUTIND</t>
+          <t>TRT</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Multiple Site EU Site Trial Indicator</t>
+          <t>Investigational Therapy or Treatment</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': 'LY900018'}</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>NARMS</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Planned Number of Arms</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>NCOHORT</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Number of Groups/Cohorts</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>NUMSEUST</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Number of Trial Sites EU State</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>OBJEXP</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Trial Exploratory Objective</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>OBJPRIM</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t>Study Primary Objective; Trial Primary Objective</t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>{'Objective_1': '•\tTo evaluate the effect of intravenous infusions of Beroclin administered once daily on motor symptoms in subjects with early stage Parkinson s disease.'}</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>OBJSEC</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Study Secondary Objective; Trial Secondary Objective</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>{'Objective_2': '•\tTo evaluate the safety and tolerability of intravenous infusions of Beroclin administered once daily in subjects with early stage Parkinson s disease.'}</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>OBSMODEL</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Observational Model</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>COHORT</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>OBSTIMP</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>Observational Time Perspective</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>PROSPECTIVE</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>OBSTPOPD</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Obs Study Population Description</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>OBSTSMM</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Observational Study Sampling Method</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>OUTMSEXP</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Exploratory Outcome Measure</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>OUTMSPRI</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Primary Outcome Measure</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>OUTMSSEC</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Secondary Outcome Measure</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>PCLAS</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Pharmacologic Class</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>PIPIND</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Pediatric Investigation Plan Indicator</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>PLANSUB</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Anticipated Enrollment; Planned Enrollment; Planned Number of Subjects; Target Enrollment</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>PTRTDUR</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Planned Treatment Duration</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>{'StudyIntervention_1': '14 Day'}</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>RANDOM</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Trial is Randomized</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>RDIND</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>Rare Disease Indicator</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>REGID</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>Registry Identifier</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>ROUTE</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Route of Administration</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>RTSPCDES</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Retained Biospecimen Description</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>SEXPOP</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Sex of Participants</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>SPONSOR</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>Clinical Study Sponsor; Sponsor; Study Sponsor</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>Error in expression for Clinical Study Sponsor; Sponsor; Study Sponsor: study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>SPREFID</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Sponsor's Study Reference ID</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>SSEUTIND</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Single Site EU State Trial Indicator</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>STYPE</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>Study Type; Study Type Classification</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>TBLIND</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>Study Blinding Design; Study Blinding Schema; Study Masking Design; Trial Blinding Design; Trial Blinding Schema; Trial Masking Design</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>Double Blind Study</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>TCNTRL</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Control Type</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>{}</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>THERAREA</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Therapeutic Area</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>TINDTP</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>Trial Intent Type</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>TITLE</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Official Study Title; Study Title; Trial Title</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>A Phase II, Placebo-, Real-World Data Controlled study of Beroclin in subjects with early Parkinson disease</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>TPHASE</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Trial Phase; Trial Phase Classification</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>TRT</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Investigational Therapy or Treatment</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>{'StudyIntervention_1': 'LY900018'}</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>"TS"</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>TTYPE</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Trial Scope; Trial Type</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
         <is>
           <t> </t>
         </is>

</xml_diff>

<commit_message>
Added code columns to output
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -3820,13 +3820,31 @@
           <t>Adaptive Design</t>
         </is>
       </c>
-      <c r="G2" s="35" t="inlineStr"/>
+      <c r="G2" s="35" t="inlineStr">
+        <is>
+          <t>Error in expression for Adaptive Design: $exists(study.versions.studyDesigns.characteristics[code="C98704"]) ? "Y" : ""</t>
+        </is>
+      </c>
       <c r="H2" s="34" t="inlineStr">
         <is>
           <t> </t>
         </is>
       </c>
-      <c r="I2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="9" t="n"/>
@@ -3857,7 +3875,8 @@
       </c>
       <c r="G3" s="33" t="inlineStr">
         <is>
-          <t>18  ["Year","Year"]</t>
+          <t>Error in expression for Planned Minimum Age of Subjects: $min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
+study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode</t>
         </is>
       </c>
       <c r="H3" s="9" t="inlineStr">
@@ -3867,7 +3886,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>18  ["Year","Year"]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -3900,7 +3929,8 @@
       </c>
       <c r="G4" s="33" t="inlineStr">
         <is>
-          <t>70  ["Year","Year"]</t>
+          <t>Error in expression for Planned Minimum Age of Subjects: $max([study.versions.studyDesigns.population.plannedAge.maxValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.value]) &amp; " " &amp; 
+study.versions.studyDesigns.population.plannedAge.maxValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.unit.standardCode.decode</t>
         </is>
       </c>
       <c r="H4" s="34" t="inlineStr">
@@ -3910,7 +3940,17 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>70  ["Year","Year"]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -3933,17 +3973,17 @@
       </c>
       <c r="E5" s="9" t="inlineStr">
         <is>
-          <t>CRMDUR</t>
+          <t>BRDNAIND</t>
         </is>
       </c>
       <c r="F5" s="12" t="inlineStr">
         <is>
-          <t>Confirmed Response Minimum Duration</t>
+          <t>Biospecimen Retention contains DNA Ind</t>
         </is>
       </c>
       <c r="G5" s="33" t="inlineStr">
         <is>
-          <t>[{'StudyIntervention_1': '1 Day'}, {'StudyIntervention_2': '1 Day'}]</t>
+          <t>Error in expression for Biospecimen Retention contains DNA Ind: study.versions.studyDesigns.biospecimenRetentions.includesDNA</t>
         </is>
       </c>
       <c r="H5" s="34" t="inlineStr">
@@ -3953,7 +3993,17 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>[{'StudyIntervention_1': '1 Day'}, {'StudyIntervention_2': '1 Day'}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -3976,17 +4026,17 @@
       </c>
       <c r="E6" s="9" t="inlineStr">
         <is>
-          <t>DOSE</t>
+          <t>BRIND</t>
         </is>
       </c>
       <c r="F6" s="12" t="inlineStr">
         <is>
-          <t>Dose Level; Dose per Administration</t>
+          <t>Biospecimen Retention indicator</t>
         </is>
       </c>
       <c r="G6" s="33" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 3.0, 'StudyIntervention_2': 1.0}</t>
+          <t>Error in expression for Biospecimen Retention indicator: study.versions.studyDesigns.biospecimenRetentions.isRetained</t>
         </is>
       </c>
       <c r="H6" s="34" t="inlineStr">
@@ -3996,7 +4046,17 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 3.0, 'StudyIntervention_2': 1.0}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4019,17 +4079,17 @@
       </c>
       <c r="E7" s="9" t="inlineStr">
         <is>
-          <t>DOSFRM</t>
+          <t>COMPTRT</t>
         </is>
       </c>
       <c r="F7" s="12" t="inlineStr">
         <is>
-          <t>Dose Form</t>
+          <t>Comparative Treatment Name</t>
         </is>
       </c>
       <c r="G7" s="33" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>Error in expression for Comparative Treatment Name: study.versions.studyInterventions[role.code="C68609"].{id: label}</t>
         </is>
       </c>
       <c r="H7" s="34" t="inlineStr">
@@ -4039,7 +4099,17 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4062,17 +4132,17 @@
       </c>
       <c r="E8" s="9" t="inlineStr">
         <is>
-          <t>DOSFRQ</t>
+          <t>CRMDUR</t>
         </is>
       </c>
       <c r="F8" s="12" t="inlineStr">
         <is>
-          <t>Dosing Frequency</t>
+          <t>Confirmed Response Minimum Duration</t>
         </is>
       </c>
       <c r="G8" s="33" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Once', 'StudyIntervention_2': 'Once'}</t>
+          <t>Error in expression for Confirmed Response Minimum Duration: study.versions.studyInterventions.{id: minimumResponseDuration.value &amp; " " &amp; minimumResponseDuration.unit.standardCode.decode}</t>
         </is>
       </c>
       <c r="H8" s="34" t="inlineStr">
@@ -4082,7 +4152,17 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Once', 'StudyIntervention_2': 'Once'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4105,17 +4185,17 @@
       </c>
       <c r="E9" s="9" t="inlineStr">
         <is>
-          <t>DOSU</t>
+          <t>CURTRT</t>
         </is>
       </c>
       <c r="F9" s="12" t="inlineStr">
         <is>
-          <t>Dose Units</t>
+          <t>Current Therapy or Treatment</t>
         </is>
       </c>
       <c r="G9" s="33" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Milligram', 'StudyIntervention_2': 'Milligram'}</t>
+          <t>Error in expression for Current Therapy or Treatment: study.versions.studyInterventions[role.code="C165822"].{id: label}</t>
         </is>
       </c>
       <c r="H9" s="34" t="inlineStr">
@@ -4125,7 +4205,17 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Milligram', 'StudyIntervention_2': 'Milligram'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4148,17 +4238,17 @@
       </c>
       <c r="E10" s="9" t="inlineStr">
         <is>
-          <t>INDIC</t>
+          <t>DOSE</t>
         </is>
       </c>
       <c r="F10" s="12" t="inlineStr">
         <is>
-          <t>Trial Disease/Condition Indication; Trial Disease/Condition Indication Description</t>
+          <t>Dose Level; Dose per Administration</t>
         </is>
       </c>
       <c r="G10" s="33" t="inlineStr">
         <is>
-          <t>['T1DM', 'T2DM']</t>
+          <t>Error in expression for Dose Level; Dose per Administration: study.versions.studyInterventions{id: administrations.dose.value}</t>
         </is>
       </c>
       <c r="H10" s="34" t="inlineStr">
@@ -4168,7 +4258,17 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>['T1DM', 'T2DM']</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4191,17 +4291,17 @@
       </c>
       <c r="E11" s="9" t="inlineStr">
         <is>
-          <t>INTMODEL</t>
+          <t>DOSFRM</t>
         </is>
       </c>
       <c r="F11" s="12" t="inlineStr">
         <is>
-          <t>Intervention Model</t>
+          <t>Dose Form</t>
         </is>
       </c>
       <c r="G11" s="33" t="inlineStr">
         <is>
-          <t>Parallel Study</t>
+          <t>Error in expression for Dose Form: study.versions.studyInterventions{id: administrations.administrableProduct.administrableDoseForm.standardCode.decode}</t>
         </is>
       </c>
       <c r="H11" s="34" t="inlineStr">
@@ -4211,7 +4311,17 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Parallel Study</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4234,27 +4344,37 @@
       </c>
       <c r="E12" s="9" t="inlineStr">
         <is>
-          <t>INTTYPE</t>
+          <t>DOSFRQ</t>
         </is>
       </c>
       <c r="F12" s="12" t="inlineStr">
         <is>
-          <t>Intervention Type</t>
+          <t>Dosing Frequency</t>
         </is>
       </c>
       <c r="G12" s="33" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Pharmacologic Substance', 'StudyIntervention_2': 'Pharmacologic Substance'}</t>
+          <t>{'StudyIntervention_1': 'Once', 'StudyIntervention_2': 'Once'}</t>
         </is>
       </c>
       <c r="H12" s="34" t="inlineStr">
         <is>
-          <t>NI</t>
+          <t> </t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Pharmacologic Substance', 'StudyIntervention_2': 'Pharmacologic Substance'}</t>
+          <t>{'StudyIntervention_1': 'C64576', 'StudyIntervention_2': 'C64576'}</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
         </is>
       </c>
     </row>
@@ -4276,17 +4396,17 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>LENGTH</t>
+          <t>DOSU</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Trial Length</t>
+          <t>Dose Units</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': 'Milligram', 'StudyIntervention_2': 'Milligram'}</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -4296,7 +4416,17 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t> </t>
+          <t>{'StudyIntervention_1': 'C28253', 'StudyIntervention_2': 'C28253'}</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
         </is>
       </c>
     </row>
@@ -4318,17 +4448,17 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>NARMS</t>
+          <t>INDIC</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Planned Number of Arms</t>
+          <t>Trial Disease/Condition Indication; Trial Disease/Condition Indication Description</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Error in expression for Trial Disease/Condition Indication; Trial Disease/Condition Indication Description: study.versions.studyDesigns.indications.label</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -4338,7 +4468,17 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4360,17 +4500,17 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>NCOHORT</t>
+          <t>INTMODEL</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Number of Groups/Cohorts</t>
+          <t>Intervention Model</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Parallel Study</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -4380,7 +4520,17 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>C82639</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>http://www.cdisc.org</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>2024-09-27</t>
         </is>
       </c>
     </row>
@@ -4402,17 +4552,17 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>OBJEXP</t>
+          <t>INTTYPE</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Trial Exploratory Objective</t>
+          <t>Intervention Type</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>[{'Objective_5': 'Explore the formation of anti-glucagon antibodies to glucagon'}, {'Objective_6': 'To evaluate the recovery from clinical symptoms of hypoglycemia'}]</t>
+          <t>{'StudyIntervention_1': 'Pharmacologic Substance', 'StudyIntervention_2': 'Pharmacologic Substance'}</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
@@ -4422,7 +4572,17 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>[{'Objective_5': 'Explore the formation of anti-glucagon antibodies to glucagon'}, {'Objective_6': 'To evaluate the recovery from clinical symptoms of hypoglycemia'}]</t>
+          <t>{'StudyIntervention_1': 'C1909', 'StudyIntervention_2': 'C1909'}</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
         </is>
       </c>
     </row>
@@ -4444,17 +4604,17 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>OBJPRIM</t>
+          <t>LENGTH</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Study Primary Objective; Trial Primary Objective</t>
+          <t>Trial Length</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>{'Objective_1': 'To demonstrate that 3 mg LY900018 is non-inferior to 1 mg IMG for the proportion of patients achieving treatment success from insulin-induced hypoglycemia using a non-inferiority margin of 10%'}</t>
+          <t>Error in expression for Trial Length: study.versions.studyDesigns.scheduleTimelines[mainTimeline=true].plannedDuration.quantity.value &amp; " " &amp; study.versions.studyDesigns.scheduleTimelines[mainTimeline=true].plannedDuration.quantity.unit.standardCode.decode</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -4464,7 +4624,17 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>{'Objective_1': 'To demonstrate that 3 mg LY900018 is non-inferior to 1 mg IMG for the proportion of patients achieving treatment success from insulin-induced hypoglycemia using a non-inferiority margin of 10%'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4486,17 +4656,17 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>OBJSEC</t>
+          <t>NARMS</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Study Secondary Objective; Trial Secondary Objective</t>
+          <t>Planned Number of Arms</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[{'Objective_2': 'To compare the safety and tolerability of 3 mg LY900018 with 1 mg IMG'}, {'Objective_3': 'To characterize the PK profile of 3 mg LY900018\ncompared to 1 mg IMG'}, {'Objective_4': 'To characterize the PD profile of 3 mg LY900018\ncompared to 1 mg IMG'}]</t>
+          <t>Error in expression for Planned Number of Arms: $count(study.versions.studyDesigns.arms)</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -4506,7 +4676,17 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>[{'Objective_2': 'To compare the safety and tolerability of 3 mg LY900018 with 1 mg IMG'}, {'Objective_3': 'To characterize the PK profile of 3 mg LY900018\ncompared to 1 mg IMG'}, {'Objective_4': 'To characterize the PD profile of 3 mg LY900018\ncompared to 1 mg IMG'}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4528,17 +4708,17 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>OUTMSEXP</t>
+          <t>NCOHORT</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Exploratory Outcome Measure</t>
+          <t>Number of Groups/Cohorts</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[{}, {}]</t>
+          <t>Error in expression for Number of Groups/Cohorts: $exists(study.versions.studyDesigns.population.cohorts) ? $count(study.versions.studyDesigns.population.cohorts) : ""</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -4548,7 +4728,17 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>[{}, {}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4570,17 +4760,17 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>OUTMSPRI</t>
+          <t>OBJEXP</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Primary Outcome Measure</t>
+          <t>Trial Exploratory Objective</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>Error in expression for Trial Exploratory Objective: study.versions.studyDesigns.objectives[level.code="C163559"].{id: text}</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -4590,7 +4780,17 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4612,17 +4812,17 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>OUTMSSEC</t>
+          <t>OBJPRIM</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Secondary Outcome Measure</t>
+          <t>Study Primary Objective; Trial Primary Objective</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[{}, {}, {}]</t>
+          <t>Error in expression for Study Primary Objective; Trial Primary Objective: study.versions.studyDesigns.objectives[level.code="C85826"].{id: text}</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -4632,7 +4832,17 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>[{}, {}, {}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4654,17 +4864,17 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>PLANSUB</t>
+          <t>OBJSEC</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Anticipated Enrollment; Planned Enrollment; Planned Number of Subjects; Target Enrollment</t>
+          <t>Study Secondary Objective; Trial Secondary Objective</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>75.0</t>
+          <t>Error in expression for Study Secondary Objective; Trial Secondary Objective: study.versions.studyDesigns.objectives[level.code="C85827"].{id: text}</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
@@ -4674,7 +4884,17 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>75.0</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4696,17 +4916,17 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>PTRTDUR</t>
+          <t>OBSTPOPD</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Planned Treatment Duration</t>
+          <t>Obs Study Population Description</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': '1 Day', 'StudyIntervention_2': '1 Day'}</t>
+          <t>Error in expression for Obs Study Population Description: study.versions.studyDesigns[studyType.code="C16084"].populations.description</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -4716,7 +4936,17 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': '1 Day', 'StudyIntervention_2': '1 Day'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4738,17 +4968,17 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ROUTE</t>
+          <t>OUTMSEXP</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Route of Administration</t>
+          <t>Exploratory Outcome Measure</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t>Error in expression for Exploratory Outcome Measure: study.versions.studyDesigns.objectives[level.code="C163559"].{id: objectives.endpoint.text}</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -4758,7 +4988,17 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4780,17 +5020,17 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>SPONSOR</t>
+          <t>OUTMSPRI</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Clinical Study Sponsor; Sponsor; Study Sponsor</t>
+          <t>Primary Outcome Measure</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Error in expression for Clinical Study Sponsor; Sponsor; Study Sponsor: study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
+          <t>Error in expression for Primary Outcome Measure: study.versions.studyDesigns.objectives[level.code="C85826"].{id: objectives.endpoint.text}</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -4800,7 +5040,17 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4822,17 +5072,17 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>TBLIND</t>
+          <t>OUTMSSEC</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Study Blinding Design; Study Blinding Schema; Study Masking Design; Trial Blinding Design; Trial Blinding Schema; Trial Masking Design</t>
+          <t>Secondary Outcome Measure</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Open Label Study</t>
+          <t>Error in expression for Secondary Outcome Measure: study.versions.studyDesigns.objectives[level.code="C85827"].{id: objectives.endpoint.text}</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -4842,7 +5092,17 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Open Label Study</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4864,27 +5124,37 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>TCNTRL</t>
+          <t>PLANSUB</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Control Type</t>
+          <t>Anticipated Enrollment; Planned Enrollment; Planned Number of Subjects; Target Enrollment</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t xml:space="preserve">Error in expression for Anticipated Enrollment; Planned Enrollment; Planned Number of Subjects; Target Enrollment: study.versions.studyDesigns.population.plannedEnrollmentNumber.value </t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>NI</t>
+          <t> </t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -4906,25 +5176,35 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>TPHASE</t>
+          <t>PTRTDUR</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Trial Phase; Trial Phase Classification</t>
+          <t>Planned Treatment Duration</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Error in expression for Planned Treatment Duration: study.versions.studyInterventions{id: administrations.duration.quantity.value &amp; " " &amp; administrations.duration.quantity.unit.standardCode.decode}</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>NI</t>
+          <t> </t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -4948,67 +5228,347 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
+          <t>ROUTE</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Route of Administration</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'C38284', 'StudyIntervention_2': 'C28161'}</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>SPONSOR</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Clinical Study Sponsor; Sponsor; Study Sponsor</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Error in expression for Clinical Study Sponsor; Sponsor; Study Sponsor: study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0];</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>TBLIND</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Study Blinding Design; Study Blinding Schema; Study Masking Design; Trial Blinding Design; Trial Blinding Schema; Trial Masking Design</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Open Label Study</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>C49659</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>http://www.cdisc.org</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>2024-09-27</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>TCNTRL</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Control Type</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>TITLE</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Official Study Title; Study Title; Trial Title</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Error in expression for Official Study Title; Study Title; Trial Title: study.versions.titles[type.code="C207616"].text</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>NI</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>TPHASE</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Trial Phase; Trial Phase Classification</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>NI</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>TS</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
           <t>TRT</t>
         </is>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>Investigational Therapy or Treatment</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>[{'StudyIntervention_1': 'LY900018'}, {'StudyIntervention_2': 'GlucaGen'}]</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>[{'StudyIntervention_1': 'LY900018'}, {'StudyIntervention_2': 'GlucaGen'}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>{'Objective_1': 'To demonstrate that 3 mg LY900018 is non-inferior to 1 mg IMG for the proportion of patients achieving treatment success from insulin-induced hypoglycemia using a non-inferiority margin of 10%'}</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>[{'Objective_2': 'To compare the safety and tolerability of 3 mg LY900018 with 1 mg IMG'}, {'Objective_3': 'To characterize the PK profile of 3 mg LY900018\ncompared to 1 mg IMG'}, {'Objective_4': 'To characterize the PD profile of 3 mg LY900018\ncompared to 1 mg IMG'}]</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="I32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="I33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="I34" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Error in expression for Investigational Therapy or Treatment: study.versions.studyInterventions[role.code="C41161"].{id: label}</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
       <c r="I35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t> </t>
         </is>
@@ -5017,126 +5577,306 @@
     <row r="36">
       <c r="I36" t="inlineStr">
         <is>
-          <t>[{}, {}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="I37" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="I38" t="inlineStr">
         <is>
-          <t>[{}, {}, {}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="I39" t="inlineStr">
         <is>
-          <t>[{}, {}, {}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="I40" t="inlineStr">
         <is>
-          <t>[{}, {}, {}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="I41" t="inlineStr">
         <is>
-          <t>75.0</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="I42" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': '1 Day', 'StudyIntervention_2': '1 Day'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="I43" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': '1 Day', 'StudyIntervention_2': '1 Day'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="I44" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': '1 Day', 'StudyIntervention_2': '1 Day'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="I45" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': '1 Day', 'StudyIntervention_2': '1 Day'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="I46" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t>{'StudyIntervention_1': 'C38284', 'StudyIntervention_2': 'C28161'}</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': 'http://www.cdisc.org', 'StudyIntervention_2': 'http://www.cdisc.org'}</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>{'StudyIntervention_1': '2024-09-27', 'StudyIntervention_2': '2024-09-27'}</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="I47" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="I48" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="I49" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="I50" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="I51" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="I52" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 'Nasal Route of Administration', 'StudyIntervention_2': 'Intramuscular Route of Administration'}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="I53" t="inlineStr">
         <is>
-          <t>Open Label Study</t>
+          <t>C49659</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>http://www.cdisc.org</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2024-09-27</t>
         </is>
       </c>
     </row>
@@ -5146,18 +5886,48 @@
           <t>{}</t>
         </is>
       </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>{}</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="I55" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="I56" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5167,6 +5937,16 @@
           <t> </t>
         </is>
       </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="I58" t="inlineStr">
@@ -5174,18 +5954,48 @@
           <t> </t>
         </is>
       </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="I59" t="inlineStr">
         <is>
-          <t>[{'StudyIntervention_1': 'LY900018'}, {'StudyIntervention_2': 'GlucaGen'}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="I60" t="inlineStr">
         <is>
-          <t>[{'StudyIntervention_1': 'LY900018'}, {'StudyIntervention_2': 'GlucaGen'}]</t>
+          <t> </t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>
@@ -5301,7 +6111,11 @@
           <t>Adaptive Design Indicator</t>
         </is>
       </c>
-      <c r="G2" s="31" t="inlineStr"/>
+      <c r="G2" s="31" t="inlineStr">
+        <is>
+          <t>Error in expression for Adaptive Design: $exists(study.versions.studyDesigns.characteristics[code="C98704"]) ? "Y" : ""</t>
+        </is>
+      </c>
       <c r="H2" t="inlineStr">
         <is>
           <t> </t>
@@ -5333,7 +6147,8 @@
       </c>
       <c r="G3" s="31" t="inlineStr">
         <is>
-          <t>18  ["Year","Year"]</t>
+          <t>Error in expression for Planned Minimum Age of Subjects: $min([study.versions.studyDesigns.population.plannedAge.minValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.minValue.value]) &amp; " " &amp; 
+study.versions.studyDesigns.population.plannedAge.minValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.minValue.unit.standardCode.decode</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -5367,7 +6182,8 @@
       </c>
       <c r="G4" s="29" t="inlineStr">
         <is>
-          <t>70  ["Year","Year"]</t>
+          <t>Error in expression for Planned Minimum Age of Subjects: $max([study.versions.studyDesigns.population.plannedAge.maxValue.value,study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.value]) &amp; " " &amp; 
+study.versions.studyDesigns.population.plannedAge.maxValue.unit.standardCode.decode &amp; " " &amp; study.versions.studyDesigns.population.cohorts.plannedAge.maxValue.unit.standardCode.decode</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -5409,7 +6225,7 @@
       </c>
       <c r="G5" s="29" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Error in expression for Biospecimen Retention contains DNA Ind: study.versions.studyDesigns.biospecimenRetentions.includesDNA</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -5451,7 +6267,7 @@
       </c>
       <c r="G6" s="29" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Error in expression for Biospecimen Retention indicator: study.versions.studyDesigns.biospecimenRetentions.isRetained</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -5489,7 +6305,7 @@
       <c r="F7" s="14" t="n"/>
       <c r="G7" s="29" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Error in expression for Comparative Treatment Name: study.versions.studyInterventions[role.code="C68609"].{id: label}</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -5615,7 +6431,7 @@
       </c>
       <c r="G10" s="29" t="inlineStr">
         <is>
-          <t>[{'StudyIntervention_1': '1 Day'}, {'StudyIntervention_2': '1 Day'}]</t>
+          <t>Error in expression for Confirmed Response Minimum Duration: study.versions.studyInterventions.{id: minimumResponseDuration.value &amp; " " &amp; minimumResponseDuration.unit.standardCode.decode}</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -5657,7 +6473,7 @@
       </c>
       <c r="G11" s="29" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Error in expression for Current Therapy or Treatment: study.versions.studyInterventions[role.code="C165822"].{id: label}</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -5733,7 +6549,7 @@
       </c>
       <c r="G13" s="29" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': 3.0, 'StudyIntervention_2': 1.0}</t>
+          <t>Error in expression for Dose Level; Dose per Administration: study.versions.studyInterventions{id: administrations.dose.value}</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -5775,7 +6591,7 @@
       </c>
       <c r="G14" s="29" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>Error in expression for Dose Form: study.versions.studyInterventions{id: administrations.administrableProduct.administrableDoseForm.standardCode.decode}</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -6063,7 +6879,7 @@
       </c>
       <c r="G21" s="29" t="inlineStr">
         <is>
-          <t>['T1DM', 'T2DM']</t>
+          <t>Error in expression for Trial Disease/Condition Indication; Trial Disease/Condition Indication Description: study.versions.studyDesigns.indications.label</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -6203,7 +7019,7 @@
       </c>
       <c r="G24" s="29" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Error in expression for Trial Length: study.versions.studyDesigns.scheduleTimelines[mainTimeline=true].plannedDuration.quantity.value &amp; " " &amp; study.versions.studyDesigns.scheduleTimelines[mainTimeline=true].plannedDuration.quantity.unit.standardCode.decode</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -6271,7 +7087,7 @@
       </c>
       <c r="G26" s="29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Error in expression for Planned Number of Arms: $count(study.versions.studyDesigns.arms)</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
@@ -6305,7 +7121,7 @@
       </c>
       <c r="G27" s="30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>Error in expression for Number of Groups/Cohorts: $exists(study.versions.studyDesigns.population.cohorts) ? $count(study.versions.studyDesigns.population.cohorts) : ""</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -6381,7 +7197,7 @@
       </c>
       <c r="G29" s="29" t="inlineStr">
         <is>
-          <t>[{'Objective_5': 'Explore the formation of anti-glucagon antibodies to glucagon'}, {'Objective_6': 'To evaluate the recovery from clinical symptoms of hypoglycemia'}]</t>
+          <t>Error in expression for Trial Exploratory Objective: study.versions.studyDesigns.objectives[level.code="C163559"].{id: text}</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -6423,7 +7239,7 @@
       </c>
       <c r="G30" s="29" t="inlineStr">
         <is>
-          <t>{'Objective_1': 'To demonstrate that 3 mg LY900018 is non-inferior to 1 mg IMG for the proportion of patients achieving treatment success from insulin-induced hypoglycemia using a non-inferiority margin of 10%'}</t>
+          <t>Error in expression for Study Primary Objective; Trial Primary Objective: study.versions.studyDesigns.objectives[level.code="C85826"].{id: text}</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -6465,7 +7281,7 @@
       </c>
       <c r="G31" s="29" t="inlineStr">
         <is>
-          <t>[{'Objective_2': 'To compare the safety and tolerability of 3 mg LY900018 with 1 mg IMG'}, {'Objective_3': 'To characterize the PK profile of 3 mg LY900018\ncompared to 1 mg IMG'}, {'Objective_4': 'To characterize the PD profile of 3 mg LY900018\ncompared to 1 mg IMG'}]</t>
+          <t>Error in expression for Study Secondary Objective; Trial Secondary Objective: study.versions.studyDesigns.objectives[level.code="C85827"].{id: text}</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -6597,7 +7413,7 @@
       </c>
       <c r="G34" s="30" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Error in expression for Obs Study Population Description: study.versions.studyDesigns[studyType.code="C16084"].populations.description</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
@@ -6688,7 +7504,7 @@
       </c>
       <c r="G36" s="29" t="inlineStr">
         <is>
-          <t>[{}, {}]</t>
+          <t>Error in expression for Exploratory Outcome Measure: study.versions.studyDesigns.objectives[level.code="C163559"].{id: objectives.endpoint.text}</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -6730,7 +7546,7 @@
       </c>
       <c r="G37" s="29" t="inlineStr">
         <is>
-          <t>{}</t>
+          <t>Error in expression for Primary Outcome Measure: study.versions.studyDesigns.objectives[level.code="C85826"].{id: objectives.endpoint.text}</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
@@ -6772,7 +7588,7 @@
       </c>
       <c r="G38" s="29" t="inlineStr">
         <is>
-          <t>[{}, {}, {}]</t>
+          <t>Error in expression for Secondary Outcome Measure: study.versions.studyDesigns.objectives[level.code="C85827"].{id: objectives.endpoint.text}</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -6878,7 +7694,7 @@
       </c>
       <c r="G41" s="29" t="inlineStr">
         <is>
-          <t>75.0</t>
+          <t xml:space="preserve">Error in expression for Anticipated Enrollment; Planned Enrollment; Planned Number of Subjects; Target Enrollment: study.versions.studyDesigns.population.plannedEnrollmentNumber.value </t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
@@ -6916,7 +7732,7 @@
       </c>
       <c r="G42" s="30" t="inlineStr">
         <is>
-          <t>{'StudyIntervention_1': '1 Day', 'StudyIntervention_2': '1 Day'}</t>
+          <t>Error in expression for Planned Treatment Duration: study.versions.studyInterventions{id: administrations.duration.quantity.value &amp; " " &amp; administrations.duration.quantity.unit.standardCode.decode}</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -7503,7 +8319,7 @@
       </c>
       <c r="G57" s="29" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Error in expression for Official Study Title; Study Title; Trial Title: study.versions.titles[type.code="C207616"].text</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
@@ -7594,7 +8410,7 @@
       </c>
       <c r="G59" s="29" t="inlineStr">
         <is>
-          <t>[{'StudyIntervention_1': 'LY900018'}, {'StudyIntervention_2': 'GlucaGen'}]</t>
+          <t>Error in expression for Investigational Therapy or Treatment: study.versions.studyInterventions[role.code="C41161"].{id: label}</t>
         </is>
       </c>
       <c r="H59" s="40" t="inlineStr">

</xml_diff>

<commit_message>
improved a bit / not ready
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -2803,12 +2803,12 @@
     <row r="2" ht="72.5" customHeight="1">
       <c r="A2" s="9" t="inlineStr">
         <is>
-          <t>STUDYID</t>
+          <t> </t>
         </is>
       </c>
       <c r="B2" s="9" t="inlineStr">
         <is>
-          <t>Study Identifier</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="C2" s="9" t="inlineStr">
@@ -2836,17 +2836,21 @@
           <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0]; studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
         </is>
       </c>
-      <c r="H2" s="33" t="n"/>
+      <c r="H2" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="29" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>DOMAIN</t>
+          <t> </t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
-          <t>Domain Abbreviation</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="C3" s="9" t="inlineStr">
@@ -2868,171 +2872,187 @@
       <c r="G3" s="38" t="n"/>
       <c r="H3" s="9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t> </t>
         </is>
       </c>
     </row>
     <row r="4" ht="29" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>IETESTCD</t>
+          <t> </t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_3': '3'</t>
+        </is>
+      </c>
+      <c r="D4" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> insulin aspar</t>
+        </is>
+      </c>
+      <c r="E4" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_3': 'Inclusion Criteria</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="inlineStr">
+        <is>
           <t>Incl/Excl Criterion Short Name</t>
         </is>
       </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_3': '3'</t>
-        </is>
-      </c>
-      <c r="D4" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> insulin aspar</t>
-        </is>
-      </c>
-      <c r="E4" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_3': 'Inclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F4" s="4" t="inlineStr">
-        <is>
-          <t>Incl/Excl Criterion Short Name</t>
-        </is>
-      </c>
       <c r="G4" s="39" t="inlineStr">
         <is>
           <t>study.versions.studyDesigns.eligibilityCriteria.{id: identifier}</t>
         </is>
       </c>
-      <c r="H4" s="33" t="n"/>
+      <c r="H4" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="5" ht="87" customHeight="1">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t>IETEST</t>
+          <t> </t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C5" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_4': '4'</t>
+        </is>
+      </c>
+      <c r="D5" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> or insulin glulisine</t>
+        </is>
+      </c>
+      <c r="E5" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_4': 'Inclusion Criteria</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="inlineStr">
+        <is>
           <t>Inclusion/Exclusion Criterion</t>
         </is>
       </c>
-      <c r="C5" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_4': '4'</t>
-        </is>
-      </c>
-      <c r="D5" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> or insulin glulisine</t>
-        </is>
-      </c>
-      <c r="E5" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_4': 'Inclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F5" s="4" t="inlineStr">
-        <is>
-          <t>Inclusion/Exclusion Criterion</t>
-        </is>
-      </c>
       <c r="G5" s="41" t="inlineStr">
         <is>
           <t>study.versions.($EligTxt := function($id) {(eligibilityCriterionItems[id=$id].text)}; studyDesigns.eligibilityCriteria{id: $EligTxt(criterionItemId)})</t>
         </is>
       </c>
-      <c r="H5" s="33" t="n"/>
+      <c r="H5" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="6" ht="43.5" customHeight="1">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t>IECAT</t>
+          <t> </t>
         </is>
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_5': '5'</t>
+        </is>
+      </c>
+      <c r="D6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> or&lt;/p&gt;\n      &lt;p&gt;[B] continuous subcutaneous insulin infusion (CSII)&lt;/p&gt;    \n    &lt;/ul&gt;\n  &lt;/li&gt;\n  &lt;p&gt;Or&lt;/p&gt;\n  &lt;li&gt;\n    &lt;p&gt;[1b] T2DM based on the WHO diagnostic criteri</t>
+        </is>
+      </c>
+      <c r="E6" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_5': 'Inclusion Criteria</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="inlineStr">
+        <is>
           <t>Inclusion/Exclusion Category</t>
         </is>
       </c>
-      <c r="C6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_5': '5'</t>
-        </is>
-      </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> or&lt;/p&gt;\n      &lt;p&gt;[B] continuous subcutaneous insulin infusion (CSII)&lt;/p&gt;    \n    &lt;/ul&gt;\n  &lt;/li&gt;\n  &lt;p&gt;Or&lt;/p&gt;\n  &lt;li&gt;\n    &lt;p&gt;[1b] T2DM based on the WHO diagnostic criteri</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_5': 'Inclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>Inclusion/Exclusion Category</t>
-        </is>
-      </c>
       <c r="G6" s="39" t="inlineStr">
         <is>
           <t>study.versions.studyDesigns.eligibilityCriteria{id: category.decode}</t>
         </is>
       </c>
-      <c r="H6" s="33" t="n"/>
+      <c r="H6" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="7" ht="43.5" customHeight="1">
       <c r="A7" s="9" t="inlineStr">
         <is>
-          <t>IESCAT</t>
+          <t> </t>
         </is>
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C7" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_6': '6'</t>
+        </is>
+      </c>
+      <c r="D7" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> and have received the&lt;/p&gt;\n    &lt;p&gt;following daily insulin therapy with or without oral anti-hyperglycemic medications (OAMs) for at least 1 year&lt;/p&gt;\n    &lt;ul&gt;\n      &lt;p&gt;[A] insulin: long-acting insulin analog (either insulin glargine [U-100 or U-300] or insulin degludec [U-100]) alon</t>
+        </is>
+      </c>
+      <c r="E7" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_6': 'Inclusion Criteria</t>
+        </is>
+      </c>
+      <c r="F7" s="4" t="inlineStr">
+        <is>
           <t>Inclusion/Exclusion Subcategory</t>
         </is>
       </c>
-      <c r="C7" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_6': '6'</t>
-        </is>
-      </c>
-      <c r="D7" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> and have received the&lt;/p&gt;\n    &lt;p&gt;following daily insulin therapy with or without oral anti-hyperglycemic medications (OAMs) for at least 1 year&lt;/p&gt;\n    &lt;ul&gt;\n      &lt;p&gt;[A] insulin: long-acting insulin analog (either insulin glargine [U-100 or U-300] or insulin degludec [U-100]) alon</t>
-        </is>
-      </c>
-      <c r="E7" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_6': 'Inclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>Inclusion/Exclusion Subcategory</t>
-        </is>
-      </c>
       <c r="G7" s="39" t="inlineStr">
         <is>
           <t>study.versions.studyDesigns.eligibilityCriteria{id: notes.codes.decode}</t>
         </is>
       </c>
-      <c r="H7" s="33" t="n"/>
+      <c r="H7" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="8" ht="29" customHeight="1">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>TIRL</t>
+          <t> </t>
         </is>
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>Inclusion/Exclusion Criterion Rule</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr">
@@ -3052,47 +3072,65 @@
       </c>
       <c r="F8" s="4" t="n"/>
       <c r="G8" s="38" t="n"/>
-      <c r="H8" s="33" t="n"/>
+      <c r="H8" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="9" ht="29" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>TIVERS</t>
+          <t> </t>
         </is>
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="C9" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_8': '8'</t>
+        </is>
+      </c>
+      <c r="D9" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> insulin aspar</t>
+        </is>
+      </c>
+      <c r="E9" s="9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 'EligibilityCriterion_8': 'Inclusion Criteria</t>
+        </is>
+      </c>
+      <c r="F9" s="4" t="inlineStr">
+        <is>
           <t>Protocol Criteria Versions</t>
         </is>
       </c>
-      <c r="C9" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_8': '8'</t>
-        </is>
-      </c>
-      <c r="D9" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> insulin aspar</t>
-        </is>
-      </c>
-      <c r="E9" s="9" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_8': 'Inclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F9" s="4" t="inlineStr">
-        <is>
-          <t>Protocol Criteria Versions</t>
-        </is>
-      </c>
       <c r="G9" s="38" t="inlineStr">
         <is>
           <t>study.versions.versionIdentifier</t>
         </is>
       </c>
-      <c r="H9" s="33" t="n"/>
+      <c r="H9" s="33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C10" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_9': '9'</t>
@@ -3108,8 +3146,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_9': 'Inclusion Criteria</t>
         </is>
       </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C11" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_10': '10'</t>
@@ -3125,8 +3178,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_10': 'Inclusion Criteria</t>
         </is>
       </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C12" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_11': '11'</t>
@@ -3142,8 +3210,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_11': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_12': '12'</t>
@@ -3159,8 +3242,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_12': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C14" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_13': '13'</t>
@@ -3176,8 +3274,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_13': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C15" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_14': '14'</t>
@@ -3193,8 +3306,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_14': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C16" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_15': '15'</t>
@@ -3210,8 +3338,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_15': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C17" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_16': '16'</t>
@@ -3227,8 +3370,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_16': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C18" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_17': '17'</t>
@@ -3244,8 +3402,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_17': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_18': '18'</t>
@@ -3261,8 +3434,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_18': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C20" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_19': '19'</t>
@@ -3278,8 +3466,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_19': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C21" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_20': '20'</t>
@@ -3295,8 +3498,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_20': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C22" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_21': '21'</t>
@@ -3312,8 +3530,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_21': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C23" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_22': '22'</t>
@@ -3329,8 +3562,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_22': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C24" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_23': '23'</t>
@@ -3346,8 +3594,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_23': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C25" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_24': '24'</t>
@@ -3363,8 +3626,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_24': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C26" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_25': '25'</t>
@@ -3380,8 +3658,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_25': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_26': '26'</t>
@@ -3397,8 +3690,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_26': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C28" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_27': '27'</t>
@@ -3414,8 +3722,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_27': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C29" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_28': '28'</t>
@@ -3431,8 +3754,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_28': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C30" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_29': '29'</t>
@@ -3448,8 +3786,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_29': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_30': '30'</t>
@@ -3465,8 +3818,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_30': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_31': '31'</t>
@@ -3482,8 +3850,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_31': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C33" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_32': '32'</t>
@@ -3499,8 +3882,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_32': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_33': '33'</t>
@@ -3516,8 +3914,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_33': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C35" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_34': '34'</t>
@@ -3533,8 +3946,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_34': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C36" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_35': '35'</t>
@@ -3550,8 +3978,23 @@
           <t xml:space="preserve"> 'EligibilityCriterion_35': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="C37" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_36': '36</t>
@@ -3567,515 +4010,1615 @@
           <t xml:space="preserve"> 'EligibilityCriterion_36': 'Exclusion Criteria</t>
         </is>
       </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D38" t="inlineStr">
         <is>
           <t>\n            or&lt;/li&gt;\n          &lt;li&gt;[iii] a woman at least 55 years of age with a diagnosis of menopause prior to starting hormone replacement\n            therapy&lt;/li&gt;\n        &lt;/ul&gt;\n      &lt;/li&gt;\n    &lt;/ul&gt;\n  &lt;/li&gt;\n&lt;/ul&gt;</t>
         </is>
       </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D39" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_4': '&lt;p&gt;are between 18 and 64 years old for T1D</t>
         </is>
       </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D40" t="inlineStr">
         <is>
           <t xml:space="preserve"> or between 20 and 70 years old for T2DM at the time of informed consent&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D41" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_5': '&lt;p&gt;have a body mass index of 18.5 to 30.0 kg/m 2 for T1D</t>
         </is>
       </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D42" t="inlineStr">
         <is>
           <t xml:space="preserve"> or 18.5 to 35.0 kg/m 2 for T2DM at the time of screening&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D43" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_6': '&lt;p&gt;have a hemoglobin A1c value ≤10% at the time of screening&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D44" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_7': '&lt;p&gt;have clinical laboratory test results within normal reference range (except for glycemic parameters) for the population or investigative sit</t>
         </is>
       </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D45" t="inlineStr">
         <is>
           <t xml:space="preserve"> or results with acceptable deviations that are judged to be not clinically significant by the investigator&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D46" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_8': '&lt;p&gt;have venous access sufficient to allow for blood sampling and administration of insulin for IV administration as per the protocol&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D47" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_9': '&lt;p&gt;are reliable and willing to make themselves available for the duration of the study and are willing to follow study procedures&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D48" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_10': '&lt;p&gt;are able and willing to give signed informed consent&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D49" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_11': '&lt;p&gt;are investigative site personnel directly affiliated with this study and their immediate families. Immediate family is defined as a spous</t>
         </is>
       </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D50" t="inlineStr">
         <is>
           <t xml:space="preserve"> biological or legal guardia</t>
         </is>
       </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D51" t="inlineStr">
         <is>
           <t xml:space="preserve"> chil</t>
         </is>
       </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D52" t="inlineStr">
         <is>
           <t xml:space="preserve"> or sibling&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D53" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_12': '&lt;p&gt;are Lilly employees&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D54" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_13': '&lt;p&gt;are currently enrolled in a clinical trial involving an investigational product or any other type of medical research judged not to be scientifically or medically compatible with this study&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D55" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_14': '&lt;p&gt;have participate</t>
         </is>
       </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D56" t="inlineStr">
         <is>
           <t xml:space="preserve"> within the last 4 month</t>
         </is>
       </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D57" t="inlineStr">
         <is>
           <t xml:space="preserve"> in a clinical trial involving an investigational product. If the previous investigational product has a long half-lif</t>
         </is>
       </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D58" t="inlineStr">
         <is>
           <t xml:space="preserve"> 4 months or 5 half-lives (whichever is longer) should have passed from the last dose of investigational product&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D59" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_15': '&lt;p&gt;have previously completed or withdrawn from this study or any other study investigating LY90001</t>
         </is>
       </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D60" t="inlineStr">
         <is>
           <t xml:space="preserve"> and have previously received LY900018&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D61" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_16': '&lt;p&gt;have known allergies or sensitivity to LY90001</t>
         </is>
       </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D62" t="inlineStr">
         <is>
           <t xml:space="preserve"> glucago</t>
         </is>
       </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D63" t="inlineStr">
         <is>
           <t xml:space="preserve"> related compound</t>
         </is>
       </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D64" t="inlineStr">
         <is>
           <t xml:space="preserve"> or any components of the formulatio</t>
         </is>
       </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D65" t="inlineStr">
         <is>
           <t xml:space="preserve"> or history of significant atopy&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D66" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_17': '&lt;p&gt;have an abnormality in the 12-lead ECG tha</t>
         </is>
       </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D67" t="inlineStr">
         <is>
           <t xml:space="preserve"> in the opinion of the investigato</t>
         </is>
       </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D68" t="inlineStr">
         <is>
           <t xml:space="preserve"> increases the risks associated with participating in the study&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D69" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_18': '&lt;p&gt;any significant changes in insulin regimen and/or unstable blood glucose control within the past 3 months prior to screening as assessed by the investigator&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D70" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_19': '&lt;p&gt;have received a total daily dose of insulin &amp;gt;1.2 U/kg at the time of screening&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D71" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_20': '&lt;p&gt;have poorly controlled hypertension (i</t>
         </is>
       </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D72" t="inlineStr">
         <is>
           <t xml:space="preserve"> supine systolic BP &amp;gt;165 mm Hg or supine diastolic BP &amp;gt;95 mm Hg) at screenin</t>
         </is>
       </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D73" t="inlineStr">
         <is>
           <t xml:space="preserve"> or a change in antihypertensive medications within 30 days prior to screening&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D74" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_21': '&lt;p&gt;have a history of pheochromocytoma (i</t>
         </is>
       </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D75" t="inlineStr">
         <is>
           <t xml:space="preserve"> adrenal gland tumor) or insulinoma&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D76" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_22': '&lt;p&gt;have a history of an episode of severe hypoglycemia (as defined by an episode that required third party assistance for treatment) in the 1 month prior to screening or have a history of loss of consciousness within the last 2 years induced other than by hypoglycemia&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D77" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_23': '&lt;p&gt;have a history of epilepsy or seizure disorder&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D78" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_24': '&lt;p&gt;have a history or presence of cardiovascula</t>
         </is>
       </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D79" t="inlineStr">
         <is>
           <t xml:space="preserve"> respirator</t>
         </is>
       </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D80" t="inlineStr">
         <is>
           <t xml:space="preserve"> hepati</t>
         </is>
       </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D81" t="inlineStr">
         <is>
           <t xml:space="preserve"> rena</t>
         </is>
       </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D82" t="inlineStr">
         <is>
           <t xml:space="preserve"> gastrointestina</t>
         </is>
       </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D83" t="inlineStr">
         <is>
           <t xml:space="preserve"> endocrine (apart from T1DM or T2DM</t>
         </is>
       </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D84" t="inlineStr">
         <is>
           <t xml:space="preserve"> hematologica</t>
         </is>
       </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D85" t="inlineStr">
         <is>
           <t xml:space="preserve"> or neurological disorders capable of significantly altering the absorptio</t>
         </is>
       </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D86" t="inlineStr">
         <is>
           <t xml:space="preserve"> metabolis</t>
         </is>
       </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D87" t="inlineStr">
         <is>
           <t xml:space="preserve"> or elimination of drugs; of constituting a risk when taking the investigational product; or of interfering with the interpretation of data&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D88" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_25': '&lt;p&gt;have known or ongoing psychiatric disorders tha</t>
         </is>
       </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D89" t="inlineStr">
         <is>
           <t xml:space="preserve"> in the opinion of the investigato</t>
         </is>
       </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D90" t="inlineStr">
         <is>
           <t xml:space="preserve"> may preclude the patient from following and completing the protocol&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D91" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_26': '&lt;p&gt;regularly use known drugs of abuse and/or show positive findings on urinary drug screening&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D92" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_27': '&lt;p&gt;show evidence of human immunodeficiency virus (HIV) infection and/or positive HIV antibodies and/or antigen&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D93" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_28': '&lt;p&gt;show evidence of hepatitis C and/or positive hepatitis C antibody&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D94" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_29': '&lt;p&gt;show evidence of hepatitis B and/or positive hepatitis B surface antigen&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D95" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_30': '&lt;p&gt;show evidence of syphilis and/or are positive for syphilis test&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D96" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_31': '&lt;p&gt;are women who are lactating&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D97" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_32': '&lt;p&gt;use of daily systemic beta-blocke</t>
         </is>
       </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D98" t="inlineStr">
         <is>
           <t xml:space="preserve"> indomethaci</t>
         </is>
       </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D99" t="inlineStr">
         <is>
           <t xml:space="preserve"> warfari</t>
         </is>
       </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D100" t="inlineStr">
         <is>
           <t xml:space="preserve"> anticholinergic drugs&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D101" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_33': '&lt;p&gt;have donated 400 mL or more blood in the last 12 weeks (males) or in the last 16 weeks (females</t>
         </is>
       </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D102" t="inlineStr">
         <is>
           <t xml:space="preserve"> or any blood donation (including apheresis) within the last 4 week</t>
         </is>
       </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D103" t="inlineStr">
         <is>
           <t xml:space="preserve"> or total volume of blood donation within 12 months is 1200 mL (males)/800 mL (females) or more at screening&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D104" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_34': '&lt;p&gt;have an average weekly alcohol intake that exceeds 21 units per week (males up to age 65) and 14 units per week (males over 65 and females</t>
         </is>
       </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D105" t="inlineStr">
         <is>
           <t xml:space="preserve"> or are unwilling to stop alcohol consumption from Day -2 to discharge from CRU in each period (1 unit = 12 oz or 360 mL of beer; 5 oz or 150 mL of wine; 1.5 oz or 45 mL of distilled spirits)&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D106" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_35': '&lt;p&gt;in the opinion of the investigator or sponso</t>
         </is>
       </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D107" t="inlineStr">
         <is>
           <t xml:space="preserve"> are unsuitable for inclusion in the study&lt;/p&gt;</t>
         </is>
       </c>
+      <c r="H107" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D108" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_36': '&lt;p&gt;have pre-proliferative and proliferative retinopathy or maculopathy requiring treatment or not clinically stable in the last 6 month</t>
         </is>
       </c>
+      <c r="H108" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D109" t="inlineStr">
         <is>
           <t xml:space="preserve"> or patients with active changes in subjective eye symptoms as determined by the investigator if an eye exam has not been performed in the last 6 months. Note: If an eye examination has been performed no more than 6 months before screenin</t>
         </is>
       </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
       <c r="D110" t="inlineStr">
         <is>
           <t xml:space="preserve"> it will not have to be repeated; howeve</t>
+        </is>
+      </c>
+      <c r="H110" t="inlineStr">
+        <is>
+          <t> </t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Correct split of criteria
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -2740,7 +2740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K128"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="C2" s="9" t="inlineStr">
         <is>
-          <t>'EligibilityCriterion_1': '01'</t>
+          <t>'EligibilityCriterion_1': '01</t>
         </is>
       </c>
       <c r="D2" s="9" t="inlineStr">
@@ -2855,7 +2855,7 @@
       </c>
       <c r="C3" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_2': '02'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_2': '02</t>
         </is>
       </c>
       <c r="D3" s="9" t="inlineStr">
@@ -2889,12 +2889,12 @@
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_3': '03'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_3': '03</t>
         </is>
       </c>
       <c r="D4" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_3': '&lt;p&gt;Able to rea</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_3': '&lt;p&gt;Able to read, understand and to provide written consent.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E4" s="9" t="inlineStr">
@@ -2931,12 +2931,12 @@
       </c>
       <c r="C5" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_4': '04'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_4': '04</t>
         </is>
       </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> understand and to provide written consent.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_4': '&lt;p&gt;Female study participants should not be &lt;usdm:tag name="Pregnant"/&gt; or plan to become pregnant during study participation and for 6 months after last investigational product administration.</t>
         </is>
       </c>
       <c r="E5" s="9" t="inlineStr">
@@ -2973,12 +2973,12 @@
       </c>
       <c r="C6" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_5': '05'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_5': '05</t>
         </is>
       </c>
       <c r="D6" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_4': '&lt;p&gt;Female study participants should not be &lt;usdm:tag name="Pregnant"/&gt; or plan to become pregnant during study participation and for 6 months after last investigational product administration.</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_5': '&lt;p&gt;Male participants if their sexual partners can become pregnant should use a method of contraception during study participation and for 6 months after the last administration of the investigated product.</t>
         </is>
       </c>
       <c r="E6" s="9" t="inlineStr">
@@ -3015,12 +3015,12 @@
       </c>
       <c r="C7" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_6': '06'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_6': '06</t>
         </is>
       </c>
       <c r="D7" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_5': '&lt;p&gt;Male participants if their sexual partners can become pregnant should use a method of contraception during study participation and for 6 months after the last administration of the investigated product.</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_6': '&lt;p&gt;Study participant is able and willing to comply with the requirements of this clinical study.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E7" s="9" t="inlineStr">
@@ -3057,12 +3057,12 @@
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_7': '07'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_7': '07</t>
         </is>
       </c>
       <c r="D8" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_6': '&lt;p&gt;Study participant is able and willing to comply with the requirements of this clinical study.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_7': '&lt;p&gt;Parkinson s disease subjects deemed appropriate for treatment of motor symptoms with a &lt;usdm:tag name="BC1_UDPRS"/&gt; Part III score &gt;&lt;usdm:tag name="BC1_MinValExcl"/&gt;.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E8" s="9" t="inlineStr">
@@ -3091,12 +3091,12 @@
       </c>
       <c r="C9" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_8': '08'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_8': '08</t>
         </is>
       </c>
       <c r="D9" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_7': '&lt;p&gt;Parkinson s disease subjects deemed appropriate for treatment of motor symptoms with a &lt;usdm:tag name="BC1_UDPRS"/&gt; Part III score &gt;&lt;usdm:tag name="BC1_MinValExcl"/&gt;.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_8': '&lt;p&gt;A reliable caregiver who is in frequent or daily contact with the patient and who will accompany the patient to the office and/or be available by telephone at designated times, will monitor administration of prescribed medications, and will be responsible for the overall care of the patient at home. The caregiver and the patient must be able to communicate in English and willing to comply with 26 weeks of transdermal therapy.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E9" s="9" t="inlineStr">
@@ -3133,12 +3133,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_9': '09'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_9': '09</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_8': '&lt;p&gt;A reliable caregiver who is in frequent or daily contact with the patient and who will accompany the patient to the office and/or be available by telephone at designated time</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_9': '&lt;p&gt;Persons who have previously completed or withdrawn from this study or any other study investigating xanomeline TTS or the oral formulation of xanomeline.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -3165,12 +3165,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_10': '10'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_10': '10</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t xml:space="preserve"> will monitor administration of prescribed medication</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_10': "&lt;p&gt;Use of any investigational agent or approved Alzheimer's therapeutic medication within 30 days prior to enrollment into the study.&lt;/p&gt;"</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3197,12 +3197,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_11': '11'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_11': '11</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t xml:space="preserve"> and will be responsible for the overall care of the patient at home. The caregiver and the patient must be able to communicate in English and willing to comply with 26 weeks of transdermal therapy.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_12': '&lt;p&gt;Diagnosis of serious neurological conditions, including &lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Stroke or vascular dementia documented by clinical history and/or radiographic findings interpretable by the investigator as indicative of these disorders&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Seizure disorder other than simple childhood febrile seizures&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Severe head trauma resulting in protracted loss of consciousness within the last 5 years, or multiple episodes of head trauma&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Parkinson\'s disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Multiple sclerosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Amyotrophic lateral sclerosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Myasthenia gravis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -3229,12 +3229,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_12': '12'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_12': '12</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_9': '&lt;p&gt;Persons who have previously completed or withdrawn from this study or any other study investigating xanomeline TTS or the oral formulation of xanomeline.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_13': '&lt;p&gt;Episode of depression meeting DSM-IV criteria within 3 months of screening.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -3261,12 +3261,12 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_13': '13'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_13': '13</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_10': "&lt;p&gt;Use of any investigational agent or approved Alzheimer's therapeutic medication within 30 days prior to enrollment into the study.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_14': '&lt;p&gt;A history within the last 5 years of the following:&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Schizophrenia&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Bipolar Disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Ethanol or psychoactive drug abuse or dependence. &lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -3293,12 +3293,12 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_14': '14'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_14': '14</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_11': '&lt;p&gt;Serious illness which required hospitalization within 3 months of screening.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_15': '&lt;p&gt;A history of syncope within the last 5 years.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -3325,12 +3325,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_15': '15'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_15': '15</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_12': '&lt;p&gt;Diagnosis of serious neurological condition</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_16': '&lt;p&gt;Evidence from ECG recording at screening of any of the following conditions :&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Left bundle branch block&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Bradycardia ≤50 beats per minute&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Sinus pauses &amp;gt;2 seconds&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Second or third degree heart block unless treated with a pacemaker&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Wolff-Parkinson-White syndrome&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Sustained supraventricular tachyarrhythmia including SVT≥10 sec, atrial fibrillation, atrial flutter.&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Ventricular tachycardia at a rate of ≥120 beats per minute lasting≥10 seconds.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -3357,12 +3357,12 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_16': '16b'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_16': '16b</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve"> including &lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Stroke or vascular dementia documented by clinical history and/or radiographic findings interpretable by the investigator as indicative of these disorders&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Seizure disorder other than simple childhood febrile seizures&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Severe head trauma resulting in protracted loss of consciousness within the last 5 year</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_17': '&lt;p&gt;A history within the last 5 years of a serious cardiovascular disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Clinically significant arrhythmia&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Symptomatic sick sinus syndrome not treated with a pacemaker&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Congestive heart failure refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Angina except angina controlled with PRN nitroglycerin&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Resting heart rate &amp;lt;50 or &amp;gt;100 beats per minute, on physical exam&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled hypertension.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -3389,12 +3389,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_17': '17'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_17': '17</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve"> or multiple episodes of head trauma&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Parkinson\'s disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Multiple sclerosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Amyotrophic lateral sclerosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Myasthenia gravis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_18': '&lt;p&gt;A history within the last 5 years of a serious gastrointestinal disorder, including &lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Chronic peptic/duodenal/gastric/esophageal ulcer that are untreated or refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Symptomatic diverticular disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Inflammatory bowel disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Pancreatitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Hepatitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Cirrhosis of the liver.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -3421,12 +3421,12 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_18': '18'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_18': '18</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_13': '&lt;p&gt;Episode of depression meeting DSM-IV criteria within 3 months of screening.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_19': '&lt;p&gt;A history within the last 5 years of a serious endocrine disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled Insulin Dependent Diabetes Mellitus (IDDM)&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Diabetic ketoacidosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Untreated hyperthyroidism&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Untreated hypothyroidism&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Other untreated endocrinological disorder&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -3453,12 +3453,12 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_19': '19'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_19': '19</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_14': '&lt;p&gt;A history within the last 5 years of the following:&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Schizophrenia&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Bipolar Disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Ethanol or psychoactive drug abuse or dependence. &lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_20': '&lt;p&gt; A history within the last 5 years of a serious respiratory disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Asthma with bronchospasm refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Decompensated chronic obstructive pulmonary disease.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -3485,12 +3485,12 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_20': '20'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_20': '20</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_15': '&lt;p&gt;A history of syncope within the last 5 years.&lt;/p&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_21': '&lt;p&gt;A history within the last 5 years of a serious genitourinary disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Renal failure&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled urinary retention.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -3517,12 +3517,12 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_21': '21'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_21': '21</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_16': '&lt;p&gt;Evidence from ECG recording at screening of any of the following conditions :&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Left bundle branch block&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Bradycardia ≤50 beats per minute&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Sinus pauses &amp;gt;2 seconds&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Second or third degree heart block unless treated with a pacemaker&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Wolff-Parkinson-White syndrome&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Sustained supraventricular tachyarrhythmia including SVT≥10 se</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_22': '&lt;p&gt;A history within the last 5 years of a serious rheumatologic disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Lupus&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Temporal arteritis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Severe rheumatoid arthritis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -3549,12 +3549,12 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_22': '22'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_22': '22</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atrial fibrillatio</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_23': '&lt;p&gt;A known history of human immunodeficiency virus (HIV) within the last 5 years.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -3581,12 +3581,12 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_23': '23'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_23': '23</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve"> atrial flutter.&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Ventricular tachycardia at a rate of ≥120 beats per minute lasting≥10 seconds.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_24': '&lt;p&gt;A history within the last 5 years of a serious infectious disease including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;a)  Neurosyphilis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;b)  Meningitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;c)  Encephalitis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -3613,12 +3613,12 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_24': '24'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_24': '24</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_17': '&lt;p&gt;A history within the last 5 years of a serious cardiovascular disorde</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_25': '&lt;p&gt;A history within the last 5 years of a primary or recurrent malignant disease with the exception of resected cutaneous squamous cell carcinoma in situ, basal cell carcinoma, cervical carcinoma in situ, or in situ prostate cancer with a normal PSA postresection.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -3645,12 +3645,12 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_25': '25'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_25': '25</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve"> including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Clinically significant arrhythmia&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Symptomatic sick sinus syndrome not treated with a pacemaker&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Congestive heart failure refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Angina except angina controlled with PRN nitroglycerin&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Resting heart rate &amp;lt;50 or &amp;gt;100 beats per minut</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_26': '&lt;p&gt;Visual, hearing, or communication disabilities impairing the ability to participate in the study; (for example, inability to speak or understand English, illiteracy).&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -3677,12 +3677,12 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_26': '26'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_26': '26</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve"> on physical exam&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled hypertension.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_27': "&lt;p&gt;Laboratory test values exceeding the Lilly Reference Range III for the patient's age in any of the following analytes: ↑ creatinine, ↑ total bilirubin, ↑ SGOT, ↑ SGPT, ↑ alkaline phosphatase, ↑ GGT, ↑↓ hemoglobin, ↑↓ white blood cell count, ↑↓ platelet count, ↑↓ serum sodium, potassium, or calcium.&lt;/p&gt;\n&lt;p&gt;If values exceed these laboratory reference ranges, clinical significance will be judged by the monitoring physicians. If the monitoring physician determines that the deviation from the reference range is not clinically significant, the patient may be included in the study. This decision will be documented.&lt;/p&gt;"</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -3709,12 +3709,12 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_27': '27b'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_27': '27b</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_18': '&lt;p&gt;A history within the last 5 years of a serious gastrointestinal disorde</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_29': '&lt;p&gt;Positive syphilis screening.&lt;/p&gt;\n&lt;p&gt;Positive syphilis screening. As determined by positive RPR followed up by confirmatory FTA-Abs. Confirmed patients are excluded unless there is a documented medical history of an alternative disease (for example, yaws) which caused the lab abnormality.&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3741,12 +3741,12 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_28': '28b'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_28': '28b</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve"> including &lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Chronic peptic/duodenal/gastric/esophageal ulcer that are untreated or refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Symptomatic diverticular disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Inflammatory bowel disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Pancreatitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Hepatitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Cirrhosis of the liver.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_30': '&lt;p&gt;Glycosylated hemoglobin (A1C). Required only on patients with known diabetes mellitus or random blood sugar &amp;gt;200 on screening labs. Patients will be excluded if levels are &amp;gt;9.5%&lt;/p&gt;</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -3773,12 +3773,12 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_29': '29b'</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_29': '29b</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_19': '&lt;p&gt;A history within the last 5 years of a serious endocrine disorde</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_31': '&lt;p&gt;Treatment with the following medications within the specified washout periods prior to enrollment and during the\n  study:&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n  &lt;li&gt;\n    &lt;p&gt;Anticonvulsants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Depakote&amp;#174; (valproic acid) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dilantin&amp;#174; (phenytoin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Felbatol&amp;#174;\n          (felbamate)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Klonopin&amp;#174; (clonazepam)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lamictal&amp;#174; (lamotrigine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mysoline&amp;#174; (primidone)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Neurontin&amp;#174;\n          (gabapentin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Phenobarbitol&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tegretol&amp;#174; (carbamazepine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Alpha receptor blockers including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aldomet&amp;#174; (methyldopa) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cardura&amp;#174;\n          (doxazosin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Catapres&amp;#174; (clonidine)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Hytrin&amp;#174; (terazosin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Minipress&amp;#174; (prazosin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tenex&amp;#174; (guanfacine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wytensin&amp;#174;\n          (guanabenz) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;The use of low doses\n        (2 mg daily) of either Hytrin&lt;/b&gt;&amp;#174; &lt;b&gt;or Cardura&lt;/b&gt;&amp;#174; &lt;b&gt;for relief of\n        urinary retention for patients with prostatic hypertrophy will be considered\n        on a case-by-case basis provided blood pressure is stable and the medication\n        has not had demonstrable effect on dementia symptoms in the opinion of the treating\n        physician. Contact CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Calcium channel blockers\n      that are CNS active including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Calan&amp;#174; , Isoptin&amp;#174; , Verelan&amp;#174; (verapamil) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cardizem&amp;#174; (diltiazem) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nimotop&amp;#174;\n          (nimodipine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Adalat&amp;#174; , Procardia XL&amp;#174;\n          (nifedipine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Cardene&lt;/b&gt;&amp;#174; &lt;b&gt;(nicardipine),\n        Norvasc&lt;/b&gt;&amp;#174; &lt;b&gt;, (amlodipine), and DynaCirc&lt;/b&gt;&amp;#174; &lt;b&gt;(isradipine) will\n        be allowed during the study. If a patient is taking an excluded calcium channel\n        blocker and is changed to an equivalent dose of an allowed calcium channel blocker,\n        enrollment may proceed in as little as 24 hours though 1 week is preferred when\n        possible.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Beta blockers including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Betapace&amp;#174; (sotalol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Inderal&amp;#174; (propranolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lopressor&amp;#174;\n          , Toprol XL&amp;#174; (metoprolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Corgard&amp;#174; (nadolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Sectral&amp;#174; (acebutolol)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tenormin&amp;#174; (atenolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Visken&amp;#174; (pindolol)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Beta\n        blocker eye drops for glaucoma will be considered on a case-by-case basis. Call\n        medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Beta sympathomimetics (unless inhaled) including\n      but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Alupent&amp;#174; tablets\n          (metaproterenol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Brethine&amp;#174; tablets\n          (terbutaline) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dopamine &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Proventil Repetabs&amp;#174; , Ventolin&amp;#174; tablets (albuterol tablets)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;Parasympathomimetics (cholinergics) (unless opthalmic) including but not limited to\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Antilirium&amp;#174; (physostigmine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aricept&amp;#174; (donepezil) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cognex&amp;#174; (tacrine) &lt;/td&gt;\n        &lt;td&gt;1\n          month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mestinon&amp;#174; (pyridostigmine) &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Reglan&amp;#174; (metoclopramide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Urecholine&amp;#174;\n          , Duvoid (bethanechol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Cholinergic eye drops for treatment of glaucoma will be allowed during the study on a case-by-case basis.\n        Please contact the CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Muscle relaxants-centrally active including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Equanil&amp;#174; (meprobamate) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Flexeril&amp;#174; (cyclobenzaprine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lioresal&amp;#174; (baclofen) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norflex&amp;#174; (orphenadrine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Parafon Forte&amp;#174; (chlorzoxazone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Robaxin&amp;#174; (methocarbamol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Skelaxin&amp;#174; (metaxalone)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Soma&amp;#174; (carisoprodol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Monamine oxidase inhibitors (MAOI) including but not limited to&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Eldepryl&amp;#174; (selegiline)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nardil&amp;#174; (phenelzine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Parnate&amp;#174; (tranylcypromine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Parasympatholytics including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Antivert&amp;#174; , Bonine&amp;#174; , Dramamine II&amp;#174; (meclizine)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Artane&amp;#174; (trihexyphenidyl)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Bellergal-S&amp;#174; (alkaloids of belladonna and ergotamine) &lt;/td&gt;\n        &lt;td&gt;2 weeks &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Bentyl&amp;#174; (dicyclomine) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cogentin&amp;#174; (benztropine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cystospaz&amp;#174;, Levsin&amp;#174; , Levsinex&amp;#174; (hyoscyamine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ditropan&amp;#174;\n          (oxybutynin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Donnatal&amp;#174; , Hyosophen&amp;#174;\n          (atropine, scopolamine, hyoscyamine and phenobarbitol) &lt;/td&gt;\n        &lt;td&gt;1 month &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dramamine&amp;#174; (dimenhydrinate)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lomotil&amp;#174;, Lonox&amp;#174; (atropine, diphenoxylate) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pro-Banthine&amp;#174;(propantheline) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Robinul&amp;#174; (glycopyrrolate)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tigan&amp;#174; (trimethobenzamide) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Transderm-Scop&amp;#174; (scopolamine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Urispas&amp;#174; (flavoxate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antidepressants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Anafranil&amp;#174; (clomipramine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Asendin&amp;#174;\n          (amoxapine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Desyrel&amp;#174; (trazodone)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Effexor&amp;#174; (venlafaxine) &lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Elavil&amp;#174; (amitriptyline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ludiomil&amp;#174;\n          (maprotiline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norpramin&amp;#174; (desipramine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pamelor&amp;#174; , Aventyl&amp;#174; (nortriptyline)&lt;/td&gt;\n        &lt;td&gt; 1\n          month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Paxil&amp;#174; (paroxetine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prozac&amp;#174;\n          (fluoxetine&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Remeron&amp;#174; (mirtazapine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serzone&amp;#174; (nefazodone) &lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Sinequan&amp;#174;\n          (doxepin)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tofranil&amp;#174; (imipramine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vivactil&amp;#174; (protriptyline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wellbutrin&amp;#174; (bupropion)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zoloft&amp;#174;\n          (sertraline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Systemic corticosteroids including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cortisone&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Decadron&amp;#174; (dexamethasone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Depo-Medrol&amp;#174; (methylprednisolone)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prednisone&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Xanthine derivatives\n      including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aminophylline&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Fioricet&amp;#174; , Esgic&amp;#174; , Phrenilin Forte&amp;#174; (caffeine, butalbital)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Theo-Dur&amp;#174; (theophylline)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wigraine&amp;#174; , Cafergot&amp;#174; (caffeine, ergotamine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Histamine (H2 ) antagonists including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Axid&amp;#174; (nizatidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pepcid&amp;#174; (famotidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tagamet&amp;#174; (cimetidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zantac&amp;#174; (ranitidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;If an H 2 antagonist is needed by the patient, Axid&lt;/b&gt;&amp;#174; &lt;b&gt;will be&lt;/b&gt; &lt;b&gt;allowed on a case-by-case\n        basis. Please consult CRO&lt;/b&gt; &lt;b&gt;medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Narcotic Analgesics including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Darvocet-N\n          100&amp;#174; , (propoxyphene)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Demerol&amp;#174; (meperidine)&lt;/td&gt;\n        &lt;td&gt;1\n          week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dilaudid&amp;#174; (hydromorphone)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Duragesic&amp;#174; (fentanyl)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;MS\n          Contin&amp;#174; , Roxanol&amp;#174; , Oramorph&amp;#174; (morphine) &lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Percocet&amp;#174; , Roxicet&amp;#174; (oxycodone with acetaminophen)&lt;/td&gt;\n        &lt;td&gt;3\n          days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Percodan&amp;#174; , Roxiprin&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Stadol&amp;#174; (butorphanol)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Talacen&amp;#174;\n          (pentazocine)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tylenol #2&amp;#174; , #3&amp;#174;\n          , #4&amp;#174; (codeine and acetaminophen) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tylox&amp;#174;\n          , Roxilox&amp;#174; (oxycodone)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vicodin&amp;#174;, Lorcet&amp;#174; (hydrocodone)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Percocet\n        (oxycodone with acetaminophen) and Tylenol&lt;/b&gt;&amp;#174; &lt;b&gt;with codeine #2, #3, #4\n        (acetaminophen + codeine) ARE allowed in the month prior to enrollment, but\n        are not permitted in the 3 days prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Neuroleptics\n      (antipsychotics) including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Clozaril&amp;#174;\n          (clozapine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Haldol&amp;#174; (haloperidol)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Loxitane&amp;#174; (loxapine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mellaril&amp;#174; (thioridazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Moban&amp;#174;\n          (molindone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Navane&amp;#174; (thiothixene)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Orap&amp;#174; (pimozide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prolixin&amp;#174; (fluphenazine)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Risperdal&amp;#174;\n          (risperidone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Stelazine&amp;#174; (trifluoperazine)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Thorazine&amp;#174; (chlorpromazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Trilafon&amp;#174; (perphenazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serentil&amp;#174;\n          (mesoridazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;The use of neuroleptics\n        on a daily basis must be discontinued 2 to 4 weeks prior to enrollment. The\n        use of neuroleptics on an as-needed basis is allowable during the screening\n        period, but the last dose must be at least 7 days prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antianxiety agents including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Atarax&amp;#174; (hydroxyzine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;BuSpar&amp;#174;\n          (buspirone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Librium&amp;#174; (chlordiazepoxide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serax&amp;#174; (oxazepam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tranxene&amp;#174; (clorazepate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Valium&amp;#174; (diazepam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vistaril&amp;#174; (hydroxyzine pamoate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Xanax&amp;#174; (alprazolam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Ativan&lt;/b&gt;&amp;#174; &lt;b&gt;(lorazepam) should be discontinued on a daily\n        basis 2 weeks&lt;/b&gt;&lt;/p&gt;\n    &lt;p&gt;&lt;b&gt;prior to enrollment. It may be used on an as-needed\n        basis during the screening period, but is not permitted in the 24 hours prior\n        to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Hypnotics/Sedatives including but not limited to&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ambien&amp;#174; (zolpidem)&lt;/td&gt;\n        &lt;td&gt; 3 days\n        &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dalmane&amp;#174; (flurazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Doral&amp;#174; (quazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Halcion&amp;#174; (triazolam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nembutal&amp;#174; &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;ProSom&amp;#174; (estazolam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Restoril&amp;#174;\n          (temazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Seconal&amp;#174;&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Chloral Hydrate is allowed on an as-needed basis during screening, but is not permitted in the 24 hours prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Histamine (H1 ) antagonists including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Actifed&amp;#174; , Actifed Plus&amp;#174; (triprolidine) Benadryl&amp;#174;\n          , Unisom&amp;#174; , Tylenol P.M.&amp;#174; &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;(diphenhydramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Compazine&amp;#174; (prochlorperazine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Contac&amp;#174; , Coricidin D&amp;#174; , Sinutab&amp;#174; , Novahistine&amp;#174; , Alka\n          Seltzer Plus&amp;#174; , Naldecon&amp;#174; , Sudafed Plus&amp;#174; , Tylenol Cold&amp;#174; , Tylenol\n          Cold and Flu&amp;#174; (chlorpheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dimetapp&amp;#174;\n          (brompheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Drixoral&amp;#174; (dexbrompheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Hismanal&amp;#174; (astemizole)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Phenergan&amp;#174;\n          (promethazine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Seldane&amp;#174; (terfenadine)&lt;/td&gt;\n        &lt;td&gt;1\n          week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tavist&amp;#174; (clemastine fumarate)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zyrtec&amp;#174; (cetrizine) &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Allegra&lt;/b&gt;&amp;#174;\n      &lt;b&gt;(fexofenadine hydrochloride) or Claritin&lt;/b&gt;&amp;#174; &lt;b&gt;(loratadine) may be taken\n        on as-needed basis during screening but must be discontinued within 24 hours\n        of enrollment.&lt;/b&gt;\n    &lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Stimulants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cylert&amp;#174; (pemoline) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ritalin&amp;#174; (methylphenidate)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antiarrhythmics including but not limited to the following&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Adenocard&amp;#174; (adenosine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cordarone&amp;#174;\n          (amiodarone) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ethmozine&amp;#174; (moricizine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mexitil&amp;#174; (mexiletine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norpace&amp;#174; (disopyramide)\n        &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Procan&amp;#174; (procainamide) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Quinaglute&amp;#174;\n          (quinidine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Rythmol&amp;#174; (propafenone) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tambocor&amp;#174;\n          (flecainide) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tonocard&amp;#174; (tocainide)&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Requirement of these drugs for control of cardiac arrhythmia indicates that\n        the patient should be excluded from the study. If discontinuation of an antiarrhythmic\n        is considered, please discuss case with CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Miscellaneous drugs including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Coenzyme\n          Q&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Eskalith&amp;#174; , Lithobid&amp;#174; (lithium)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ginkgo biloba&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lecithin\n        &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lecithin &lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lupron&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tamoxifen&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Estrogen supplements are permitted during the study, but dosage must be stable for at least 3 months prior to\n      enrollment.&lt;/p&gt;\n  &lt;/li&gt;\n&lt;/ol&gt;</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -3805,12 +3805,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_30': '30b'</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled Insulin Dependent Diabetes Mellitus (IDDM)&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Diabetic ketoacidosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Untreated hyperthyroidism&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Untreated hypothyroidism&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Other untreated endocrinological disorder&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
+          <t xml:space="preserve"> 'EligibilityCriterion_30': '30b</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -3840,2129 +3835,12 @@
           <t xml:space="preserve"> 'EligibilityCriterion_31': '31b</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_20': '&lt;p&gt; A history within the last 5 years of a serious respiratory disorde</t>
-        </is>
-      </c>
       <c r="E32" t="inlineStr">
         <is>
           <t xml:space="preserve"> 'EligibilityCriterion_31': 'Exclusion Criteria</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Asthma with bronchospasm refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Decompensated chronic obstructive pulmonary disease.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_21': '&lt;p&gt;A history within the last 5 years of a serious genitourinary disorde</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Renal failure&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled urinary retention.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_22': '&lt;p&gt;A history within the last 5 years of a serious rheumatologic disorde</t>
-        </is>
-      </c>
-      <c r="H36" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Lupus&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Temporal arteritis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Severe rheumatoid arthritis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_23': '&lt;p&gt;A known history of human immunodeficiency virus (HIV) within the last 5 years.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_24': '&lt;p&gt;A history within the last 5 years of a serious infectious disease including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;a)  Neurosyphilis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;b)  Meningitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;c)  Encephalitis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_25': '&lt;p&gt;A history within the last 5 years of a primary or recurrent malignant disease with the exception of resected cutaneous squamous cell carcinoma in sit</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> basal cell carcinom</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> cervical carcinoma in sit</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> or in situ prostate cancer with a normal PSA postresection.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="H43" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_26': '&lt;p&gt;Visua</t>
-        </is>
-      </c>
-      <c r="H44" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> hearin</t>
-        </is>
-      </c>
-      <c r="H45" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> or communication disabilities impairing the ability to participate in the study; (for exampl</t>
-        </is>
-      </c>
-      <c r="H46" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> inability to speak or understand Englis</t>
-        </is>
-      </c>
-      <c r="H47" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> illiteracy).&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_27': "&lt;p&gt;Laboratory test values exceeding the Lilly Reference Range III for the patient's age in any of the following analytes: ↑ creatinin</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑ total bilirubi</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑ SGO</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑ SGP</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑ alkaline phosphatas</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑ GG</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑↓ hemoglobi</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑↓ white blood cell coun</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑↓ platelet coun</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ↑↓ serum sodiu</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> potassiu</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> or calcium.&lt;/p&gt;\n&lt;p&gt;If values exceed these laboratory reference range</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> clinical significance will be judged by the monitoring physicians. If the monitoring physician determines that the deviation from the reference range is not clinically significan</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> the patient may be included in the study. This decision will be documented.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_28': '&lt;p&gt;Central laboratory test values below reference range for folat</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> and Vitamin B 12</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> and outside reference range for thyroid function tests.&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n  &lt;li&gt;\n    &lt;p&gt;Folate reference range 2.0 to 25.0 ng/mL. Patients will be allowed to enroll if their folate levels are above the upper end of the range if patients are taking vitamin supplements.&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Vitamin B 12 reference range 130 to 900 pg/mL. Patients will be allowed to enroll if their B 12 levels are above the upper reference range if patients are taking oral vitamin supplements.&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Thyroid functions&lt;/p&gt;\n    &lt;ol&gt;\n      &lt;li&gt;\n        &lt;p&gt;Thyroid Uptake reference range 25 to 38%. Patients will be allowed to enroll with results of 23 to 51% provided the remainder of the thyroid profile is normal and there are no clinical signs or symptoms of thyroid abnormality.&lt;/p&gt;\n      &lt;/li&gt;\n      &lt;li&gt;\n        &lt;p&gt;TSH reference range 0.32 to 5.0. Patients will be allowed to enroll with results of 0.03 to 6.2 if patients are taking stable doses of exogenous thyroid supplement</t>
-        </is>
-      </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> with normal free thyroid inde</t>
-        </is>
-      </c>
-      <c r="H66" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> and show no clinical signs or symptoms of thyroid abnormality.&lt;/p&gt;\n      &lt;/li&gt;\n      &lt;li&gt;\n        &lt;p&gt;Total T4 reference range 4.5 to 12.5. Patients will be allowed to enroll with results of 4.1 to 13.4 if patients are taking stable doses of exogenous thyroid hormon</t>
-        </is>
-      </c>
-      <c r="H67" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> with normal free thyroid inde</t>
-        </is>
-      </c>
-      <c r="H68" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> and show no clinical signs or symptoms of thyroid abnormality.&lt;/p&gt;\n      &lt;/li&gt;\n      &lt;li&gt;\n        &lt;p&gt;Free Thyroid Index reference range 1.1 to 4.6.&lt;/p&gt;\n      &lt;/li&gt;\n    &lt;/ol&gt;\n  &lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_29': '&lt;p&gt;Positive syphilis screening.&lt;/p&gt;\n&lt;p&gt;Positive syphilis screening. As determined by positive RPR followed up by confirmatory FTA-Abs. Confirmed patients are excluded unless there is a documented medical history of an alternative disease (for exampl</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> yaws) which caused the lab abnormality.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_30': '&lt;p&gt;Glycosylated hemoglobin (A1C). Required only on patients with known diabetes mellitus or random blood sugar &amp;gt;200 on screening labs. Patients will be excluded if levels are &amp;gt;9.5%&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 'EligibilityCriterion_31': '&lt;p&gt;Treatment with the following medications within the specified washout periods prior to enrollment and during the\n  study:&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n  &lt;li&gt;\n    &lt;p&gt;Anticonvulsants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Depakote&amp;#174; (valproic acid) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dilantin&amp;#174; (phenytoin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Felbatol&amp;#174;\n          (felbamate)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Klonopin&amp;#174; (clonazepam)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lamictal&amp;#174; (lamotrigine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mysoline&amp;#174; (primidone)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Neurontin&amp;#174;\n          (gabapentin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Phenobarbitol&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tegretol&amp;#174; (carbamazepine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Alpha receptor blockers including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aldomet&amp;#174; (methyldopa) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cardura&amp;#174;\n          (doxazosin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Catapres&amp;#174; (clonidine)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Hytrin&amp;#174; (terazosin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Minipress&amp;#174; (prazosin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tenex&amp;#174; (guanfacine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wytensin&amp;#174;\n          (guanabenz) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;The use of low doses\n        (2 mg daily) of either Hytrin&lt;/b&gt;&amp;#174; &lt;b&gt;or Cardura&lt;/b&gt;&amp;#174; &lt;b&gt;for relief of\n        urinary retention for patients with prostatic hypertrophy will be considered\n        on a case-by-case basis provided blood pressure is stable and the medication\n        has not had demonstrable effect on dementia symptoms in the opinion of the treating\n        physician. Contact CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Calcium channel blockers\n      that are CNS active including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Calan&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H73" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Isoptin&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H74" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Verelan&amp;#174; (verapamil) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cardizem&amp;#174; (diltiazem) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nimotop&amp;#174;\n          (nimodipine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Adalat&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H75" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Procardia XL&amp;#174;\n          (nifedipine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Cardene&lt;/b&gt;&amp;#174; &lt;b&gt;(nicardipine</t>
-        </is>
-      </c>
-      <c r="H76" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>\n        Norvasc&lt;/b&gt;&amp;#174; &lt;b</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (amlodipine</t>
-        </is>
-      </c>
-      <c r="H78" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> and DynaCirc&lt;/b&gt;&amp;#174; &lt;b&gt;(isradipine) will\n        be allowed during the study. If a patient is taking an excluded calcium channel\n        blocker and is changed to an equivalent dose of an allowed calcium channel blocke</t>
-        </is>
-      </c>
-      <c r="H79" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t xml:space="preserve">\n        enrollment may proceed in as little as 24 hours though 1 week is preferred when\n        possible.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Beta blockers including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Betapace&amp;#174; (sotalol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Inderal&amp;#174; (propranolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lopressor&amp;#174;\n         </t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Toprol XL&amp;#174; (metoprolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Corgard&amp;#174; (nadolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Sectral&amp;#174; (acebutolol)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tenormin&amp;#174; (atenolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Visken&amp;#174; (pindolol)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Beta\n        blocker eye drops for glaucoma will be considered on a case-by-case basis. Call\n        medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Beta sympathomimetics (unless inhaled) including\n      but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Alupent&amp;#174; tablets\n          (metaproterenol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Brethine&amp;#174; tablets\n          (terbutaline) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dopamine &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Proventil Repetabs&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ventolin&amp;#174; tablets (albuterol tablets)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;Parasympathomimetics (cholinergics) (unless opthalmic) including but not limited to\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Antilirium&amp;#174; (physostigmine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aricept&amp;#174; (donepezil) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cognex&amp;#174; (tacrine) &lt;/td&gt;\n        &lt;td&gt;1\n          month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mestinon&amp;#174; (pyridostigmine) &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Reglan&amp;#174; (metoclopramide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Urecholine&amp;#174;\n         </t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Duvoid (bethanechol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Cholinergic eye drops for treatment of glaucoma will be allowed during the study on a case-by-case basis.\n        Please contact the CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Muscle relaxants-centrally active including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Equanil&amp;#174; (meprobamate) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Flexeril&amp;#174; (cyclobenzaprine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lioresal&amp;#174; (baclofen) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norflex&amp;#174; (orphenadrine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Parafon Forte&amp;#174; (chlorzoxazone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Robaxin&amp;#174; (methocarbamol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Skelaxin&amp;#174; (metaxalone)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Soma&amp;#174; (carisoprodol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Monamine oxidase inhibitors (MAOI) including but not limited to&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Eldepryl&amp;#174; (selegiline)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nardil&amp;#174; (phenelzine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Parnate&amp;#174; (tranylcypromine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Parasympatholytics including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Antivert&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Bonine&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Dramamine II&amp;#174; (meclizine)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Artane&amp;#174; (trihexyphenidyl)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Bellergal-S&amp;#174; (alkaloids of belladonna and ergotamine) &lt;/td&gt;\n        &lt;td&gt;2 weeks &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Bentyl&amp;#174; (dicyclomine) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cogentin&amp;#174; (benztropine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cystospaz&amp;#174</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Levsin&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Levsinex&amp;#174; (hyoscyamine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ditropan&amp;#174;\n          (oxybutynin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Donnatal&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Hyosophen&amp;#174;\n          (atropin</t>
-        </is>
-      </c>
-      <c r="H88" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> scopolamin</t>
-        </is>
-      </c>
-      <c r="H89" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> hyoscyamine and phenobarbitol) &lt;/td&gt;\n        &lt;td&gt;1 month &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dramamine&amp;#174; (dimenhydrinate)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lomotil&amp;#174</t>
-        </is>
-      </c>
-      <c r="H90" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Lonox&amp;#174; (atropin</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> diphenoxylate) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pro-Banthine&amp;#174;(propantheline) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Robinul&amp;#174; (glycopyrrolate)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tigan&amp;#174; (trimethobenzamide) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Transderm-Scop&amp;#174; (scopolamine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Urispas&amp;#174; (flavoxate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antidepressants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Anafranil&amp;#174; (clomipramine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Asendin&amp;#174;\n          (amoxapine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Desyrel&amp;#174; (trazodone)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Effexor&amp;#174; (venlafaxine) &lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Elavil&amp;#174; (amitriptyline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ludiomil&amp;#174;\n          (maprotiline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norpramin&amp;#174; (desipramine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pamelor&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D93" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Aventyl&amp;#174; (nortriptyline)&lt;/td&gt;\n        &lt;td&gt; 1\n          month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Paxil&amp;#174; (paroxetine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prozac&amp;#174;\n          (fluoxetine&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Remeron&amp;#174; (mirtazapine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serzone&amp;#174; (nefazodone) &lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Sinequan&amp;#174;\n          (doxepin)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tofranil&amp;#174; (imipramine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vivactil&amp;#174; (protriptyline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wellbutrin&amp;#174; (bupropion)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zoloft&amp;#174;\n          (sertraline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Systemic corticosteroids including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cortisone&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Decadron&amp;#174; (dexamethasone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Depo-Medrol&amp;#174; (methylprednisolone)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prednisone&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Xanthine derivatives\n      including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aminophylline&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Fioricet&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D94" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Esgic&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D95" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Phrenilin Forte&amp;#174; (caffein</t>
-        </is>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D96" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> butalbital)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Theo-Dur&amp;#174; (theophylline)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wigraine&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D97" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Cafergot&amp;#174; (caffein</t>
-        </is>
-      </c>
-      <c r="H97" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D98" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> ergotamine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Histamine (H2 ) antagonists including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Axid&amp;#174; (nizatidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pepcid&amp;#174; (famotidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tagamet&amp;#174; (cimetidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zantac&amp;#174; (ranitidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;If an H 2 antagonist is needed by the patien</t>
-        </is>
-      </c>
-      <c r="H98" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D99" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Axid&lt;/b&gt;&amp;#174; &lt;b&gt;will be&lt;/b&gt; &lt;b&gt;allowed on a case-by-case\n        basis. Please consult CRO&lt;/b&gt; &lt;b&gt;medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Narcotic Analgesics including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Darvocet-N\n          100&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H99" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D100" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> (propoxyphene)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Demerol&amp;#174; (meperidine)&lt;/td&gt;\n        &lt;td&gt;1\n          week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dilaudid&amp;#174; (hydromorphone)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Duragesic&amp;#174; (fentanyl)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;MS\n          Contin&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H100" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D101" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Roxanol&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H101" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D102" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Oramorph&amp;#174; (morphine) &lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Percocet&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H102" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D103" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Roxicet&amp;#174; (oxycodone with acetaminophen)&lt;/td&gt;\n        &lt;td&gt;3\n          days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Percodan&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H103" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D104" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Roxiprin&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Stadol&amp;#174; (butorphanol)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Talacen&amp;#174;\n          (pentazocine)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tylenol #2&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H104" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D105" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #3&amp;#174;\n         </t>
-        </is>
-      </c>
-      <c r="H105" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D106" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #4&amp;#174; (codeine and acetaminophen) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tylox&amp;#174;\n         </t>
-        </is>
-      </c>
-      <c r="H106" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D107" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Roxilox&amp;#174; (oxycodone)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vicodin&amp;#174</t>
-        </is>
-      </c>
-      <c r="H107" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Lorcet&amp;#174; (hydrocodone)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Percocet\n        (oxycodone with acetaminophen) and Tylenol&lt;/b&gt;&amp;#174; &lt;b&gt;with codeine #</t>
-        </is>
-      </c>
-      <c r="H108" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D109" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #</t>
-        </is>
-      </c>
-      <c r="H109" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D110" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> #4\n        (acetaminophen + codeine) ARE allowed in the month prior to enrollmen</t>
-        </is>
-      </c>
-      <c r="H110" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D111" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> but\n        are not permitted in the 3 days prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Neuroleptics\n      (antipsychotics) including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Clozaril&amp;#174;\n          (clozapine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Haldol&amp;#174; (haloperidol)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Loxitane&amp;#174; (loxapine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mellaril&amp;#174; (thioridazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Moban&amp;#174;\n          (molindone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Navane&amp;#174; (thiothixene)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Orap&amp;#174; (pimozide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prolixin&amp;#174; (fluphenazine)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Risperdal&amp;#174;\n          (risperidone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Stelazine&amp;#174; (trifluoperazine)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Thorazine&amp;#174; (chlorpromazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Trilafon&amp;#174; (perphenazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serentil&amp;#174;\n          (mesoridazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;The use of neuroleptics\n        on a daily basis must be discontinued 2 to 4 weeks prior to enrollment. The\n        use of neuroleptics on an as-needed basis is allowable during the screening\n        perio</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B112" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D112" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> but the last dose must be at least 7 days prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antianxiety agents including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Atarax&amp;#174; (hydroxyzine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;BuSpar&amp;#174;\n          (buspirone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Librium&amp;#174; (chlordiazepoxide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serax&amp;#174; (oxazepam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tranxene&amp;#174; (clorazepate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Valium&amp;#174; (diazepam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vistaril&amp;#174; (hydroxyzine pamoate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Xanax&amp;#174; (alprazolam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Ativan&lt;/b&gt;&amp;#174; &lt;b&gt;(lorazepam) should be discontinued on a daily\n        basis 2 weeks&lt;/b&gt;&lt;/p&gt;\n    &lt;p&gt;&lt;b&gt;prior to enrollment. It may be used on an as-needed\n        basis during the screening perio</t>
-        </is>
-      </c>
-      <c r="H112" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B113" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D113" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> but is not permitted in the 24 hours prior\n        to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Hypnotics/Sedatives including but not limited to&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ambien&amp;#174; (zolpidem)&lt;/td&gt;\n        &lt;td&gt; 3 days\n        &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dalmane&amp;#174; (flurazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Doral&amp;#174; (quazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Halcion&amp;#174; (triazolam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nembutal&amp;#174; &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;ProSom&amp;#174; (estazolam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Restoril&amp;#174;\n          (temazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Seconal&amp;#174;&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Chloral Hydrate is allowed on an as-needed basis during screenin</t>
-        </is>
-      </c>
-      <c r="H113" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D114" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> but is not permitted in the 24 hours prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Histamine (H1 ) antagonists including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Actifed&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H114" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D115" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Actifed Plus&amp;#174; (triprolidine) Benadryl&amp;#174;\n         </t>
-        </is>
-      </c>
-      <c r="H115" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B116" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D116" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Unisom&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H116" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B117" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D117" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Tylenol P.M.&amp;#174; &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;(diphenhydramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Compazine&amp;#174; (prochlorperazine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Contac&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H117" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B118" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D118" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Coricidin D&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H118" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B119" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D119" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Sinutab&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H119" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D120" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Novahistine&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H120" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D121" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Alka\n          Seltzer Plus&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H121" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D122" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Naldecon&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H122" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B123" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D123" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Sudafed Plus&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H123" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B124" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D124" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Tylenol Cold&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H124" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B125" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D125" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Tylenol\n          Cold and Flu&amp;#174; (chlorpheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dimetapp&amp;#174;\n          (brompheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Drixoral&amp;#174; (dexbrompheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Hismanal&amp;#174; (astemizole)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Phenergan&amp;#174;\n          (promethazine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Seldane&amp;#174; (terfenadine)&lt;/td&gt;\n        &lt;td&gt;1\n          week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tavist&amp;#174; (clemastine fumarate)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zyrtec&amp;#174; (cetrizine) &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Allegra&lt;/b&gt;&amp;#174;\n      &lt;b&gt;(fexofenadine hydrochloride) or Claritin&lt;/b&gt;&amp;#174; &lt;b&gt;(loratadine) may be taken\n        on as-needed basis during screening but must be discontinued within 24 hours\n        of enrollment.&lt;/b&gt;\n    &lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Stimulants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cylert&amp;#174; (pemoline) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ritalin&amp;#174; (methylphenidate)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antiarrhythmics including but not limited to the following&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Adenocard&amp;#174; (adenosine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cordarone&amp;#174;\n          (amiodarone) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ethmozine&amp;#174; (moricizine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mexitil&amp;#174; (mexiletine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norpace&amp;#174; (disopyramide)\n        &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Procan&amp;#174; (procainamide) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Quinaglute&amp;#174;\n          (quinidine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Rythmol&amp;#174; (propafenone) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tambocor&amp;#174;\n          (flecainide) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tonocard&amp;#174; (tocainide)&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Requirement of these drugs for control of cardiac arrhythmia indicates that\n        the patient should be excluded from the study. If discontinuation of an antiarrhythmic\n        is considere</t>
-        </is>
-      </c>
-      <c r="H125" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D126" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> please discuss case with CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Miscellaneous drugs including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Coenzyme\n          Q&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Eskalith&amp;#174;</t>
-        </is>
-      </c>
-      <c r="H126" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D127" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Lithobid&amp;#174; (lithium)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ginkgo biloba&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lecithin\n        &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lecithin &lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lupron&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tamoxifen&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Estrogen supplements are permitted during the stud</t>
-        </is>
-      </c>
-      <c r="H127" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="D128" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> but dosage must be stable for at least 3 months prior to\n      enrollment.&lt;/p&gt;\n  &lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="H128" t="inlineStr">
         <is>
           <t> </t>
         </is>

</xml_diff>

<commit_message>
Created main and adjusted TS and TI acc.
</commit_message>
<xml_diff>
--- a/Output/sdtm_mapping_results.xlsx
+++ b/Output/sdtm_mapping_results.xlsx
@@ -2740,7 +2740,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
@@ -2803,7 +2803,7 @@
     <row r="2" ht="72.5" customHeight="1">
       <c r="A2" s="9" t="inlineStr">
         <is>
-          <t>CB0321</t>
+          <t>Error in expression for TIVERS: study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0]; studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
         </is>
       </c>
       <c r="B2" s="9" t="inlineStr">
@@ -2813,27 +2813,27 @@
       </c>
       <c r="C2" s="9" t="inlineStr">
         <is>
-          <t>01</t>
+          <t>tudy.versions.studyDesigns.eligibilityCriteria.{id: identifier}</t>
         </is>
       </c>
       <c r="D2" s="9" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Male and female participants &lt;usdm:tag name="min_age"/&gt; - &lt;usdm:tag name="max_age"/&gt; years of age.&lt;/p&gt;</t>
+          <t>tudy.versions.($EligTxt := function($id) {(eligibilityCriterionItems[id=$id].text)}; studyDesigns.eligibilityCriteria{id: $EligTxt(criterionItemId)})</t>
         </is>
       </c>
       <c r="E2" s="9" t="inlineStr">
         <is>
-          <t>Inclusion Criteria</t>
+          <t>tudy.versions.studyDesigns.eligibilityCriteria{id: category.decode}</t>
         </is>
       </c>
       <c r="F2" s="6" t="inlineStr">
         <is>
-          <t> </t>
+          <t>tudy.versions.studyDesigns.eligibilityCriteria{id: notes.codes.decode}</t>
         </is>
       </c>
       <c r="G2" s="34" t="inlineStr">
         <is>
-          <t> </t>
+          <t>study.versions.($sponsorIdVal:=roles[code.code="C70793"].organizationIds[0]; studyIdentifiers[scopeId=$sponsorIdVal].text;)</t>
         </is>
       </c>
       <c r="H2" s="33" t="inlineStr">
@@ -2845,1252 +2845,256 @@
     <row r="3" ht="29" customHeight="1">
       <c r="A3" s="9" t="inlineStr">
         <is>
-          <t>CB0321</t>
+          <t>DOMAIN</t>
         </is>
       </c>
       <c r="B3" s="9" t="inlineStr">
         <is>
+          <t>Domain Abbreviation</t>
+        </is>
+      </c>
+      <c r="C3" s="9" t="inlineStr">
+        <is>
+          <t>Char</t>
+        </is>
+      </c>
+      <c r="D3" s="9" t="inlineStr">
+        <is>
+          <t>Identifier</t>
+        </is>
+      </c>
+      <c r="E3" s="9" t="inlineStr">
+        <is>
+          <t>Req</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="n"/>
+      <c r="G3" s="38" t="n"/>
+      <c r="H3" s="9" t="inlineStr">
+        <is>
           <t>TI</t>
-        </is>
-      </c>
-      <c r="C3" s="9" t="inlineStr">
-        <is>
-          <t>02</t>
-        </is>
-      </c>
-      <c r="D3" s="9" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Diagnosed with early and/or moderate &lt;usdm:tag name="StudyIndication"/&gt; at least 6 months before study participation.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E3" s="9" t="inlineStr">
-        <is>
-          <t>Inclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F3" s="4" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G3" s="38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H3" s="9" t="inlineStr">
-        <is>
-          <t> </t>
         </is>
       </c>
     </row>
     <row r="4" ht="29" customHeight="1">
       <c r="A4" s="9" t="inlineStr">
         <is>
-          <t>CB0321</t>
+          <t>IETESTCD</t>
         </is>
       </c>
       <c r="B4" s="9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Incl/Excl Criterion Short Name</t>
         </is>
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>03</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D4" s="9" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Able to read, understand and to provide written consent.&lt;/p&gt;</t>
+          <t>Topic</t>
         </is>
       </c>
       <c r="E4" s="9" t="inlineStr">
         <is>
-          <t>Inclusion Criteria</t>
+          <t>Req</t>
         </is>
       </c>
       <c r="F4" s="4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Incl/Excl Criterion Short Name</t>
         </is>
       </c>
       <c r="G4" s="39" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H4" s="33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>study.versions.studyDesigns.eligibilityCriteria.{id: identifier}</t>
+        </is>
+      </c>
+      <c r="H4" s="33" t="n"/>
     </row>
     <row r="5" ht="87" customHeight="1">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t>CB0321</t>
+          <t>IETEST</t>
         </is>
       </c>
       <c r="B5" s="9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Inclusion/Exclusion Criterion</t>
         </is>
       </c>
       <c r="C5" s="9" t="inlineStr">
         <is>
-          <t>04</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D5" s="9" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Female study participants should not be &lt;usdm:tag name="Pregnant"/&gt; or plan to become pregnant during study participation and for 6 months after last investigational product administration.</t>
+          <t>Synonym Qualifier</t>
         </is>
       </c>
       <c r="E5" s="9" t="inlineStr">
         <is>
-          <t>Inclusion Criteria</t>
+          <t>Req</t>
         </is>
       </c>
       <c r="F5" s="4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Inclusion/Exclusion Criterion</t>
         </is>
       </c>
       <c r="G5" s="41" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H5" s="33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>study.versions.($EligTxt := function($id) {(eligibilityCriterionItems[id=$id].text)}; studyDesigns.eligibilityCriteria{id: $EligTxt(criterionItemId)})</t>
+        </is>
+      </c>
+      <c r="H5" s="33" t="n"/>
     </row>
     <row r="6" ht="43.5" customHeight="1">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t>CB0321</t>
+          <t>IECAT</t>
         </is>
       </c>
       <c r="B6" s="9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Inclusion/Exclusion Category</t>
         </is>
       </c>
       <c r="C6" s="9" t="inlineStr">
         <is>
-          <t>05</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D6" s="9" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Male participants if their sexual partners can become pregnant should use a method of contraception during study participation and for 6 months after the last administration of the investigated product.</t>
+          <t>Grouping Qualifier</t>
         </is>
       </c>
       <c r="E6" s="9" t="inlineStr">
         <is>
-          <t>Inclusion Criteria</t>
+          <t>Req</t>
         </is>
       </c>
       <c r="F6" s="4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Inclusion/Exclusion Category</t>
         </is>
       </c>
       <c r="G6" s="39" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H6" s="33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>study.versions.studyDesigns.eligibilityCriteria{id: category.decode}</t>
+        </is>
+      </c>
+      <c r="H6" s="33" t="n"/>
     </row>
     <row r="7" ht="43.5" customHeight="1">
       <c r="A7" s="9" t="inlineStr">
         <is>
-          <t>CB0321</t>
+          <t>IESCAT</t>
         </is>
       </c>
       <c r="B7" s="9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Inclusion/Exclusion Subcategory</t>
         </is>
       </c>
       <c r="C7" s="9" t="inlineStr">
         <is>
-          <t>06</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D7" s="9" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Study participant is able and willing to comply with the requirements of this clinical study.&lt;/p&gt;</t>
+          <t>Grouping Qualifier</t>
         </is>
       </c>
       <c r="E7" s="9" t="inlineStr">
         <is>
-          <t>Inclusion Criteria</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="F7" s="4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Inclusion/Exclusion Subcategory</t>
         </is>
       </c>
       <c r="G7" s="39" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H7" s="33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>study.versions.studyDesigns.eligibilityCriteria{id: notes.codes.decode}</t>
+        </is>
+      </c>
+      <c r="H7" s="33" t="n"/>
     </row>
     <row r="8" ht="29" customHeight="1">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>CB0321</t>
+          <t>TIRL</t>
         </is>
       </c>
       <c r="B8" s="9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Inclusion/Exclusion Criterion Rule</t>
         </is>
       </c>
       <c r="C8" s="9" t="inlineStr">
         <is>
-          <t>07</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D8" s="9" t="inlineStr">
         <is>
-          <t>&lt;p&gt;Parkinson s disease subjects deemed appropriate for treatment of motor symptoms with a &lt;usdm:tag name="BC1_UDPRS"/&gt; Part III score &gt;&lt;usdm:tag name="BC1_MinValExcl"/&gt;.&lt;/p&gt;</t>
+          <t>Rule</t>
         </is>
       </c>
       <c r="E8" s="9" t="inlineStr">
         <is>
-          <t>Inclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F8" s="4" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G8" s="38" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H8" s="33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>Perm</t>
+        </is>
+      </c>
+      <c r="F8" s="4" t="n"/>
+      <c r="G8" s="38" t="n"/>
+      <c r="H8" s="33" t="n"/>
     </row>
     <row r="9" ht="29" customHeight="1">
       <c r="A9" s="9" t="inlineStr">
         <is>
-          <t>CB0321</t>
+          <t>TIVERS</t>
         </is>
       </c>
       <c r="B9" s="9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Protocol Criteria Versions</t>
         </is>
       </c>
       <c r="C9" s="9" t="inlineStr">
         <is>
-          <t>08</t>
+          <t>Char</t>
         </is>
       </c>
       <c r="D9" s="9" t="inlineStr">
         <is>
-          <t>&lt;p&gt;A reliable caregiver who is in frequent or daily contact with the patient and who will accompany the patient to the office and/or be available by telephone at designated times, will monitor administration of prescribed medications, and will be responsible for the overall care of the patient at home. The caregiver and the patient must be able to communicate in English and willing to comply with 26 weeks of transdermal therapy.&lt;/p&gt;</t>
+          <t>Record Qualifier</t>
         </is>
       </c>
       <c r="E9" s="9" t="inlineStr">
         <is>
-          <t>Inclusion Criteria</t>
+          <t>Perm</t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t> </t>
+          <t>Protocol Criteria Versions</t>
         </is>
       </c>
       <c r="G9" s="38" t="inlineStr">
         <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H9" s="33" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>09</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Persons who have previously completed or withdrawn from this study or any other study investigating xanomeline TTS or the oral formulation of xanomeline.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Use of any investigational agent or approved Alzheimer's therapeutic medication within 30 days prior to enrollment into the study.&lt;/p&gt;"</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Diagnosis of serious neurological conditions, including &lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Stroke or vascular dementia documented by clinical history and/or radiographic findings interpretable by the investigator as indicative of these disorders&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Seizure disorder other than simple childhood febrile seizures&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Severe head trauma resulting in protracted loss of consciousness within the last 5 years, or multiple episodes of head trauma&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Parkinson\'s disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Multiple sclerosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Amyotrophic lateral sclerosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Myasthenia gravis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Episode of depression meeting DSM-IV criteria within 3 months of screening.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history within the last 5 years of the following:&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Schizophrenia&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Bipolar Disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Ethanol or psychoactive drug abuse or dependence. &lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history of syncope within the last 5 years.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>16b</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Evidence from ECG recording at screening of any of the following conditions :&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Left bundle branch block&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Bradycardia ≤50 beats per minute&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Sinus pauses &amp;gt;2 seconds&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Second or third degree heart block unless treated with a pacemaker&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Wolff-Parkinson-White syndrome&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Sustained supraventricular tachyarrhythmia including SVT≥10 sec, atrial fibrillation, atrial flutter.&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Ventricular tachycardia at a rate of ≥120 beats per minute lasting≥10 seconds.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history within the last 5 years of a serious cardiovascular disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Clinically significant arrhythmia&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Symptomatic sick sinus syndrome not treated with a pacemaker&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Congestive heart failure refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Angina except angina controlled with PRN nitroglycerin&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Resting heart rate &amp;lt;50 or &amp;gt;100 beats per minute, on physical exam&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled hypertension.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history within the last 5 years of a serious gastrointestinal disorder, including &lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Chronic peptic/duodenal/gastric/esophageal ulcer that are untreated or refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Symptomatic diverticular disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Inflammatory bowel disease&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Pancreatitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Hepatitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Cirrhosis of the liver.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history within the last 5 years of a serious endocrine disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled Insulin Dependent Diabetes Mellitus (IDDM)&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Diabetic ketoacidosis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Untreated hyperthyroidism&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Untreated hypothyroidism&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Other untreated endocrinological disorder&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>&lt;p&gt; A history within the last 5 years of a serious respiratory disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Asthma with bronchospasm refractory to treatment&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Decompensated chronic obstructive pulmonary disease.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history within the last 5 years of a serious genitourinary disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Renal failure&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Uncontrolled urinary retention.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history within the last 5 years of a serious rheumatologic disorder, including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;Lupus&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Temporal arteritis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;Severe rheumatoid arthritis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A known history of human immunodeficiency virus (HIV) within the last 5 years.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>24</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history within the last 5 years of a serious infectious disease including&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n&lt;li&gt;&lt;p&gt;a)  Neurosyphilis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;b)  Meningitis&lt;/p&gt;&lt;/li&gt;\n&lt;li&gt;&lt;p&gt;c)  Encephalitis.&lt;/p&gt;&lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;A history within the last 5 years of a primary or recurrent malignant disease with the exception of resected cutaneous squamous cell carcinoma in situ, basal cell carcinoma, cervical carcinoma in situ, or in situ prostate cancer with a normal PSA postresection.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Visual, hearing, or communication disabilities impairing the ability to participate in the study; (for example, inability to speak or understand English, illiteracy).&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>27b</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Laboratory test values exceeding the Lilly Reference Range III for the patient's age in any of the following analytes: ↑ creatinine, ↑ total bilirubin, ↑ SGOT, ↑ SGPT, ↑ alkaline phosphatase, ↑ GGT, ↑↓ hemoglobin, ↑↓ white blood cell count, ↑↓ platelet count, ↑↓ serum sodium, potassium, or calcium.&lt;/p&gt;\n&lt;p&gt;If values exceed these laboratory reference ranges, clinical significance will be judged by the monitoring physicians. If the monitoring physician determines that the deviation from the reference range is not clinically significant, the patient may be included in the study. This decision will be documented.&lt;/p&gt;"</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>28b</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>29b</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Positive syphilis screening.&lt;/p&gt;\n&lt;p&gt;Positive syphilis screening. As determined by positive RPR followed up by confirmatory FTA-Abs. Confirmed patients are excluded unless there is a documented medical history of an alternative disease (for example, yaws) which caused the lab abnormality.&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F30" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>30b</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Glycosylated hemoglobin (A1C). Required only on patients with known diabetes mellitus or random blood sugar &amp;gt;200 on screening labs. Patients will be excluded if levels are &amp;gt;9.5%&lt;/p&gt;</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>CB0321</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>TI</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>31b</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>&lt;p&gt;Treatment with the following medications within the specified washout periods prior to enrollment and during the\n  study:&lt;/p&gt;\n&lt;ol style="list-style-type: lower-alpha;"&gt;\n  &lt;li&gt;\n    &lt;p&gt;Anticonvulsants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Depakote&amp;#174; (valproic acid) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dilantin&amp;#174; (phenytoin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Felbatol&amp;#174;\n          (felbamate)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Klonopin&amp;#174; (clonazepam)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lamictal&amp;#174; (lamotrigine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mysoline&amp;#174; (primidone)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Neurontin&amp;#174;\n          (gabapentin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Phenobarbitol&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tegretol&amp;#174; (carbamazepine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Alpha receptor blockers including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aldomet&amp;#174; (methyldopa) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cardura&amp;#174;\n          (doxazosin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Catapres&amp;#174; (clonidine)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Hytrin&amp;#174; (terazosin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Minipress&amp;#174; (prazosin)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tenex&amp;#174; (guanfacine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wytensin&amp;#174;\n          (guanabenz) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;The use of low doses\n        (2 mg daily) of either Hytrin&lt;/b&gt;&amp;#174; &lt;b&gt;or Cardura&lt;/b&gt;&amp;#174; &lt;b&gt;for relief of\n        urinary retention for patients with prostatic hypertrophy will be considered\n        on a case-by-case basis provided blood pressure is stable and the medication\n        has not had demonstrable effect on dementia symptoms in the opinion of the treating\n        physician. Contact CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Calcium channel blockers\n      that are CNS active including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Calan&amp;#174; , Isoptin&amp;#174; , Verelan&amp;#174; (verapamil) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cardizem&amp;#174; (diltiazem) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nimotop&amp;#174;\n          (nimodipine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Adalat&amp;#174; , Procardia XL&amp;#174;\n          (nifedipine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Cardene&lt;/b&gt;&amp;#174; &lt;b&gt;(nicardipine),\n        Norvasc&lt;/b&gt;&amp;#174; &lt;b&gt;, (amlodipine), and DynaCirc&lt;/b&gt;&amp;#174; &lt;b&gt;(isradipine) will\n        be allowed during the study. If a patient is taking an excluded calcium channel\n        blocker and is changed to an equivalent dose of an allowed calcium channel blocker,\n        enrollment may proceed in as little as 24 hours though 1 week is preferred when\n        possible.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Beta blockers including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Betapace&amp;#174; (sotalol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Inderal&amp;#174; (propranolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lopressor&amp;#174;\n          , Toprol XL&amp;#174; (metoprolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Corgard&amp;#174; (nadolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Sectral&amp;#174; (acebutolol)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tenormin&amp;#174; (atenolol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Visken&amp;#174; (pindolol)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Beta\n        blocker eye drops for glaucoma will be considered on a case-by-case basis. Call\n        medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Beta sympathomimetics (unless inhaled) including\n      but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Alupent&amp;#174; tablets\n          (metaproterenol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Brethine&amp;#174; tablets\n          (terbutaline) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dopamine &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Proventil Repetabs&amp;#174; , Ventolin&amp;#174; tablets (albuterol tablets)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;Parasympathomimetics (cholinergics) (unless opthalmic) including but not limited to\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Antilirium&amp;#174; (physostigmine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aricept&amp;#174; (donepezil) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cognex&amp;#174; (tacrine) &lt;/td&gt;\n        &lt;td&gt;1\n          month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mestinon&amp;#174; (pyridostigmine) &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Reglan&amp;#174; (metoclopramide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Urecholine&amp;#174;\n          , Duvoid (bethanechol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Cholinergic eye drops for treatment of glaucoma will be allowed during the study on a case-by-case basis.\n        Please contact the CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Muscle relaxants-centrally active including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Equanil&amp;#174; (meprobamate) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Flexeril&amp;#174; (cyclobenzaprine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lioresal&amp;#174; (baclofen) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norflex&amp;#174; (orphenadrine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Parafon Forte&amp;#174; (chlorzoxazone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Robaxin&amp;#174; (methocarbamol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Skelaxin&amp;#174; (metaxalone)\n        &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Soma&amp;#174; (carisoprodol) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Monamine oxidase inhibitors (MAOI) including but not limited to&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Eldepryl&amp;#174; (selegiline)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nardil&amp;#174; (phenelzine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Parnate&amp;#174; (tranylcypromine) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Parasympatholytics including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Antivert&amp;#174; , Bonine&amp;#174; , Dramamine II&amp;#174; (meclizine)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Artane&amp;#174; (trihexyphenidyl)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Bellergal-S&amp;#174; (alkaloids of belladonna and ergotamine) &lt;/td&gt;\n        &lt;td&gt;2 weeks &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Bentyl&amp;#174; (dicyclomine) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cogentin&amp;#174; (benztropine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cystospaz&amp;#174;, Levsin&amp;#174; , Levsinex&amp;#174; (hyoscyamine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ditropan&amp;#174;\n          (oxybutynin) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Donnatal&amp;#174; , Hyosophen&amp;#174;\n          (atropine, scopolamine, hyoscyamine and phenobarbitol) &lt;/td&gt;\n        &lt;td&gt;1 month &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dramamine&amp;#174; (dimenhydrinate)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lomotil&amp;#174;, Lonox&amp;#174; (atropine, diphenoxylate) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pro-Banthine&amp;#174;(propantheline) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Robinul&amp;#174; (glycopyrrolate)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tigan&amp;#174; (trimethobenzamide) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Transderm-Scop&amp;#174; (scopolamine) &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Urispas&amp;#174; (flavoxate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antidepressants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Anafranil&amp;#174; (clomipramine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Asendin&amp;#174;\n          (amoxapine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Desyrel&amp;#174; (trazodone)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Effexor&amp;#174; (venlafaxine) &lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Elavil&amp;#174; (amitriptyline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ludiomil&amp;#174;\n          (maprotiline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norpramin&amp;#174; (desipramine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pamelor&amp;#174; , Aventyl&amp;#174; (nortriptyline)&lt;/td&gt;\n        &lt;td&gt; 1\n          month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Paxil&amp;#174; (paroxetine)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prozac&amp;#174;\n          (fluoxetine&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Remeron&amp;#174; (mirtazapine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serzone&amp;#174; (nefazodone) &lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Sinequan&amp;#174;\n          (doxepin)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tofranil&amp;#174; (imipramine)&lt;/td&gt;\n        &lt;td&gt;\n          1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vivactil&amp;#174; (protriptyline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wellbutrin&amp;#174; (bupropion)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zoloft&amp;#174;\n          (sertraline)&lt;/td&gt;\n        &lt;td&gt; 1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Systemic corticosteroids including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cortisone&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Decadron&amp;#174; (dexamethasone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Depo-Medrol&amp;#174; (methylprednisolone)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prednisone&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Xanthine derivatives\n      including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Aminophylline&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Fioricet&amp;#174; , Esgic&amp;#174; , Phrenilin Forte&amp;#174; (caffeine, butalbital)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Theo-Dur&amp;#174; (theophylline)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Wigraine&amp;#174; , Cafergot&amp;#174; (caffeine, ergotamine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n        &lt;td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Histamine (H2 ) antagonists including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Axid&amp;#174; (nizatidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Pepcid&amp;#174; (famotidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tagamet&amp;#174; (cimetidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zantac&amp;#174; (ranitidine)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;If an H 2 antagonist is needed by the patient, Axid&lt;/b&gt;&amp;#174; &lt;b&gt;will be&lt;/b&gt; &lt;b&gt;allowed on a case-by-case\n        basis. Please consult CRO&lt;/b&gt; &lt;b&gt;medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Narcotic Analgesics including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Darvocet-N\n          100&amp;#174; , (propoxyphene)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Demerol&amp;#174; (meperidine)&lt;/td&gt;\n        &lt;td&gt;1\n          week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dilaudid&amp;#174; (hydromorphone)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Duragesic&amp;#174; (fentanyl)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;MS\n          Contin&amp;#174; , Roxanol&amp;#174; , Oramorph&amp;#174; (morphine) &lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Percocet&amp;#174; , Roxicet&amp;#174; (oxycodone with acetaminophen)&lt;/td&gt;\n        &lt;td&gt;3\n          days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Percodan&amp;#174; , Roxiprin&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Stadol&amp;#174; (butorphanol)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Talacen&amp;#174;\n          (pentazocine)&lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tylenol #2&amp;#174; , #3&amp;#174;\n          , #4&amp;#174; (codeine and acetaminophen) &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tylox&amp;#174;\n          , Roxilox&amp;#174; (oxycodone)&lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vicodin&amp;#174;, Lorcet&amp;#174; (hydrocodone)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Percocet\n        (oxycodone with acetaminophen) and Tylenol&lt;/b&gt;&amp;#174; &lt;b&gt;with codeine #2, #3, #4\n        (acetaminophen + codeine) ARE allowed in the month prior to enrollment, but\n        are not permitted in the 3 days prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Neuroleptics\n      (antipsychotics) including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Clozaril&amp;#174;\n          (clozapine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Haldol&amp;#174; (haloperidol)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Loxitane&amp;#174; (loxapine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mellaril&amp;#174; (thioridazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Moban&amp;#174;\n          (molindone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Navane&amp;#174; (thiothixene)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Orap&amp;#174; (pimozide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Prolixin&amp;#174; (fluphenazine)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Risperdal&amp;#174;\n          (risperidone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Stelazine&amp;#174; (trifluoperazine)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Thorazine&amp;#174; (chlorpromazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Trilafon&amp;#174; (perphenazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serentil&amp;#174;\n          (mesoridazine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;The use of neuroleptics\n        on a daily basis must be discontinued 2 to 4 weeks prior to enrollment. The\n        use of neuroleptics on an as-needed basis is allowable during the screening\n        period, but the last dose must be at least 7 days prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antianxiety agents including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Atarax&amp;#174; (hydroxyzine)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;BuSpar&amp;#174;\n          (buspirone)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Librium&amp;#174; (chlordiazepoxide)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Serax&amp;#174; (oxazepam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tranxene&amp;#174; (clorazepate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Valium&amp;#174; (diazepam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Vistaril&amp;#174; (hydroxyzine pamoate)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Xanax&amp;#174; (alprazolam)&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Ativan&lt;/b&gt;&amp;#174; &lt;b&gt;(lorazepam) should be discontinued on a daily\n        basis 2 weeks&lt;/b&gt;&lt;/p&gt;\n    &lt;p&gt;&lt;b&gt;prior to enrollment. It may be used on an as-needed\n        basis during the screening period, but is not permitted in the 24 hours prior\n        to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Hypnotics/Sedatives including but not limited to&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ambien&amp;#174; (zolpidem)&lt;/td&gt;\n        &lt;td&gt; 3 days\n        &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dalmane&amp;#174; (flurazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Doral&amp;#174; (quazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Halcion&amp;#174; (triazolam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Nembutal&amp;#174; &lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;ProSom&amp;#174; (estazolam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Restoril&amp;#174;\n          (temazepam)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Seconal&amp;#174;&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Chloral Hydrate is allowed on an as-needed basis during screening, but is not permitted in the 24 hours prior to enrollment.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Histamine (H1 ) antagonists including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Actifed&amp;#174; , Actifed Plus&amp;#174; (triprolidine) Benadryl&amp;#174;\n          , Unisom&amp;#174; , Tylenol P.M.&amp;#174; &lt;/td&gt;\n        &lt;td&gt;3 days &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;(diphenhydramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Compazine&amp;#174; (prochlorperazine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Contac&amp;#174; , Coricidin D&amp;#174; , Sinutab&amp;#174; , Novahistine&amp;#174; , Alka\n          Seltzer Plus&amp;#174; , Naldecon&amp;#174; , Sudafed Plus&amp;#174; , Tylenol Cold&amp;#174; , Tylenol\n          Cold and Flu&amp;#174; (chlorpheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Dimetapp&amp;#174;\n          (brompheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Drixoral&amp;#174; (dexbrompheniramine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Hismanal&amp;#174; (astemizole)&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Phenergan&amp;#174;\n          (promethazine)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Seldane&amp;#174; (terfenadine)&lt;/td&gt;\n        &lt;td&gt;1\n          week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tavist&amp;#174; (clemastine fumarate)&lt;/td&gt;\n        &lt;td&gt;3 days&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Zyrtec&amp;#174; (cetrizine) &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Allegra&lt;/b&gt;&amp;#174;\n      &lt;b&gt;(fexofenadine hydrochloride) or Claritin&lt;/b&gt;&amp;#174; &lt;b&gt;(loratadine) may be taken\n        on as-needed basis during screening but must be discontinued within 24 hours\n        of enrollment.&lt;/b&gt;\n    &lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Stimulants including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cylert&amp;#174; (pemoline) &lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ritalin&amp;#174; (methylphenidate)&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Antiarrhythmics including but not limited to the following&lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Adenocard&amp;#174; (adenosine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Cordarone&amp;#174;\n          (amiodarone) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ethmozine&amp;#174; (moricizine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Mexitil&amp;#174; (mexiletine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Norpace&amp;#174; (disopyramide)\n        &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Procan&amp;#174; (procainamide) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Quinaglute&amp;#174;\n          (quinidine) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Rythmol&amp;#174; (propafenone) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tambocor&amp;#174;\n          (flecainide) &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tonocard&amp;#174; (tocainide)&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n    &lt;p&gt;&lt;b&gt;Requirement of these drugs for control of cardiac arrhythmia indicates that\n        the patient should be excluded from the study. If discontinuation of an antiarrhythmic\n        is considered, please discuss case with CRO medical monitor.&lt;/b&gt;&lt;/p&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Miscellaneous drugs including but not limited to &lt;/p&gt;\n    &lt;table class="table"&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Coenzyme\n          Q&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Eskalith&amp;#174; , Lithobid&amp;#174; (lithium)&lt;/td&gt;\n        &lt;td&gt;2\n          weeks &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Ginkgo biloba&lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lecithin\n        &lt;/td&gt;\n        &lt;td&gt;1 week&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lecithin &lt;/td&gt;\n        &lt;td&gt;1 week &lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Lupron&lt;/td&gt;\n        &lt;td&gt;2 weeks&lt;/td&gt;\n      &lt;/tr&gt;\n      &lt;tr&gt;\n        &lt;td&gt;Tamoxifen&lt;/td&gt;\n        &lt;td&gt;1 month&lt;/td&gt;\n      &lt;/tr&gt;\n    &lt;/table&gt;\n  &lt;/li&gt;\n  &lt;li&gt;\n    &lt;p&gt;Estrogen supplements are permitted during the study, but dosage must be stable for at least 3 months prior to\n      enrollment.&lt;/p&gt;\n  &lt;/li&gt;\n&lt;/ol&gt;</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>Exclusion Criteria</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
-      </c>
+          <t>study.versions.versionIdentifier</t>
+        </is>
+      </c>
+      <c r="H9" s="33" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>